<commit_message>
Update reference files: styles of merged cells slightly differ, though visually they are the same
</commit_message>
<xml_diff>
--- a/tests/Gauges/GroupTagTests_WithHeader.xlsx
+++ b/tests/Gauges/GroupTagTests_WithHeader.xlsx
@@ -532,7 +532,7 @@
       </x:patternFill>
     </x:fill>
   </x:fills>
-  <x:borders count="8">
+  <x:borders count="6">
     <x:border>
       <x:left/>
       <x:right/>
@@ -605,42 +605,8 @@
       </x:bottom>
       <x:diagonal/>
     </x:border>
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="thin">
-        <x:color indexed="64"/>
-      </x:left>
-      <x:right style="thin">
-        <x:color indexed="64"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
-    </x:border>
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="thin">
-        <x:color indexed="64"/>
-      </x:left>
-      <x:right style="thin">
-        <x:color indexed="64"/>
-      </x:right>
-      <x:top style="none">
-        <x:color indexed="64"/>
-      </x:top>
-      <x:bottom style="thin">
-        <x:color indexed="64"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
-    </x:border>
   </x:borders>
-  <x:cellStyleXfs count="22">
+  <x:cellStyleXfs count="16">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
@@ -687,26 +653,8 @@
     <x:xf numFmtId="4" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="6" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="45">
+  <x:cellXfs count="39">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <x:alignment vertical="center"/>
@@ -824,30 +772,6 @@
     </x:xf>
     <x:xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
@@ -1418,7 +1342,7 @@
       </x:c>
     </x:row>
     <x:row r="6" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
-      <x:c r="B6" s="39" t="s"/>
+      <x:c r="B6" s="35" t="s"/>
       <x:c r="C6" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -1432,7 +1356,7 @@
       </x:c>
     </x:row>
     <x:row r="7" spans="1:10" outlineLevel="3" x14ac:dyDescent="0.2">
-      <x:c r="B7" s="40" t="s"/>
+      <x:c r="B7" s="35" t="s"/>
       <x:c r="C7" s="36" t="s"/>
       <x:c r="D7" s="37" t="n">
         <x:v>1014</x:v>
@@ -1454,7 +1378,7 @@
       </x:c>
     </x:row>
     <x:row r="8" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
-      <x:c r="B8" s="40" t="s"/>
+      <x:c r="B8" s="35" t="s"/>
       <x:c r="C8" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -1474,7 +1398,7 @@
       </x:c>
     </x:row>
     <x:row r="9" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
-      <x:c r="B9" s="40" t="s"/>
+      <x:c r="B9" s="35" t="s"/>
       <x:c r="C9" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -1491,8 +1415,8 @@
       </x:c>
     </x:row>
     <x:row r="10" spans="1:10" outlineLevel="3">
-      <x:c r="B10" s="40" t="s"/>
-      <x:c r="C10" s="41" t="s"/>
+      <x:c r="B10" s="35" t="s"/>
+      <x:c r="C10" s="36" t="s"/>
       <x:c r="D10" s="37" t="n">
         <x:v>1129</x:v>
       </x:c>
@@ -1510,8 +1434,8 @@
       </x:c>
     </x:row>
     <x:row r="11" spans="1:10" outlineLevel="3">
-      <x:c r="B11" s="40" t="s"/>
-      <x:c r="C11" s="42" t="s"/>
+      <x:c r="B11" s="35" t="s"/>
+      <x:c r="C11" s="36" t="s"/>
       <x:c r="D11" s="37" t="n">
         <x:v>1029</x:v>
       </x:c>
@@ -1529,7 +1453,7 @@
       </x:c>
     </x:row>
     <x:row r="12" spans="1:10" outlineLevel="2">
-      <x:c r="B12" s="40" t="s"/>
+      <x:c r="B12" s="35" t="s"/>
       <x:c r="C12" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -1546,7 +1470,7 @@
       </x:c>
     </x:row>
     <x:row r="13" spans="1:10" outlineLevel="2">
-      <x:c r="B13" s="40" t="s"/>
+      <x:c r="B13" s="35" t="s"/>
       <x:c r="C13" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -1557,7 +1481,7 @@
       <x:c r="H13" s="34" t="s"/>
     </x:row>
     <x:row r="14" spans="1:10" outlineLevel="3">
-      <x:c r="B14" s="40" t="s"/>
+      <x:c r="B14" s="35" t="s"/>
       <x:c r="C14" s="36" t="s"/>
       <x:c r="D14" s="37" t="n">
         <x:v>1038</x:v>
@@ -1576,7 +1500,7 @@
       </x:c>
     </x:row>
     <x:row r="15" spans="1:10" outlineLevel="2">
-      <x:c r="B15" s="43" t="s"/>
+      <x:c r="B15" s="35" t="s"/>
       <x:c r="C15" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -1621,7 +1545,7 @@
       <x:c r="H17" s="34" t="s"/>
     </x:row>
     <x:row r="18" spans="1:10" outlineLevel="2">
-      <x:c r="B18" s="39" t="s"/>
+      <x:c r="B18" s="35" t="s"/>
       <x:c r="C18" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -1632,7 +1556,7 @@
       <x:c r="H18" s="34" t="s"/>
     </x:row>
     <x:row r="19" spans="1:10" outlineLevel="3">
-      <x:c r="B19" s="40" t="s"/>
+      <x:c r="B19" s="35" t="s"/>
       <x:c r="C19" s="36" t="s"/>
       <x:c r="D19" s="37" t="n">
         <x:v>1039</x:v>
@@ -1651,7 +1575,7 @@
       </x:c>
     </x:row>
     <x:row r="20" spans="1:10" outlineLevel="2">
-      <x:c r="B20" s="43" t="s"/>
+      <x:c r="B20" s="35" t="s"/>
       <x:c r="C20" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -1696,7 +1620,7 @@
       <x:c r="H22" s="34" t="s"/>
     </x:row>
     <x:row r="23" spans="1:10" outlineLevel="2">
-      <x:c r="B23" s="39" t="s"/>
+      <x:c r="B23" s="35" t="s"/>
       <x:c r="C23" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1707,8 +1631,8 @@
       <x:c r="H23" s="34" t="s"/>
     </x:row>
     <x:row r="24" spans="1:10" outlineLevel="3">
-      <x:c r="B24" s="40" t="s"/>
-      <x:c r="C24" s="41" t="s"/>
+      <x:c r="B24" s="35" t="s"/>
+      <x:c r="C24" s="36" t="s"/>
       <x:c r="D24" s="37" t="n">
         <x:v>1017</x:v>
       </x:c>
@@ -1726,8 +1650,8 @@
       </x:c>
     </x:row>
     <x:row r="25" spans="1:10" outlineLevel="3">
-      <x:c r="B25" s="40" t="s"/>
-      <x:c r="C25" s="44" t="s"/>
+      <x:c r="B25" s="35" t="s"/>
+      <x:c r="C25" s="36" t="s"/>
       <x:c r="D25" s="37" t="n">
         <x:v>1217</x:v>
       </x:c>
@@ -1745,8 +1669,8 @@
       </x:c>
     </x:row>
     <x:row r="26" spans="1:10" outlineLevel="3">
-      <x:c r="B26" s="40" t="s"/>
-      <x:c r="C26" s="44" t="s"/>
+      <x:c r="B26" s="35" t="s"/>
+      <x:c r="C26" s="36" t="s"/>
       <x:c r="D26" s="37" t="n">
         <x:v>1117</x:v>
       </x:c>
@@ -1764,8 +1688,8 @@
       </x:c>
     </x:row>
     <x:row r="27" spans="1:10" outlineLevel="3">
-      <x:c r="B27" s="40" t="s"/>
-      <x:c r="C27" s="42" t="s"/>
+      <x:c r="B27" s="35" t="s"/>
+      <x:c r="C27" s="36" t="s"/>
       <x:c r="D27" s="37" t="n">
         <x:v>1317</x:v>
       </x:c>
@@ -1783,7 +1707,7 @@
       </x:c>
     </x:row>
     <x:row r="28" spans="1:10" outlineLevel="2">
-      <x:c r="B28" s="40" t="s"/>
+      <x:c r="B28" s="35" t="s"/>
       <x:c r="C28" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -1800,7 +1724,7 @@
       </x:c>
     </x:row>
     <x:row r="29" spans="1:10" outlineLevel="2">
-      <x:c r="B29" s="40" t="s"/>
+      <x:c r="B29" s="35" t="s"/>
       <x:c r="C29" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -1811,8 +1735,8 @@
       <x:c r="H29" s="34" t="s"/>
     </x:row>
     <x:row r="30" spans="1:10" outlineLevel="3">
-      <x:c r="B30" s="40" t="s"/>
-      <x:c r="C30" s="41" t="s"/>
+      <x:c r="B30" s="35" t="s"/>
+      <x:c r="C30" s="36" t="s"/>
       <x:c r="D30" s="37" t="n">
         <x:v>1137</x:v>
       </x:c>
@@ -1830,8 +1754,8 @@
       </x:c>
     </x:row>
     <x:row r="31" spans="1:10" outlineLevel="3">
-      <x:c r="B31" s="40" t="s"/>
-      <x:c r="C31" s="44" t="s"/>
+      <x:c r="B31" s="35" t="s"/>
+      <x:c r="C31" s="36" t="s"/>
       <x:c r="D31" s="37" t="n">
         <x:v>1037</x:v>
       </x:c>
@@ -1849,8 +1773,8 @@
       </x:c>
     </x:row>
     <x:row r="32" spans="1:10" outlineLevel="3">
-      <x:c r="B32" s="40" t="s"/>
-      <x:c r="C32" s="42" t="s"/>
+      <x:c r="B32" s="35" t="s"/>
+      <x:c r="C32" s="36" t="s"/>
       <x:c r="D32" s="37" t="n">
         <x:v>1099</x:v>
       </x:c>
@@ -1868,7 +1792,7 @@
       </x:c>
     </x:row>
     <x:row r="33" spans="1:10" outlineLevel="2">
-      <x:c r="B33" s="40" t="s"/>
+      <x:c r="B33" s="35" t="s"/>
       <x:c r="C33" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -1885,7 +1809,7 @@
       </x:c>
     </x:row>
     <x:row r="34" spans="1:10" outlineLevel="2">
-      <x:c r="B34" s="40" t="s"/>
+      <x:c r="B34" s="35" t="s"/>
       <x:c r="C34" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -1896,8 +1820,8 @@
       <x:c r="H34" s="34" t="s"/>
     </x:row>
     <x:row r="35" spans="1:10" outlineLevel="3">
-      <x:c r="B35" s="40" t="s"/>
-      <x:c r="C35" s="41" t="s"/>
+      <x:c r="B35" s="35" t="s"/>
+      <x:c r="C35" s="36" t="s"/>
       <x:c r="D35" s="37" t="n">
         <x:v>1294</x:v>
       </x:c>
@@ -1915,8 +1839,8 @@
       </x:c>
     </x:row>
     <x:row r="36" spans="1:10" outlineLevel="3">
-      <x:c r="B36" s="40" t="s"/>
-      <x:c r="C36" s="42" t="s"/>
+      <x:c r="B36" s="35" t="s"/>
+      <x:c r="C36" s="36" t="s"/>
       <x:c r="D36" s="37" t="n">
         <x:v>1074</x:v>
       </x:c>
@@ -1934,7 +1858,7 @@
       </x:c>
     </x:row>
     <x:row r="37" spans="1:10" outlineLevel="2">
-      <x:c r="B37" s="43" t="s"/>
+      <x:c r="B37" s="35" t="s"/>
       <x:c r="C37" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -1979,7 +1903,7 @@
       <x:c r="H39" s="34" t="s"/>
     </x:row>
     <x:row r="40" spans="1:10" outlineLevel="2">
-      <x:c r="B40" s="39" t="s"/>
+      <x:c r="B40" s="35" t="s"/>
       <x:c r="C40" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1990,7 +1914,7 @@
       <x:c r="H40" s="34" t="s"/>
     </x:row>
     <x:row r="41" spans="1:10" outlineLevel="3">
-      <x:c r="B41" s="40" t="s"/>
+      <x:c r="B41" s="35" t="s"/>
       <x:c r="C41" s="36" t="s"/>
       <x:c r="D41" s="37" t="n">
         <x:v>1204</x:v>
@@ -2009,7 +1933,7 @@
       </x:c>
     </x:row>
     <x:row r="42" spans="1:10" outlineLevel="2">
-      <x:c r="B42" s="40" t="s"/>
+      <x:c r="B42" s="35" t="s"/>
       <x:c r="C42" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -2026,7 +1950,7 @@
       </x:c>
     </x:row>
     <x:row r="43" spans="1:10" outlineLevel="2">
-      <x:c r="B43" s="40" t="s"/>
+      <x:c r="B43" s="35" t="s"/>
       <x:c r="C43" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -2037,8 +1961,8 @@
       <x:c r="H43" s="34" t="s"/>
     </x:row>
     <x:row r="44" spans="1:10" outlineLevel="3">
-      <x:c r="B44" s="40" t="s"/>
-      <x:c r="C44" s="41" t="s"/>
+      <x:c r="B44" s="35" t="s"/>
+      <x:c r="C44" s="36" t="s"/>
       <x:c r="D44" s="37" t="n">
         <x:v>1355</x:v>
       </x:c>
@@ -2056,8 +1980,8 @@
       </x:c>
     </x:row>
     <x:row r="45" spans="1:10" outlineLevel="3">
-      <x:c r="B45" s="40" t="s"/>
-      <x:c r="C45" s="42" t="s"/>
+      <x:c r="B45" s="35" t="s"/>
+      <x:c r="C45" s="36" t="s"/>
       <x:c r="D45" s="37" t="n">
         <x:v>1263</x:v>
       </x:c>
@@ -2075,7 +1999,7 @@
       </x:c>
     </x:row>
     <x:row r="46" spans="1:10" outlineLevel="2">
-      <x:c r="B46" s="43" t="s"/>
+      <x:c r="B46" s="35" t="s"/>
       <x:c r="C46" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -2120,7 +2044,7 @@
       <x:c r="H48" s="34" t="s"/>
     </x:row>
     <x:row r="49" spans="1:10" outlineLevel="2">
-      <x:c r="B49" s="39" t="s"/>
+      <x:c r="B49" s="35" t="s"/>
       <x:c r="C49" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -2131,7 +2055,7 @@
       <x:c r="H49" s="34" t="s"/>
     </x:row>
     <x:row r="50" spans="1:10" outlineLevel="3">
-      <x:c r="B50" s="40" t="s"/>
+      <x:c r="B50" s="35" t="s"/>
       <x:c r="C50" s="36" t="s"/>
       <x:c r="D50" s="37" t="n">
         <x:v>1065</x:v>
@@ -2150,7 +2074,7 @@
       </x:c>
     </x:row>
     <x:row r="51" spans="1:10" outlineLevel="2">
-      <x:c r="B51" s="43" t="s"/>
+      <x:c r="B51" s="35" t="s"/>
       <x:c r="C51" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -2195,7 +2119,7 @@
       <x:c r="H53" s="34" t="s"/>
     </x:row>
     <x:row r="54" spans="1:10" outlineLevel="2">
-      <x:c r="B54" s="39" t="s"/>
+      <x:c r="B54" s="35" t="s"/>
       <x:c r="C54" s="29" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -2206,8 +2130,8 @@
       <x:c r="H54" s="34" t="s"/>
     </x:row>
     <x:row r="55" spans="1:10" outlineLevel="3">
-      <x:c r="B55" s="40" t="s"/>
-      <x:c r="C55" s="41" t="s"/>
+      <x:c r="B55" s="35" t="s"/>
+      <x:c r="C55" s="36" t="s"/>
       <x:c r="D55" s="37" t="n">
         <x:v>1042</x:v>
       </x:c>
@@ -2225,8 +2149,8 @@
       </x:c>
     </x:row>
     <x:row r="56" spans="1:10" outlineLevel="3">
-      <x:c r="B56" s="40" t="s"/>
-      <x:c r="C56" s="42" t="s"/>
+      <x:c r="B56" s="35" t="s"/>
+      <x:c r="C56" s="36" t="s"/>
       <x:c r="D56" s="37" t="n">
         <x:v>1142</x:v>
       </x:c>
@@ -2244,7 +2168,7 @@
       </x:c>
     </x:row>
     <x:row r="57" spans="1:10" outlineLevel="2">
-      <x:c r="B57" s="43" t="s"/>
+      <x:c r="B57" s="35" t="s"/>
       <x:c r="C57" s="29" t="s">
         <x:v>29</x:v>
       </x:c>
@@ -2289,7 +2213,7 @@
       <x:c r="H59" s="34" t="s"/>
     </x:row>
     <x:row r="60" spans="1:10" outlineLevel="2">
-      <x:c r="B60" s="39" t="s"/>
+      <x:c r="B60" s="35" t="s"/>
       <x:c r="C60" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -2300,8 +2224,8 @@
       <x:c r="H60" s="34" t="s"/>
     </x:row>
     <x:row r="61" spans="1:10" outlineLevel="3">
-      <x:c r="B61" s="40" t="s"/>
-      <x:c r="C61" s="41" t="s"/>
+      <x:c r="B61" s="35" t="s"/>
+      <x:c r="C61" s="36" t="s"/>
       <x:c r="D61" s="37" t="n">
         <x:v>1079</x:v>
       </x:c>
@@ -2319,8 +2243,8 @@
       </x:c>
     </x:row>
     <x:row r="62" spans="1:10" outlineLevel="3">
-      <x:c r="B62" s="40" t="s"/>
-      <x:c r="C62" s="44" t="s"/>
+      <x:c r="B62" s="35" t="s"/>
+      <x:c r="C62" s="36" t="s"/>
       <x:c r="D62" s="37" t="n">
         <x:v>1153</x:v>
       </x:c>
@@ -2338,8 +2262,8 @@
       </x:c>
     </x:row>
     <x:row r="63" spans="1:10" outlineLevel="3">
-      <x:c r="B63" s="40" t="s"/>
-      <x:c r="C63" s="42" t="s"/>
+      <x:c r="B63" s="35" t="s"/>
+      <x:c r="C63" s="36" t="s"/>
       <x:c r="D63" s="37" t="n">
         <x:v>1253</x:v>
       </x:c>
@@ -2357,7 +2281,7 @@
       </x:c>
     </x:row>
     <x:row r="64" spans="1:10" outlineLevel="2">
-      <x:c r="B64" s="40" t="s"/>
+      <x:c r="B64" s="35" t="s"/>
       <x:c r="C64" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -2374,7 +2298,7 @@
       </x:c>
     </x:row>
     <x:row r="65" spans="1:10" outlineLevel="2">
-      <x:c r="B65" s="40" t="s"/>
+      <x:c r="B65" s="35" t="s"/>
       <x:c r="C65" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -2385,8 +2309,8 @@
       <x:c r="H65" s="34" t="s"/>
     </x:row>
     <x:row r="66" spans="1:10" outlineLevel="3">
-      <x:c r="B66" s="40" t="s"/>
-      <x:c r="C66" s="41" t="s"/>
+      <x:c r="B66" s="35" t="s"/>
+      <x:c r="C66" s="36" t="s"/>
       <x:c r="D66" s="37" t="n">
         <x:v>1106</x:v>
       </x:c>
@@ -2404,8 +2328,8 @@
       </x:c>
     </x:row>
     <x:row r="67" spans="1:10" outlineLevel="3">
-      <x:c r="B67" s="40" t="s"/>
-      <x:c r="C67" s="42" t="s"/>
+      <x:c r="B67" s="35" t="s"/>
+      <x:c r="C67" s="36" t="s"/>
       <x:c r="D67" s="37" t="n">
         <x:v>1006</x:v>
       </x:c>
@@ -2423,7 +2347,7 @@
       </x:c>
     </x:row>
     <x:row r="68" spans="1:10" outlineLevel="2">
-      <x:c r="B68" s="43" t="s"/>
+      <x:c r="B68" s="35" t="s"/>
       <x:c r="C68" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -2468,7 +2392,7 @@
       <x:c r="H70" s="34" t="s"/>
     </x:row>
     <x:row r="71" spans="1:10" outlineLevel="2">
-      <x:c r="B71" s="39" t="s"/>
+      <x:c r="B71" s="35" t="s"/>
       <x:c r="C71" s="29" t="s">
         <x:v>34</x:v>
       </x:c>
@@ -2479,8 +2403,8 @@
       <x:c r="H71" s="34" t="s"/>
     </x:row>
     <x:row r="72" spans="1:10" outlineLevel="3">
-      <x:c r="B72" s="40" t="s"/>
-      <x:c r="C72" s="41" t="s"/>
+      <x:c r="B72" s="35" t="s"/>
+      <x:c r="C72" s="36" t="s"/>
       <x:c r="D72" s="37" t="n">
         <x:v>1283</x:v>
       </x:c>
@@ -2498,8 +2422,8 @@
       </x:c>
     </x:row>
     <x:row r="73" spans="1:10" outlineLevel="3">
-      <x:c r="B73" s="40" t="s"/>
-      <x:c r="C73" s="42" t="s"/>
+      <x:c r="B73" s="35" t="s"/>
+      <x:c r="C73" s="36" t="s"/>
       <x:c r="D73" s="37" t="n">
         <x:v>1083</x:v>
       </x:c>
@@ -2517,7 +2441,7 @@
       </x:c>
     </x:row>
     <x:row r="74" spans="1:10" outlineLevel="2">
-      <x:c r="B74" s="40" t="s"/>
+      <x:c r="B74" s="35" t="s"/>
       <x:c r="C74" s="29" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -2534,7 +2458,7 @@
       </x:c>
     </x:row>
     <x:row r="75" spans="1:10" outlineLevel="2">
-      <x:c r="B75" s="40" t="s"/>
+      <x:c r="B75" s="35" t="s"/>
       <x:c r="C75" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -2545,8 +2469,8 @@
       <x:c r="H75" s="34" t="s"/>
     </x:row>
     <x:row r="76" spans="1:10" outlineLevel="3">
-      <x:c r="B76" s="40" t="s"/>
-      <x:c r="C76" s="41" t="s"/>
+      <x:c r="B76" s="35" t="s"/>
+      <x:c r="C76" s="36" t="s"/>
       <x:c r="D76" s="37" t="n">
         <x:v>1061</x:v>
       </x:c>
@@ -2564,8 +2488,8 @@
       </x:c>
     </x:row>
     <x:row r="77" spans="1:10" outlineLevel="3">
-      <x:c r="B77" s="40" t="s"/>
-      <x:c r="C77" s="44" t="s"/>
+      <x:c r="B77" s="35" t="s"/>
+      <x:c r="C77" s="36" t="s"/>
       <x:c r="D77" s="37" t="n">
         <x:v>1057</x:v>
       </x:c>
@@ -2583,8 +2507,8 @@
       </x:c>
     </x:row>
     <x:row r="78" spans="1:10" outlineLevel="3">
-      <x:c r="B78" s="40" t="s"/>
-      <x:c r="C78" s="44" t="s"/>
+      <x:c r="B78" s="35" t="s"/>
+      <x:c r="C78" s="36" t="s"/>
       <x:c r="D78" s="37" t="n">
         <x:v>1212</x:v>
       </x:c>
@@ -2602,8 +2526,8 @@
       </x:c>
     </x:row>
     <x:row r="79" spans="1:10" outlineLevel="3">
-      <x:c r="B79" s="40" t="s"/>
-      <x:c r="C79" s="44" t="s"/>
+      <x:c r="B79" s="35" t="s"/>
+      <x:c r="C79" s="36" t="s"/>
       <x:c r="D79" s="37" t="n">
         <x:v>1091</x:v>
       </x:c>
@@ -2621,8 +2545,8 @@
       </x:c>
     </x:row>
     <x:row r="80" spans="1:10" outlineLevel="3">
-      <x:c r="B80" s="40" t="s"/>
-      <x:c r="C80" s="44" t="s"/>
+      <x:c r="B80" s="35" t="s"/>
+      <x:c r="C80" s="36" t="s"/>
       <x:c r="D80" s="37" t="n">
         <x:v>1261</x:v>
       </x:c>
@@ -2640,8 +2564,8 @@
       </x:c>
     </x:row>
     <x:row r="81" spans="1:10" outlineLevel="3">
-      <x:c r="B81" s="40" t="s"/>
-      <x:c r="C81" s="44" t="s"/>
+      <x:c r="B81" s="35" t="s"/>
+      <x:c r="C81" s="36" t="s"/>
       <x:c r="D81" s="37" t="n">
         <x:v>1012</x:v>
       </x:c>
@@ -2659,8 +2583,8 @@
       </x:c>
     </x:row>
     <x:row r="82" spans="1:10" outlineLevel="3">
-      <x:c r="B82" s="40" t="s"/>
-      <x:c r="C82" s="42" t="s"/>
+      <x:c r="B82" s="35" t="s"/>
+      <x:c r="C82" s="36" t="s"/>
       <x:c r="D82" s="37" t="n">
         <x:v>1161</x:v>
       </x:c>
@@ -2678,7 +2602,7 @@
       </x:c>
     </x:row>
     <x:row r="83" spans="1:10" outlineLevel="2">
-      <x:c r="B83" s="40" t="s"/>
+      <x:c r="B83" s="35" t="s"/>
       <x:c r="C83" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -2695,7 +2619,7 @@
       </x:c>
     </x:row>
     <x:row r="84" spans="1:10" outlineLevel="2">
-      <x:c r="B84" s="40" t="s"/>
+      <x:c r="B84" s="35" t="s"/>
       <x:c r="C84" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -2706,7 +2630,7 @@
       <x:c r="H84" s="34" t="s"/>
     </x:row>
     <x:row r="85" spans="1:10" outlineLevel="3">
-      <x:c r="B85" s="40" t="s"/>
+      <x:c r="B85" s="35" t="s"/>
       <x:c r="C85" s="36" t="s"/>
       <x:c r="D85" s="37" t="n">
         <x:v>1168</x:v>
@@ -2725,7 +2649,7 @@
       </x:c>
     </x:row>
     <x:row r="86" spans="1:10" outlineLevel="2">
-      <x:c r="B86" s="40" t="s"/>
+      <x:c r="B86" s="35" t="s"/>
       <x:c r="C86" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -2742,7 +2666,7 @@
       </x:c>
     </x:row>
     <x:row r="87" spans="1:10" outlineLevel="2">
-      <x:c r="B87" s="40" t="s"/>
+      <x:c r="B87" s="35" t="s"/>
       <x:c r="C87" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -2753,7 +2677,7 @@
       <x:c r="H87" s="34" t="s"/>
     </x:row>
     <x:row r="88" spans="1:10" outlineLevel="3">
-      <x:c r="B88" s="40" t="s"/>
+      <x:c r="B88" s="35" t="s"/>
       <x:c r="C88" s="36" t="s"/>
       <x:c r="D88" s="37" t="n">
         <x:v>1148</x:v>
@@ -2772,7 +2696,7 @@
       </x:c>
     </x:row>
     <x:row r="89" spans="1:10" outlineLevel="2">
-      <x:c r="B89" s="43" t="s"/>
+      <x:c r="B89" s="35" t="s"/>
       <x:c r="C89" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -2817,7 +2741,7 @@
       <x:c r="H91" s="34" t="s"/>
     </x:row>
     <x:row r="92" spans="1:10" outlineLevel="2">
-      <x:c r="B92" s="39" t="s"/>
+      <x:c r="B92" s="35" t="s"/>
       <x:c r="C92" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2828,8 +2752,8 @@
       <x:c r="H92" s="34" t="s"/>
     </x:row>
     <x:row r="93" spans="1:10" outlineLevel="3">
-      <x:c r="B93" s="40" t="s"/>
-      <x:c r="C93" s="41" t="s"/>
+      <x:c r="B93" s="35" t="s"/>
+      <x:c r="C93" s="36" t="s"/>
       <x:c r="D93" s="37" t="n">
         <x:v>1018</x:v>
       </x:c>
@@ -2847,8 +2771,8 @@
       </x:c>
     </x:row>
     <x:row r="94" spans="1:10" outlineLevel="3">
-      <x:c r="B94" s="40" t="s"/>
-      <x:c r="C94" s="42" t="s"/>
+      <x:c r="B94" s="35" t="s"/>
+      <x:c r="C94" s="36" t="s"/>
       <x:c r="D94" s="37" t="n">
         <x:v>1118</x:v>
       </x:c>
@@ -2866,7 +2790,7 @@
       </x:c>
     </x:row>
     <x:row r="95" spans="1:10" outlineLevel="2">
-      <x:c r="B95" s="40" t="s"/>
+      <x:c r="B95" s="35" t="s"/>
       <x:c r="C95" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -2883,7 +2807,7 @@
       </x:c>
     </x:row>
     <x:row r="96" spans="1:10" outlineLevel="2">
-      <x:c r="B96" s="40" t="s"/>
+      <x:c r="B96" s="35" t="s"/>
       <x:c r="C96" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -2894,8 +2818,8 @@
       <x:c r="H96" s="34" t="s"/>
     </x:row>
     <x:row r="97" spans="1:10" outlineLevel="3">
-      <x:c r="B97" s="40" t="s"/>
-      <x:c r="C97" s="41" t="s"/>
+      <x:c r="B97" s="35" t="s"/>
+      <x:c r="C97" s="36" t="s"/>
       <x:c r="D97" s="37" t="n">
         <x:v>1162</x:v>
       </x:c>
@@ -2913,8 +2837,8 @@
       </x:c>
     </x:row>
     <x:row r="98" spans="1:10" outlineLevel="3">
-      <x:c r="B98" s="40" t="s"/>
-      <x:c r="C98" s="44" t="s"/>
+      <x:c r="B98" s="35" t="s"/>
+      <x:c r="C98" s="36" t="s"/>
       <x:c r="D98" s="37" t="n">
         <x:v>1031</x:v>
       </x:c>
@@ -2932,8 +2856,8 @@
       </x:c>
     </x:row>
     <x:row r="99" spans="1:10" outlineLevel="3">
-      <x:c r="B99" s="40" t="s"/>
-      <x:c r="C99" s="44" t="s"/>
+      <x:c r="B99" s="35" t="s"/>
+      <x:c r="C99" s="36" t="s"/>
       <x:c r="D99" s="37" t="n">
         <x:v>1064</x:v>
       </x:c>
@@ -2951,8 +2875,8 @@
       </x:c>
     </x:row>
     <x:row r="100" spans="1:10" outlineLevel="3">
-      <x:c r="B100" s="40" t="s"/>
-      <x:c r="C100" s="44" t="s"/>
+      <x:c r="B100" s="35" t="s"/>
+      <x:c r="C100" s="36" t="s"/>
       <x:c r="D100" s="37" t="n">
         <x:v>1131</x:v>
       </x:c>
@@ -2970,8 +2894,8 @@
       </x:c>
     </x:row>
     <x:row r="101" spans="1:10" outlineLevel="3">
-      <x:c r="B101" s="40" t="s"/>
-      <x:c r="C101" s="44" t="s"/>
+      <x:c r="B101" s="35" t="s"/>
+      <x:c r="C101" s="36" t="s"/>
       <x:c r="D101" s="37" t="n">
         <x:v>1058</x:v>
       </x:c>
@@ -2989,8 +2913,8 @@
       </x:c>
     </x:row>
     <x:row r="102" spans="1:10" outlineLevel="3">
-      <x:c r="B102" s="40" t="s"/>
-      <x:c r="C102" s="42" t="s"/>
+      <x:c r="B102" s="35" t="s"/>
+      <x:c r="C102" s="36" t="s"/>
       <x:c r="D102" s="37" t="n">
         <x:v>1062</x:v>
       </x:c>
@@ -3008,7 +2932,7 @@
       </x:c>
     </x:row>
     <x:row r="103" spans="1:10" outlineLevel="2">
-      <x:c r="B103" s="43" t="s"/>
+      <x:c r="B103" s="35" t="s"/>
       <x:c r="C103" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -3053,7 +2977,7 @@
       <x:c r="H105" s="34" t="s"/>
     </x:row>
     <x:row r="106" spans="1:10" outlineLevel="2">
-      <x:c r="B106" s="39" t="s"/>
+      <x:c r="B106" s="35" t="s"/>
       <x:c r="C106" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -3064,8 +2988,8 @@
       <x:c r="H106" s="34" t="s"/>
     </x:row>
     <x:row r="107" spans="1:10" outlineLevel="3">
-      <x:c r="B107" s="40" t="s"/>
-      <x:c r="C107" s="41" t="s"/>
+      <x:c r="B107" s="35" t="s"/>
+      <x:c r="C107" s="36" t="s"/>
       <x:c r="D107" s="37" t="n">
         <x:v>1066</x:v>
       </x:c>
@@ -3083,8 +3007,8 @@
       </x:c>
     </x:row>
     <x:row r="108" spans="1:10" outlineLevel="3">
-      <x:c r="B108" s="40" t="s"/>
-      <x:c r="C108" s="44" t="s"/>
+      <x:c r="B108" s="35" t="s"/>
+      <x:c r="C108" s="36" t="s"/>
       <x:c r="D108" s="37" t="n">
         <x:v>1205</x:v>
       </x:c>
@@ -3102,8 +3026,8 @@
       </x:c>
     </x:row>
     <x:row r="109" spans="1:10" outlineLevel="3">
-      <x:c r="B109" s="40" t="s"/>
-      <x:c r="C109" s="42" t="s"/>
+      <x:c r="B109" s="35" t="s"/>
+      <x:c r="C109" s="36" t="s"/>
       <x:c r="D109" s="37" t="n">
         <x:v>1166</x:v>
       </x:c>
@@ -3121,7 +3045,7 @@
       </x:c>
     </x:row>
     <x:row r="110" spans="1:10" outlineLevel="2">
-      <x:c r="B110" s="43" t="s"/>
+      <x:c r="B110" s="35" t="s"/>
       <x:c r="C110" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -3166,7 +3090,7 @@
       <x:c r="H112" s="34" t="s"/>
     </x:row>
     <x:row r="113" spans="1:10" outlineLevel="2">
-      <x:c r="B113" s="39" t="s"/>
+      <x:c r="B113" s="35" t="s"/>
       <x:c r="C113" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3177,7 +3101,7 @@
       <x:c r="H113" s="34" t="s"/>
     </x:row>
     <x:row r="114" spans="1:10" outlineLevel="3">
-      <x:c r="B114" s="40" t="s"/>
+      <x:c r="B114" s="35" t="s"/>
       <x:c r="C114" s="36" t="s"/>
       <x:c r="D114" s="37" t="n">
         <x:v>1104</x:v>
@@ -3196,7 +3120,7 @@
       </x:c>
     </x:row>
     <x:row r="115" spans="1:10" outlineLevel="2">
-      <x:c r="B115" s="40" t="s"/>
+      <x:c r="B115" s="35" t="s"/>
       <x:c r="C115" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -3213,7 +3137,7 @@
       </x:c>
     </x:row>
     <x:row r="116" spans="1:10" outlineLevel="2">
-      <x:c r="B116" s="40" t="s"/>
+      <x:c r="B116" s="35" t="s"/>
       <x:c r="C116" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -3224,7 +3148,7 @@
       <x:c r="H116" s="34" t="s"/>
     </x:row>
     <x:row r="117" spans="1:10" outlineLevel="3">
-      <x:c r="B117" s="40" t="s"/>
+      <x:c r="B117" s="35" t="s"/>
       <x:c r="C117" s="36" t="s"/>
       <x:c r="D117" s="37" t="n">
         <x:v>1292</x:v>
@@ -3243,7 +3167,7 @@
       </x:c>
     </x:row>
     <x:row r="118" spans="1:10" outlineLevel="2">
-      <x:c r="B118" s="43" t="s"/>
+      <x:c r="B118" s="35" t="s"/>
       <x:c r="C118" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -3288,7 +3212,7 @@
       <x:c r="H120" s="34" t="s"/>
     </x:row>
     <x:row r="121" spans="1:10" outlineLevel="2">
-      <x:c r="B121" s="39" t="s"/>
+      <x:c r="B121" s="35" t="s"/>
       <x:c r="C121" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3299,7 +3223,7 @@
       <x:c r="H121" s="34" t="s"/>
     </x:row>
     <x:row r="122" spans="1:10" outlineLevel="3">
-      <x:c r="B122" s="40" t="s"/>
+      <x:c r="B122" s="35" t="s"/>
       <x:c r="C122" s="36" t="s"/>
       <x:c r="D122" s="37" t="n">
         <x:v>1134</x:v>
@@ -3318,7 +3242,7 @@
       </x:c>
     </x:row>
     <x:row r="123" spans="1:10" outlineLevel="2">
-      <x:c r="B123" s="43" t="s"/>
+      <x:c r="B123" s="35" t="s"/>
       <x:c r="C123" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -3363,7 +3287,7 @@
       <x:c r="H125" s="34" t="s"/>
     </x:row>
     <x:row r="126" spans="1:10" outlineLevel="2">
-      <x:c r="B126" s="39" t="s"/>
+      <x:c r="B126" s="35" t="s"/>
       <x:c r="C126" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3374,7 +3298,7 @@
       <x:c r="H126" s="34" t="s"/>
     </x:row>
     <x:row r="127" spans="1:10" outlineLevel="3">
-      <x:c r="B127" s="40" t="s"/>
+      <x:c r="B127" s="35" t="s"/>
       <x:c r="C127" s="36" t="s"/>
       <x:c r="D127" s="37" t="n">
         <x:v>1004</x:v>
@@ -3393,7 +3317,7 @@
       </x:c>
     </x:row>
     <x:row r="128" spans="1:10" outlineLevel="2">
-      <x:c r="B128" s="40" t="s"/>
+      <x:c r="B128" s="35" t="s"/>
       <x:c r="C128" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -3410,7 +3334,7 @@
       </x:c>
     </x:row>
     <x:row r="129" spans="1:10" outlineLevel="2">
-      <x:c r="B129" s="40" t="s"/>
+      <x:c r="B129" s="35" t="s"/>
       <x:c r="C129" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -3421,8 +3345,8 @@
       <x:c r="H129" s="34" t="s"/>
     </x:row>
     <x:row r="130" spans="1:10" outlineLevel="3">
-      <x:c r="B130" s="40" t="s"/>
-      <x:c r="C130" s="41" t="s"/>
+      <x:c r="B130" s="35" t="s"/>
+      <x:c r="C130" s="36" t="s"/>
       <x:c r="D130" s="37" t="n">
         <x:v>1020</x:v>
       </x:c>
@@ -3440,8 +3364,8 @@
       </x:c>
     </x:row>
     <x:row r="131" spans="1:10" outlineLevel="3">
-      <x:c r="B131" s="40" t="s"/>
-      <x:c r="C131" s="42" t="s"/>
+      <x:c r="B131" s="35" t="s"/>
+      <x:c r="C131" s="36" t="s"/>
       <x:c r="D131" s="37" t="n">
         <x:v>1120</x:v>
       </x:c>
@@ -3459,7 +3383,7 @@
       </x:c>
     </x:row>
     <x:row r="132" spans="1:10" outlineLevel="2">
-      <x:c r="B132" s="40" t="s"/>
+      <x:c r="B132" s="35" t="s"/>
       <x:c r="C132" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -3476,7 +3400,7 @@
       </x:c>
     </x:row>
     <x:row r="133" spans="1:10" outlineLevel="2">
-      <x:c r="B133" s="40" t="s"/>
+      <x:c r="B133" s="35" t="s"/>
       <x:c r="C133" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -3487,8 +3411,8 @@
       <x:c r="H133" s="34" t="s"/>
     </x:row>
     <x:row r="134" spans="1:10" outlineLevel="3">
-      <x:c r="B134" s="40" t="s"/>
-      <x:c r="C134" s="41" t="s"/>
+      <x:c r="B134" s="35" t="s"/>
+      <x:c r="C134" s="36" t="s"/>
       <x:c r="D134" s="37" t="n">
         <x:v>1295</x:v>
       </x:c>
@@ -3506,8 +3430,8 @@
       </x:c>
     </x:row>
     <x:row r="135" spans="1:10" outlineLevel="3">
-      <x:c r="B135" s="40" t="s"/>
-      <x:c r="C135" s="42" t="s"/>
+      <x:c r="B135" s="35" t="s"/>
+      <x:c r="C135" s="36" t="s"/>
       <x:c r="D135" s="37" t="n">
         <x:v>1095</x:v>
       </x:c>
@@ -3525,7 +3449,7 @@
       </x:c>
     </x:row>
     <x:row r="136" spans="1:10" outlineLevel="2">
-      <x:c r="B136" s="43" t="s"/>
+      <x:c r="B136" s="35" t="s"/>
       <x:c r="C136" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -3570,7 +3494,7 @@
       <x:c r="H138" s="34" t="s"/>
     </x:row>
     <x:row r="139" spans="1:10" outlineLevel="2">
-      <x:c r="B139" s="39" t="s"/>
+      <x:c r="B139" s="35" t="s"/>
       <x:c r="C139" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3581,7 +3505,7 @@
       <x:c r="H139" s="34" t="s"/>
     </x:row>
     <x:row r="140" spans="1:10" outlineLevel="3">
-      <x:c r="B140" s="40" t="s"/>
+      <x:c r="B140" s="35" t="s"/>
       <x:c r="C140" s="36" t="s"/>
       <x:c r="D140" s="37" t="n">
         <x:v>1260</x:v>
@@ -3600,7 +3524,7 @@
       </x:c>
     </x:row>
     <x:row r="141" spans="1:10" outlineLevel="2">
-      <x:c r="B141" s="40" t="s"/>
+      <x:c r="B141" s="35" t="s"/>
       <x:c r="C141" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -3617,7 +3541,7 @@
       </x:c>
     </x:row>
     <x:row r="142" spans="1:10" outlineLevel="2">
-      <x:c r="B142" s="40" t="s"/>
+      <x:c r="B142" s="35" t="s"/>
       <x:c r="C142" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -3628,7 +3552,7 @@
       <x:c r="H142" s="34" t="s"/>
     </x:row>
     <x:row r="143" spans="1:10" outlineLevel="3">
-      <x:c r="B143" s="40" t="s"/>
+      <x:c r="B143" s="35" t="s"/>
       <x:c r="C143" s="36" t="s"/>
       <x:c r="D143" s="37" t="n">
         <x:v>1078</x:v>
@@ -3647,7 +3571,7 @@
       </x:c>
     </x:row>
     <x:row r="144" spans="1:10" outlineLevel="2">
-      <x:c r="B144" s="43" t="s"/>
+      <x:c r="B144" s="35" t="s"/>
       <x:c r="C144" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -3692,7 +3616,7 @@
       <x:c r="H146" s="34" t="s"/>
     </x:row>
     <x:row r="147" spans="1:10" outlineLevel="2">
-      <x:c r="B147" s="39" t="s"/>
+      <x:c r="B147" s="35" t="s"/>
       <x:c r="C147" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3703,8 +3627,8 @@
       <x:c r="H147" s="34" t="s"/>
     </x:row>
     <x:row r="148" spans="1:10" outlineLevel="3">
-      <x:c r="B148" s="40" t="s"/>
-      <x:c r="C148" s="41" t="s"/>
+      <x:c r="B148" s="35" t="s"/>
+      <x:c r="C148" s="36" t="s"/>
       <x:c r="D148" s="37" t="n">
         <x:v>1046</x:v>
       </x:c>
@@ -3722,8 +3646,8 @@
       </x:c>
     </x:row>
     <x:row r="149" spans="1:10" outlineLevel="3">
-      <x:c r="B149" s="40" t="s"/>
-      <x:c r="C149" s="42" t="s"/>
+      <x:c r="B149" s="35" t="s"/>
+      <x:c r="C149" s="36" t="s"/>
       <x:c r="D149" s="37" t="n">
         <x:v>1146</x:v>
       </x:c>
@@ -3741,7 +3665,7 @@
       </x:c>
     </x:row>
     <x:row r="150" spans="1:10" outlineLevel="2">
-      <x:c r="B150" s="40" t="s"/>
+      <x:c r="B150" s="35" t="s"/>
       <x:c r="C150" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -3758,7 +3682,7 @@
       </x:c>
     </x:row>
     <x:row r="151" spans="1:10" outlineLevel="2">
-      <x:c r="B151" s="40" t="s"/>
+      <x:c r="B151" s="35" t="s"/>
       <x:c r="C151" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -3769,8 +3693,8 @@
       <x:c r="H151" s="34" t="s"/>
     </x:row>
     <x:row r="152" spans="1:10" outlineLevel="3">
-      <x:c r="B152" s="40" t="s"/>
-      <x:c r="C152" s="41" t="s"/>
+      <x:c r="B152" s="35" t="s"/>
+      <x:c r="C152" s="36" t="s"/>
       <x:c r="D152" s="37" t="n">
         <x:v>1098</x:v>
       </x:c>
@@ -3788,8 +3712,8 @@
       </x:c>
     </x:row>
     <x:row r="153" spans="1:10" outlineLevel="3">
-      <x:c r="B153" s="40" t="s"/>
-      <x:c r="C153" s="44" t="s"/>
+      <x:c r="B153" s="35" t="s"/>
+      <x:c r="C153" s="36" t="s"/>
       <x:c r="D153" s="37" t="n">
         <x:v>1298</x:v>
       </x:c>
@@ -3807,8 +3731,8 @@
       </x:c>
     </x:row>
     <x:row r="154" spans="1:10" outlineLevel="3">
-      <x:c r="B154" s="40" t="s"/>
-      <x:c r="C154" s="42" t="s"/>
+      <x:c r="B154" s="35" t="s"/>
+      <x:c r="C154" s="36" t="s"/>
       <x:c r="D154" s="37" t="n">
         <x:v>1198</x:v>
       </x:c>
@@ -3826,7 +3750,7 @@
       </x:c>
     </x:row>
     <x:row r="155" spans="1:10" outlineLevel="2">
-      <x:c r="B155" s="43" t="s"/>
+      <x:c r="B155" s="35" t="s"/>
       <x:c r="C155" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -3871,7 +3795,7 @@
       <x:c r="H157" s="34" t="s"/>
     </x:row>
     <x:row r="158" spans="1:10" outlineLevel="2">
-      <x:c r="B158" s="39" t="s"/>
+      <x:c r="B158" s="35" t="s"/>
       <x:c r="C158" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -3882,7 +3806,7 @@
       <x:c r="H158" s="34" t="s"/>
     </x:row>
     <x:row r="159" spans="1:10" outlineLevel="3">
-      <x:c r="B159" s="40" t="s"/>
+      <x:c r="B159" s="35" t="s"/>
       <x:c r="C159" s="36" t="s"/>
       <x:c r="D159" s="37" t="n">
         <x:v>1130</x:v>
@@ -3901,7 +3825,7 @@
       </x:c>
     </x:row>
     <x:row r="160" spans="1:10" outlineLevel="2">
-      <x:c r="B160" s="43" t="s"/>
+      <x:c r="B160" s="35" t="s"/>
       <x:c r="C160" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -3946,7 +3870,7 @@
       <x:c r="H162" s="34" t="s"/>
     </x:row>
     <x:row r="163" spans="1:10" outlineLevel="2">
-      <x:c r="B163" s="39" t="s"/>
+      <x:c r="B163" s="35" t="s"/>
       <x:c r="C163" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -3957,8 +3881,8 @@
       <x:c r="H163" s="34" t="s"/>
     </x:row>
     <x:row r="164" spans="1:10" outlineLevel="3">
-      <x:c r="B164" s="40" t="s"/>
-      <x:c r="C164" s="41" t="s"/>
+      <x:c r="B164" s="35" t="s"/>
+      <x:c r="C164" s="36" t="s"/>
       <x:c r="D164" s="37" t="n">
         <x:v>1048</x:v>
       </x:c>
@@ -3976,8 +3900,8 @@
       </x:c>
     </x:row>
     <x:row r="165" spans="1:10" outlineLevel="3">
-      <x:c r="B165" s="40" t="s"/>
-      <x:c r="C165" s="42" t="s"/>
+      <x:c r="B165" s="35" t="s"/>
+      <x:c r="C165" s="36" t="s"/>
       <x:c r="D165" s="37" t="n">
         <x:v>1054</x:v>
       </x:c>
@@ -3995,7 +3919,7 @@
       </x:c>
     </x:row>
     <x:row r="166" spans="1:10" outlineLevel="2">
-      <x:c r="B166" s="43" t="s"/>
+      <x:c r="B166" s="35" t="s"/>
       <x:c r="C166" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -4040,7 +3964,7 @@
       <x:c r="H168" s="34" t="s"/>
     </x:row>
     <x:row r="169" spans="1:10" outlineLevel="2">
-      <x:c r="B169" s="39" t="s"/>
+      <x:c r="B169" s="35" t="s"/>
       <x:c r="C169" s="29" t="s">
         <x:v>34</x:v>
       </x:c>
@@ -4051,7 +3975,7 @@
       <x:c r="H169" s="34" t="s"/>
     </x:row>
     <x:row r="170" spans="1:10" outlineLevel="3">
-      <x:c r="B170" s="40" t="s"/>
+      <x:c r="B170" s="35" t="s"/>
       <x:c r="C170" s="36" t="s"/>
       <x:c r="D170" s="37" t="n">
         <x:v>1086</x:v>
@@ -4070,7 +3994,7 @@
       </x:c>
     </x:row>
     <x:row r="171" spans="1:10" outlineLevel="2">
-      <x:c r="B171" s="40" t="s"/>
+      <x:c r="B171" s="35" t="s"/>
       <x:c r="C171" s="29" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -4087,7 +4011,7 @@
       </x:c>
     </x:row>
     <x:row r="172" spans="1:10" outlineLevel="2">
-      <x:c r="B172" s="40" t="s"/>
+      <x:c r="B172" s="35" t="s"/>
       <x:c r="C172" s="29" t="s">
         <x:v>56</x:v>
       </x:c>
@@ -4098,8 +4022,8 @@
       <x:c r="H172" s="34" t="s"/>
     </x:row>
     <x:row r="173" spans="1:10" outlineLevel="3">
-      <x:c r="B173" s="40" t="s"/>
-      <x:c r="C173" s="41" t="s"/>
+      <x:c r="B173" s="35" t="s"/>
+      <x:c r="C173" s="36" t="s"/>
       <x:c r="D173" s="37" t="n">
         <x:v>1209</x:v>
       </x:c>
@@ -4117,8 +4041,8 @@
       </x:c>
     </x:row>
     <x:row r="174" spans="1:10" outlineLevel="3">
-      <x:c r="B174" s="40" t="s"/>
-      <x:c r="C174" s="44" t="s"/>
+      <x:c r="B174" s="35" t="s"/>
+      <x:c r="C174" s="36" t="s"/>
       <x:c r="D174" s="37" t="n">
         <x:v>1109</x:v>
       </x:c>
@@ -4136,8 +4060,8 @@
       </x:c>
     </x:row>
     <x:row r="175" spans="1:10" outlineLevel="3">
-      <x:c r="B175" s="40" t="s"/>
-      <x:c r="C175" s="42" t="s"/>
+      <x:c r="B175" s="35" t="s"/>
+      <x:c r="C175" s="36" t="s"/>
       <x:c r="D175" s="37" t="n">
         <x:v>1009</x:v>
       </x:c>
@@ -4155,7 +4079,7 @@
       </x:c>
     </x:row>
     <x:row r="176" spans="1:10" outlineLevel="2">
-      <x:c r="B176" s="40" t="s"/>
+      <x:c r="B176" s="35" t="s"/>
       <x:c r="C176" s="29" t="s">
         <x:v>57</x:v>
       </x:c>
@@ -4172,7 +4096,7 @@
       </x:c>
     </x:row>
     <x:row r="177" spans="1:10" outlineLevel="2">
-      <x:c r="B177" s="40" t="s"/>
+      <x:c r="B177" s="35" t="s"/>
       <x:c r="C177" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -4183,7 +4107,7 @@
       <x:c r="H177" s="34" t="s"/>
     </x:row>
     <x:row r="178" spans="1:10" outlineLevel="3">
-      <x:c r="B178" s="40" t="s"/>
+      <x:c r="B178" s="35" t="s"/>
       <x:c r="C178" s="36" t="s"/>
       <x:c r="D178" s="37" t="n">
         <x:v>1090</x:v>
@@ -4202,7 +4126,7 @@
       </x:c>
     </x:row>
     <x:row r="179" spans="1:10" outlineLevel="2">
-      <x:c r="B179" s="40" t="s"/>
+      <x:c r="B179" s="35" t="s"/>
       <x:c r="C179" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -4219,7 +4143,7 @@
       </x:c>
     </x:row>
     <x:row r="180" spans="1:10" outlineLevel="2">
-      <x:c r="B180" s="40" t="s"/>
+      <x:c r="B180" s="35" t="s"/>
       <x:c r="C180" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -4230,8 +4154,8 @@
       <x:c r="H180" s="34" t="s"/>
     </x:row>
     <x:row r="181" spans="1:10" outlineLevel="3">
-      <x:c r="B181" s="40" t="s"/>
-      <x:c r="C181" s="41" t="s"/>
+      <x:c r="B181" s="35" t="s"/>
+      <x:c r="C181" s="36" t="s"/>
       <x:c r="D181" s="37" t="n">
         <x:v>1056</x:v>
       </x:c>
@@ -4249,8 +4173,8 @@
       </x:c>
     </x:row>
     <x:row r="182" spans="1:10" outlineLevel="3">
-      <x:c r="B182" s="40" t="s"/>
-      <x:c r="C182" s="44" t="s"/>
+      <x:c r="B182" s="35" t="s"/>
+      <x:c r="C182" s="36" t="s"/>
       <x:c r="D182" s="37" t="n">
         <x:v>1197</x:v>
       </x:c>
@@ -4268,8 +4192,8 @@
       </x:c>
     </x:row>
     <x:row r="183" spans="1:10" outlineLevel="3">
-      <x:c r="B183" s="40" t="s"/>
-      <x:c r="C183" s="42" t="s"/>
+      <x:c r="B183" s="35" t="s"/>
+      <x:c r="C183" s="36" t="s"/>
       <x:c r="D183" s="37" t="n">
         <x:v>1156</x:v>
       </x:c>
@@ -4287,7 +4211,7 @@
       </x:c>
     </x:row>
     <x:row r="184" spans="1:10" outlineLevel="2">
-      <x:c r="B184" s="40" t="s"/>
+      <x:c r="B184" s="35" t="s"/>
       <x:c r="C184" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -4304,7 +4228,7 @@
       </x:c>
     </x:row>
     <x:row r="185" spans="1:10" outlineLevel="2">
-      <x:c r="B185" s="40" t="s"/>
+      <x:c r="B185" s="35" t="s"/>
       <x:c r="C185" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -4315,7 +4239,7 @@
       <x:c r="H185" s="34" t="s"/>
     </x:row>
     <x:row r="186" spans="1:10" outlineLevel="3">
-      <x:c r="B186" s="40" t="s"/>
+      <x:c r="B186" s="35" t="s"/>
       <x:c r="C186" s="36" t="s"/>
       <x:c r="D186" s="37" t="n">
         <x:v>1165</x:v>
@@ -4334,7 +4258,7 @@
       </x:c>
     </x:row>
     <x:row r="187" spans="1:10" outlineLevel="2">
-      <x:c r="B187" s="43" t="s"/>
+      <x:c r="B187" s="35" t="s"/>
       <x:c r="C187" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -4379,7 +4303,7 @@
       <x:c r="H189" s="34" t="s"/>
     </x:row>
     <x:row r="190" spans="1:10" outlineLevel="2">
-      <x:c r="B190" s="39" t="s"/>
+      <x:c r="B190" s="35" t="s"/>
       <x:c r="C190" s="29" t="s">
         <x:v>34</x:v>
       </x:c>
@@ -4390,7 +4314,7 @@
       <x:c r="H190" s="34" t="s"/>
     </x:row>
     <x:row r="191" spans="1:10" outlineLevel="3">
-      <x:c r="B191" s="40" t="s"/>
+      <x:c r="B191" s="35" t="s"/>
       <x:c r="C191" s="36" t="s"/>
       <x:c r="D191" s="37" t="n">
         <x:v>1133</x:v>
@@ -4409,7 +4333,7 @@
       </x:c>
     </x:row>
     <x:row r="192" spans="1:10" outlineLevel="2">
-      <x:c r="B192" s="40" t="s"/>
+      <x:c r="B192" s="35" t="s"/>
       <x:c r="C192" s="29" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -4426,7 +4350,7 @@
       </x:c>
     </x:row>
     <x:row r="193" spans="1:10" outlineLevel="2">
-      <x:c r="B193" s="40" t="s"/>
+      <x:c r="B193" s="35" t="s"/>
       <x:c r="C193" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -4437,7 +4361,7 @@
       <x:c r="H193" s="34" t="s"/>
     </x:row>
     <x:row r="194" spans="1:10" outlineLevel="3">
-      <x:c r="B194" s="40" t="s"/>
+      <x:c r="B194" s="35" t="s"/>
       <x:c r="C194" s="36" t="s"/>
       <x:c r="D194" s="37" t="n">
         <x:v>1024</x:v>
@@ -4456,7 +4380,7 @@
       </x:c>
     </x:row>
     <x:row r="195" spans="1:10" outlineLevel="2">
-      <x:c r="B195" s="40" t="s"/>
+      <x:c r="B195" s="35" t="s"/>
       <x:c r="C195" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -4473,7 +4397,7 @@
       </x:c>
     </x:row>
     <x:row r="196" spans="1:10" outlineLevel="2">
-      <x:c r="B196" s="40" t="s"/>
+      <x:c r="B196" s="35" t="s"/>
       <x:c r="C196" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -4484,7 +4408,7 @@
       <x:c r="H196" s="34" t="s"/>
     </x:row>
     <x:row r="197" spans="1:10" outlineLevel="3">
-      <x:c r="B197" s="40" t="s"/>
+      <x:c r="B197" s="35" t="s"/>
       <x:c r="C197" s="36" t="s"/>
       <x:c r="D197" s="37" t="n">
         <x:v>1089</x:v>
@@ -4503,7 +4427,7 @@
       </x:c>
     </x:row>
     <x:row r="198" spans="1:10" outlineLevel="2">
-      <x:c r="B198" s="43" t="s"/>
+      <x:c r="B198" s="35" t="s"/>
       <x:c r="C198" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -4548,7 +4472,7 @@
       <x:c r="H200" s="34" t="s"/>
     </x:row>
     <x:row r="201" spans="1:10" outlineLevel="2">
-      <x:c r="B201" s="39" t="s"/>
+      <x:c r="B201" s="35" t="s"/>
       <x:c r="C201" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -4559,7 +4483,7 @@
       <x:c r="H201" s="34" t="s"/>
     </x:row>
     <x:row r="202" spans="1:10" outlineLevel="3">
-      <x:c r="B202" s="40" t="s"/>
+      <x:c r="B202" s="35" t="s"/>
       <x:c r="C202" s="36" t="s"/>
       <x:c r="D202" s="37" t="n">
         <x:v>1019</x:v>
@@ -4578,7 +4502,7 @@
       </x:c>
     </x:row>
     <x:row r="203" spans="1:10" outlineLevel="2">
-      <x:c r="B203" s="43" t="s"/>
+      <x:c r="B203" s="35" t="s"/>
       <x:c r="C203" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -4623,7 +4547,7 @@
       <x:c r="H205" s="34" t="s"/>
     </x:row>
     <x:row r="206" spans="1:10" outlineLevel="2">
-      <x:c r="B206" s="39" t="s"/>
+      <x:c r="B206" s="35" t="s"/>
       <x:c r="C206" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -4634,7 +4558,7 @@
       <x:c r="H206" s="34" t="s"/>
     </x:row>
     <x:row r="207" spans="1:10" outlineLevel="3">
-      <x:c r="B207" s="40" t="s"/>
+      <x:c r="B207" s="35" t="s"/>
       <x:c r="C207" s="36" t="s"/>
       <x:c r="D207" s="37" t="n">
         <x:v>1069</x:v>
@@ -4653,7 +4577,7 @@
       </x:c>
     </x:row>
     <x:row r="208" spans="1:10" outlineLevel="2">
-      <x:c r="B208" s="43" t="s"/>
+      <x:c r="B208" s="35" t="s"/>
       <x:c r="C208" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -4698,7 +4622,7 @@
       <x:c r="H210" s="34" t="s"/>
     </x:row>
     <x:row r="211" spans="1:10" outlineLevel="2">
-      <x:c r="B211" s="39" t="s"/>
+      <x:c r="B211" s="35" t="s"/>
       <x:c r="C211" s="29" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -4709,7 +4633,7 @@
       <x:c r="H211" s="34" t="s"/>
     </x:row>
     <x:row r="212" spans="1:10" outlineLevel="3">
-      <x:c r="B212" s="40" t="s"/>
+      <x:c r="B212" s="35" t="s"/>
       <x:c r="C212" s="36" t="s"/>
       <x:c r="D212" s="37" t="n">
         <x:v>1081</x:v>
@@ -4728,7 +4652,7 @@
       </x:c>
     </x:row>
     <x:row r="213" spans="1:10" outlineLevel="2">
-      <x:c r="B213" s="40" t="s"/>
+      <x:c r="B213" s="35" t="s"/>
       <x:c r="C213" s="29" t="s">
         <x:v>29</x:v>
       </x:c>
@@ -4745,7 +4669,7 @@
       </x:c>
     </x:row>
     <x:row r="214" spans="1:10" outlineLevel="2">
-      <x:c r="B214" s="40" t="s"/>
+      <x:c r="B214" s="35" t="s"/>
       <x:c r="C214" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -4756,8 +4680,8 @@
       <x:c r="H214" s="34" t="s"/>
     </x:row>
     <x:row r="215" spans="1:10" outlineLevel="3">
-      <x:c r="B215" s="40" t="s"/>
-      <x:c r="C215" s="41" t="s"/>
+      <x:c r="B215" s="35" t="s"/>
+      <x:c r="C215" s="36" t="s"/>
       <x:c r="D215" s="37" t="n">
         <x:v>1103</x:v>
       </x:c>
@@ -4775,8 +4699,8 @@
       </x:c>
     </x:row>
     <x:row r="216" spans="1:10" outlineLevel="3">
-      <x:c r="B216" s="40" t="s"/>
-      <x:c r="C216" s="42" t="s"/>
+      <x:c r="B216" s="35" t="s"/>
+      <x:c r="C216" s="36" t="s"/>
       <x:c r="D216" s="37" t="n">
         <x:v>1063</x:v>
       </x:c>
@@ -4794,7 +4718,7 @@
       </x:c>
     </x:row>
     <x:row r="217" spans="1:10" outlineLevel="2">
-      <x:c r="B217" s="43" t="s"/>
+      <x:c r="B217" s="35" t="s"/>
       <x:c r="C217" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -4839,7 +4763,7 @@
       <x:c r="H219" s="34" t="s"/>
     </x:row>
     <x:row r="220" spans="1:10" outlineLevel="2">
-      <x:c r="B220" s="39" t="s"/>
+      <x:c r="B220" s="35" t="s"/>
       <x:c r="C220" s="29" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -4850,8 +4774,8 @@
       <x:c r="H220" s="34" t="s"/>
     </x:row>
     <x:row r="221" spans="1:10" outlineLevel="3">
-      <x:c r="B221" s="40" t="s"/>
-      <x:c r="C221" s="41" t="s"/>
+      <x:c r="B221" s="35" t="s"/>
+      <x:c r="C221" s="36" t="s"/>
       <x:c r="D221" s="37" t="n">
         <x:v>1016</x:v>
       </x:c>
@@ -4869,8 +4793,8 @@
       </x:c>
     </x:row>
     <x:row r="222" spans="1:10" outlineLevel="3">
-      <x:c r="B222" s="40" t="s"/>
-      <x:c r="C222" s="42" t="s"/>
+      <x:c r="B222" s="35" t="s"/>
+      <x:c r="C222" s="36" t="s"/>
       <x:c r="D222" s="37" t="n">
         <x:v>1116</x:v>
       </x:c>
@@ -4888,7 +4812,7 @@
       </x:c>
     </x:row>
     <x:row r="223" spans="1:10" outlineLevel="2">
-      <x:c r="B223" s="40" t="s"/>
+      <x:c r="B223" s="35" t="s"/>
       <x:c r="C223" s="29" t="s">
         <x:v>29</x:v>
       </x:c>
@@ -4905,7 +4829,7 @@
       </x:c>
     </x:row>
     <x:row r="224" spans="1:10" outlineLevel="2">
-      <x:c r="B224" s="40" t="s"/>
+      <x:c r="B224" s="35" t="s"/>
       <x:c r="C224" s="29" t="s">
         <x:v>34</x:v>
       </x:c>
@@ -4916,7 +4840,7 @@
       <x:c r="H224" s="34" t="s"/>
     </x:row>
     <x:row r="225" spans="1:10" outlineLevel="3">
-      <x:c r="B225" s="40" t="s"/>
+      <x:c r="B225" s="35" t="s"/>
       <x:c r="C225" s="36" t="s"/>
       <x:c r="D225" s="37" t="n">
         <x:v>1084</x:v>
@@ -4935,7 +4859,7 @@
       </x:c>
     </x:row>
     <x:row r="226" spans="1:10" outlineLevel="2">
-      <x:c r="B226" s="40" t="s"/>
+      <x:c r="B226" s="35" t="s"/>
       <x:c r="C226" s="29" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -4952,7 +4876,7 @@
       </x:c>
     </x:row>
     <x:row r="227" spans="1:10" outlineLevel="2">
-      <x:c r="B227" s="40" t="s"/>
+      <x:c r="B227" s="35" t="s"/>
       <x:c r="C227" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -4963,7 +4887,7 @@
       <x:c r="H227" s="34" t="s"/>
     </x:row>
     <x:row r="228" spans="1:10" outlineLevel="3">
-      <x:c r="B228" s="40" t="s"/>
+      <x:c r="B228" s="35" t="s"/>
       <x:c r="C228" s="36" t="s"/>
       <x:c r="D228" s="37" t="n">
         <x:v>1034</x:v>
@@ -4982,7 +4906,7 @@
       </x:c>
     </x:row>
     <x:row r="229" spans="1:10" outlineLevel="2">
-      <x:c r="B229" s="40" t="s"/>
+      <x:c r="B229" s="35" t="s"/>
       <x:c r="C229" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -4999,7 +4923,7 @@
       </x:c>
     </x:row>
     <x:row r="230" spans="1:10" outlineLevel="2">
-      <x:c r="B230" s="40" t="s"/>
+      <x:c r="B230" s="35" t="s"/>
       <x:c r="C230" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -5010,7 +4934,7 @@
       <x:c r="H230" s="34" t="s"/>
     </x:row>
     <x:row r="231" spans="1:10" outlineLevel="3">
-      <x:c r="B231" s="40" t="s"/>
+      <x:c r="B231" s="35" t="s"/>
       <x:c r="C231" s="36" t="s"/>
       <x:c r="D231" s="37" t="n">
         <x:v>1093</x:v>
@@ -5029,7 +4953,7 @@
       </x:c>
     </x:row>
     <x:row r="232" spans="1:10" outlineLevel="2">
-      <x:c r="B232" s="43" t="s"/>
+      <x:c r="B232" s="35" t="s"/>
       <x:c r="C232" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -5074,7 +4998,7 @@
       <x:c r="H234" s="34" t="s"/>
     </x:row>
     <x:row r="235" spans="1:10" outlineLevel="2">
-      <x:c r="B235" s="39" t="s"/>
+      <x:c r="B235" s="35" t="s"/>
       <x:c r="C235" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -5085,8 +5009,8 @@
       <x:c r="H235" s="34" t="s"/>
     </x:row>
     <x:row r="236" spans="1:10" outlineLevel="3">
-      <x:c r="B236" s="40" t="s"/>
-      <x:c r="C236" s="41" t="s"/>
+      <x:c r="B236" s="35" t="s"/>
+      <x:c r="C236" s="36" t="s"/>
       <x:c r="D236" s="37" t="n">
         <x:v>1015</x:v>
       </x:c>
@@ -5104,8 +5028,8 @@
       </x:c>
     </x:row>
     <x:row r="237" spans="1:10" outlineLevel="3">
-      <x:c r="B237" s="40" t="s"/>
-      <x:c r="C237" s="44" t="s"/>
+      <x:c r="B237" s="35" t="s"/>
+      <x:c r="C237" s="36" t="s"/>
       <x:c r="D237" s="37" t="n">
         <x:v>1315</x:v>
       </x:c>
@@ -5123,8 +5047,8 @@
       </x:c>
     </x:row>
     <x:row r="238" spans="1:10" outlineLevel="3">
-      <x:c r="B238" s="40" t="s"/>
-      <x:c r="C238" s="42" t="s"/>
+      <x:c r="B238" s="35" t="s"/>
+      <x:c r="C238" s="36" t="s"/>
       <x:c r="D238" s="37" t="n">
         <x:v>1215</x:v>
       </x:c>
@@ -5142,7 +5066,7 @@
       </x:c>
     </x:row>
     <x:row r="239" spans="1:10" outlineLevel="2">
-      <x:c r="B239" s="40" t="s"/>
+      <x:c r="B239" s="35" t="s"/>
       <x:c r="C239" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -5159,7 +5083,7 @@
       </x:c>
     </x:row>
     <x:row r="240" spans="1:10" outlineLevel="2">
-      <x:c r="B240" s="40" t="s"/>
+      <x:c r="B240" s="35" t="s"/>
       <x:c r="C240" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -5170,8 +5094,8 @@
       <x:c r="H240" s="34" t="s"/>
     </x:row>
     <x:row r="241" spans="1:10" outlineLevel="3">
-      <x:c r="B241" s="40" t="s"/>
-      <x:c r="C241" s="41" t="s"/>
+      <x:c r="B241" s="35" t="s"/>
+      <x:c r="C241" s="36" t="s"/>
       <x:c r="D241" s="37" t="n">
         <x:v>1128</x:v>
       </x:c>
@@ -5189,8 +5113,8 @@
       </x:c>
     </x:row>
     <x:row r="242" spans="1:10" outlineLevel="3">
-      <x:c r="B242" s="40" t="s"/>
-      <x:c r="C242" s="42" t="s"/>
+      <x:c r="B242" s="35" t="s"/>
+      <x:c r="C242" s="36" t="s"/>
       <x:c r="D242" s="37" t="n">
         <x:v>1028</x:v>
       </x:c>
@@ -5208,7 +5132,7 @@
       </x:c>
     </x:row>
     <x:row r="243" spans="1:10" outlineLevel="2">
-      <x:c r="B243" s="43" t="s"/>
+      <x:c r="B243" s="35" t="s"/>
       <x:c r="C243" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -5253,7 +5177,7 @@
       <x:c r="H245" s="34" t="s"/>
     </x:row>
     <x:row r="246" spans="1:10" outlineLevel="2">
-      <x:c r="B246" s="39" t="s"/>
+      <x:c r="B246" s="35" t="s"/>
       <x:c r="C246" s="29" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -5264,8 +5188,8 @@
       <x:c r="H246" s="34" t="s"/>
     </x:row>
     <x:row r="247" spans="1:10" outlineLevel="3">
-      <x:c r="B247" s="40" t="s"/>
-      <x:c r="C247" s="41" t="s"/>
+      <x:c r="B247" s="35" t="s"/>
+      <x:c r="C247" s="36" t="s"/>
       <x:c r="D247" s="37" t="n">
         <x:v>1141</x:v>
       </x:c>
@@ -5283,8 +5207,8 @@
       </x:c>
     </x:row>
     <x:row r="248" spans="1:10" outlineLevel="3">
-      <x:c r="B248" s="40" t="s"/>
-      <x:c r="C248" s="42" t="s"/>
+      <x:c r="B248" s="35" t="s"/>
+      <x:c r="C248" s="36" t="s"/>
       <x:c r="D248" s="37" t="n">
         <x:v>1041</x:v>
       </x:c>
@@ -5302,7 +5226,7 @@
       </x:c>
     </x:row>
     <x:row r="249" spans="1:10" outlineLevel="2">
-      <x:c r="B249" s="43" t="s"/>
+      <x:c r="B249" s="35" t="s"/>
       <x:c r="C249" s="29" t="s">
         <x:v>29</x:v>
       </x:c>
@@ -5347,7 +5271,7 @@
       <x:c r="H251" s="34" t="s"/>
     </x:row>
     <x:row r="252" spans="1:10" outlineLevel="2">
-      <x:c r="B252" s="39" t="s"/>
+      <x:c r="B252" s="35" t="s"/>
       <x:c r="C252" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -5358,8 +5282,8 @@
       <x:c r="H252" s="34" t="s"/>
     </x:row>
     <x:row r="253" spans="1:10" outlineLevel="3">
-      <x:c r="B253" s="40" t="s"/>
-      <x:c r="C253" s="41" t="s"/>
+      <x:c r="B253" s="35" t="s"/>
+      <x:c r="C253" s="36" t="s"/>
       <x:c r="D253" s="37" t="n">
         <x:v>1023</x:v>
       </x:c>
@@ -5377,8 +5301,8 @@
       </x:c>
     </x:row>
     <x:row r="254" spans="1:10" outlineLevel="3">
-      <x:c r="B254" s="40" t="s"/>
-      <x:c r="C254" s="42" t="s"/>
+      <x:c r="B254" s="35" t="s"/>
+      <x:c r="C254" s="36" t="s"/>
       <x:c r="D254" s="37" t="n">
         <x:v>1123</x:v>
       </x:c>
@@ -5396,7 +5320,7 @@
       </x:c>
     </x:row>
     <x:row r="255" spans="1:10" outlineLevel="2">
-      <x:c r="B255" s="40" t="s"/>
+      <x:c r="B255" s="35" t="s"/>
       <x:c r="C255" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -5413,7 +5337,7 @@
       </x:c>
     </x:row>
     <x:row r="256" spans="1:10" outlineLevel="2">
-      <x:c r="B256" s="40" t="s"/>
+      <x:c r="B256" s="35" t="s"/>
       <x:c r="C256" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -5424,8 +5348,8 @@
       <x:c r="H256" s="34" t="s"/>
     </x:row>
     <x:row r="257" spans="1:10" outlineLevel="3">
-      <x:c r="B257" s="40" t="s"/>
-      <x:c r="C257" s="41" t="s"/>
+      <x:c r="B257" s="35" t="s"/>
+      <x:c r="C257" s="36" t="s"/>
       <x:c r="D257" s="37" t="n">
         <x:v>1269</x:v>
       </x:c>
@@ -5443,8 +5367,8 @@
       </x:c>
     </x:row>
     <x:row r="258" spans="1:10" outlineLevel="3">
-      <x:c r="B258" s="40" t="s"/>
-      <x:c r="C258" s="42" t="s"/>
+      <x:c r="B258" s="35" t="s"/>
+      <x:c r="C258" s="36" t="s"/>
       <x:c r="D258" s="37" t="n">
         <x:v>1169</x:v>
       </x:c>
@@ -5462,7 +5386,7 @@
       </x:c>
     </x:row>
     <x:row r="259" spans="1:10" outlineLevel="2">
-      <x:c r="B259" s="40" t="s"/>
+      <x:c r="B259" s="35" t="s"/>
       <x:c r="C259" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -5479,7 +5403,7 @@
       </x:c>
     </x:row>
     <x:row r="260" spans="1:10" outlineLevel="2">
-      <x:c r="B260" s="40" t="s"/>
+      <x:c r="B260" s="35" t="s"/>
       <x:c r="C260" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -5490,8 +5414,8 @@
       <x:c r="H260" s="34" t="s"/>
     </x:row>
     <x:row r="261" spans="1:10" outlineLevel="3">
-      <x:c r="B261" s="40" t="s"/>
-      <x:c r="C261" s="41" t="s"/>
+      <x:c r="B261" s="35" t="s"/>
+      <x:c r="C261" s="36" t="s"/>
       <x:c r="D261" s="37" t="n">
         <x:v>1076</x:v>
       </x:c>
@@ -5509,8 +5433,8 @@
       </x:c>
     </x:row>
     <x:row r="262" spans="1:10" outlineLevel="3">
-      <x:c r="B262" s="40" t="s"/>
-      <x:c r="C262" s="42" t="s"/>
+      <x:c r="B262" s="35" t="s"/>
+      <x:c r="C262" s="36" t="s"/>
       <x:c r="D262" s="37" t="n">
         <x:v>1176</x:v>
       </x:c>
@@ -5528,7 +5452,7 @@
       </x:c>
     </x:row>
     <x:row r="263" spans="1:10" outlineLevel="2">
-      <x:c r="B263" s="43" t="s"/>
+      <x:c r="B263" s="35" t="s"/>
       <x:c r="C263" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -5573,7 +5497,7 @@
       <x:c r="H265" s="34" t="s"/>
     </x:row>
     <x:row r="266" spans="1:10" outlineLevel="2">
-      <x:c r="B266" s="39" t="s"/>
+      <x:c r="B266" s="35" t="s"/>
       <x:c r="C266" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -5584,8 +5508,8 @@
       <x:c r="H266" s="34" t="s"/>
     </x:row>
     <x:row r="267" spans="1:10" outlineLevel="3">
-      <x:c r="B267" s="40" t="s"/>
-      <x:c r="C267" s="41" t="s"/>
+      <x:c r="B267" s="35" t="s"/>
+      <x:c r="C267" s="36" t="s"/>
       <x:c r="D267" s="37" t="n">
         <x:v>1096</x:v>
       </x:c>
@@ -5603,8 +5527,8 @@
       </x:c>
     </x:row>
     <x:row r="268" spans="1:10" outlineLevel="3">
-      <x:c r="B268" s="40" t="s"/>
-      <x:c r="C268" s="42" t="s"/>
+      <x:c r="B268" s="35" t="s"/>
+      <x:c r="C268" s="36" t="s"/>
       <x:c r="D268" s="37" t="n">
         <x:v>1196</x:v>
       </x:c>
@@ -5622,7 +5546,7 @@
       </x:c>
     </x:row>
     <x:row r="269" spans="1:10" outlineLevel="2">
-      <x:c r="B269" s="43" t="s"/>
+      <x:c r="B269" s="35" t="s"/>
       <x:c r="C269" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -5667,7 +5591,7 @@
       <x:c r="H271" s="34" t="s"/>
     </x:row>
     <x:row r="272" spans="1:10" outlineLevel="2">
-      <x:c r="B272" s="39" t="s"/>
+      <x:c r="B272" s="35" t="s"/>
       <x:c r="C272" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -5678,7 +5602,7 @@
       <x:c r="H272" s="34" t="s"/>
     </x:row>
     <x:row r="273" spans="1:10" outlineLevel="3">
-      <x:c r="B273" s="40" t="s"/>
+      <x:c r="B273" s="35" t="s"/>
       <x:c r="C273" s="36" t="s"/>
       <x:c r="D273" s="37" t="n">
         <x:v>1158</x:v>
@@ -5697,7 +5621,7 @@
       </x:c>
     </x:row>
     <x:row r="274" spans="1:10" outlineLevel="2">
-      <x:c r="B274" s="43" t="s"/>
+      <x:c r="B274" s="35" t="s"/>
       <x:c r="C274" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -5742,7 +5666,7 @@
       <x:c r="H276" s="34" t="s"/>
     </x:row>
     <x:row r="277" spans="1:10" outlineLevel="2">
-      <x:c r="B277" s="39" t="s"/>
+      <x:c r="B277" s="35" t="s"/>
       <x:c r="C277" s="29" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -5753,8 +5677,8 @@
       <x:c r="H277" s="34" t="s"/>
     </x:row>
     <x:row r="278" spans="1:10" outlineLevel="3">
-      <x:c r="B278" s="40" t="s"/>
-      <x:c r="C278" s="41" t="s"/>
+      <x:c r="B278" s="35" t="s"/>
+      <x:c r="C278" s="36" t="s"/>
       <x:c r="D278" s="37" t="n">
         <x:v>1026</x:v>
       </x:c>
@@ -5772,8 +5696,8 @@
       </x:c>
     </x:row>
     <x:row r="279" spans="1:10" outlineLevel="3">
-      <x:c r="B279" s="40" t="s"/>
-      <x:c r="C279" s="42" t="s"/>
+      <x:c r="B279" s="35" t="s"/>
+      <x:c r="C279" s="36" t="s"/>
       <x:c r="D279" s="37" t="n">
         <x:v>1126</x:v>
       </x:c>
@@ -5791,7 +5715,7 @@
       </x:c>
     </x:row>
     <x:row r="280" spans="1:10" outlineLevel="2">
-      <x:c r="B280" s="40" t="s"/>
+      <x:c r="B280" s="35" t="s"/>
       <x:c r="C280" s="29" t="s">
         <x:v>29</x:v>
       </x:c>
@@ -5808,7 +5732,7 @@
       </x:c>
     </x:row>
     <x:row r="281" spans="1:10" outlineLevel="2">
-      <x:c r="B281" s="40" t="s"/>
+      <x:c r="B281" s="35" t="s"/>
       <x:c r="C281" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -5819,8 +5743,8 @@
       <x:c r="H281" s="34" t="s"/>
     </x:row>
     <x:row r="282" spans="1:10" outlineLevel="3">
-      <x:c r="B282" s="40" t="s"/>
-      <x:c r="C282" s="41" t="s"/>
+      <x:c r="B282" s="35" t="s"/>
+      <x:c r="C282" s="36" t="s"/>
       <x:c r="D282" s="37" t="n">
         <x:v>1013</x:v>
       </x:c>
@@ -5838,8 +5762,8 @@
       </x:c>
     </x:row>
     <x:row r="283" spans="1:10" outlineLevel="3">
-      <x:c r="B283" s="40" t="s"/>
-      <x:c r="C283" s="42" t="s"/>
+      <x:c r="B283" s="35" t="s"/>
+      <x:c r="C283" s="36" t="s"/>
       <x:c r="D283" s="37" t="n">
         <x:v>1113</x:v>
       </x:c>
@@ -5857,7 +5781,7 @@
       </x:c>
     </x:row>
     <x:row r="284" spans="1:10" outlineLevel="2">
-      <x:c r="B284" s="43" t="s"/>
+      <x:c r="B284" s="35" t="s"/>
       <x:c r="C284" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -5902,7 +5826,7 @@
       <x:c r="H286" s="34" t="s"/>
     </x:row>
     <x:row r="287" spans="1:10" outlineLevel="2">
-      <x:c r="B287" s="39" t="s"/>
+      <x:c r="B287" s="35" t="s"/>
       <x:c r="C287" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -5913,7 +5837,7 @@
       <x:c r="H287" s="34" t="s"/>
     </x:row>
     <x:row r="288" spans="1:10" outlineLevel="3">
-      <x:c r="B288" s="40" t="s"/>
+      <x:c r="B288" s="35" t="s"/>
       <x:c r="C288" s="36" t="s"/>
       <x:c r="D288" s="37" t="n">
         <x:v>1860</x:v>
@@ -5930,7 +5854,7 @@
       </x:c>
     </x:row>
     <x:row r="289" spans="1:10" outlineLevel="2">
-      <x:c r="B289" s="40" t="s"/>
+      <x:c r="B289" s="35" t="s"/>
       <x:c r="C289" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -5947,7 +5871,7 @@
       </x:c>
     </x:row>
     <x:row r="290" spans="1:10" outlineLevel="2">
-      <x:c r="B290" s="40" t="s"/>
+      <x:c r="B290" s="35" t="s"/>
       <x:c r="C290" s="29" t="s">
         <x:v>56</x:v>
       </x:c>
@@ -5958,7 +5882,7 @@
       <x:c r="H290" s="34" t="s"/>
     </x:row>
     <x:row r="291" spans="1:10" outlineLevel="3">
-      <x:c r="B291" s="40" t="s"/>
+      <x:c r="B291" s="35" t="s"/>
       <x:c r="C291" s="36" t="s"/>
       <x:c r="D291" s="37" t="n">
         <x:v>1309</x:v>
@@ -5977,7 +5901,7 @@
       </x:c>
     </x:row>
     <x:row r="292" spans="1:10" outlineLevel="2">
-      <x:c r="B292" s="40" t="s"/>
+      <x:c r="B292" s="35" t="s"/>
       <x:c r="C292" s="29" t="s">
         <x:v>57</x:v>
       </x:c>
@@ -5994,7 +5918,7 @@
       </x:c>
     </x:row>
     <x:row r="293" spans="1:10" outlineLevel="2">
-      <x:c r="B293" s="40" t="s"/>
+      <x:c r="B293" s="35" t="s"/>
       <x:c r="C293" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -6005,8 +5929,8 @@
       <x:c r="H293" s="34" t="s"/>
     </x:row>
     <x:row r="294" spans="1:10" outlineLevel="3">
-      <x:c r="B294" s="40" t="s"/>
-      <x:c r="C294" s="41" t="s"/>
+      <x:c r="B294" s="35" t="s"/>
+      <x:c r="C294" s="36" t="s"/>
       <x:c r="D294" s="37" t="n">
         <x:v>1030</x:v>
       </x:c>
@@ -6024,8 +5948,8 @@
       </x:c>
     </x:row>
     <x:row r="295" spans="1:10" outlineLevel="3">
-      <x:c r="B295" s="40" t="s"/>
-      <x:c r="C295" s="42" t="s"/>
+      <x:c r="B295" s="35" t="s"/>
+      <x:c r="C295" s="36" t="s"/>
       <x:c r="D295" s="37" t="n">
         <x:v>1097</x:v>
       </x:c>
@@ -6043,7 +5967,7 @@
       </x:c>
     </x:row>
     <x:row r="296" spans="1:10" outlineLevel="2">
-      <x:c r="B296" s="43" t="s"/>
+      <x:c r="B296" s="35" t="s"/>
       <x:c r="C296" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -6088,7 +6012,7 @@
       <x:c r="H298" s="34" t="s"/>
     </x:row>
     <x:row r="299" spans="1:10" outlineLevel="2">
-      <x:c r="B299" s="39" t="s"/>
+      <x:c r="B299" s="35" t="s"/>
       <x:c r="C299" s="29" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -6099,7 +6023,7 @@
       <x:c r="H299" s="34" t="s"/>
     </x:row>
     <x:row r="300" spans="1:10" outlineLevel="3">
-      <x:c r="B300" s="40" t="s"/>
+      <x:c r="B300" s="35" t="s"/>
       <x:c r="C300" s="36" t="s"/>
       <x:c r="D300" s="37" t="n">
         <x:v>1082</x:v>
@@ -6118,7 +6042,7 @@
       </x:c>
     </x:row>
     <x:row r="301" spans="1:10" outlineLevel="2">
-      <x:c r="B301" s="40" t="s"/>
+      <x:c r="B301" s="35" t="s"/>
       <x:c r="C301" s="29" t="s">
         <x:v>29</x:v>
       </x:c>
@@ -6135,7 +6059,7 @@
       </x:c>
     </x:row>
     <x:row r="302" spans="1:10" outlineLevel="2">
-      <x:c r="B302" s="40" t="s"/>
+      <x:c r="B302" s="35" t="s"/>
       <x:c r="C302" s="29" t="s">
         <x:v>56</x:v>
       </x:c>
@@ -6146,7 +6070,7 @@
       <x:c r="H302" s="34" t="s"/>
     </x:row>
     <x:row r="303" spans="1:10" outlineLevel="3">
-      <x:c r="B303" s="40" t="s"/>
+      <x:c r="B303" s="35" t="s"/>
       <x:c r="C303" s="36" t="s"/>
       <x:c r="D303" s="37" t="n">
         <x:v>1010</x:v>
@@ -6165,7 +6089,7 @@
       </x:c>
     </x:row>
     <x:row r="304" spans="1:10" outlineLevel="2">
-      <x:c r="B304" s="40" t="s"/>
+      <x:c r="B304" s="35" t="s"/>
       <x:c r="C304" s="29" t="s">
         <x:v>57</x:v>
       </x:c>
@@ -6182,7 +6106,7 @@
       </x:c>
     </x:row>
     <x:row r="305" spans="1:10" outlineLevel="2">
-      <x:c r="B305" s="40" t="s"/>
+      <x:c r="B305" s="35" t="s"/>
       <x:c r="C305" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -6193,8 +6117,8 @@
       <x:c r="H305" s="34" t="s"/>
     </x:row>
     <x:row r="306" spans="1:10" outlineLevel="3">
-      <x:c r="B306" s="40" t="s"/>
-      <x:c r="C306" s="41" t="s"/>
+      <x:c r="B306" s="35" t="s"/>
+      <x:c r="C306" s="36" t="s"/>
       <x:c r="D306" s="37" t="n">
         <x:v>1170</x:v>
       </x:c>
@@ -6212,8 +6136,8 @@
       </x:c>
     </x:row>
     <x:row r="307" spans="1:10" outlineLevel="3">
-      <x:c r="B307" s="40" t="s"/>
-      <x:c r="C307" s="42" t="s"/>
+      <x:c r="B307" s="35" t="s"/>
+      <x:c r="C307" s="36" t="s"/>
       <x:c r="D307" s="37" t="n">
         <x:v>1077</x:v>
       </x:c>
@@ -6231,7 +6155,7 @@
       </x:c>
     </x:row>
     <x:row r="308" spans="1:10" outlineLevel="2">
-      <x:c r="B308" s="43" t="s"/>
+      <x:c r="B308" s="35" t="s"/>
       <x:c r="C308" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -6276,7 +6200,7 @@
       <x:c r="H310" s="34" t="s"/>
     </x:row>
     <x:row r="311" spans="1:10" outlineLevel="2">
-      <x:c r="B311" s="39" t="s"/>
+      <x:c r="B311" s="35" t="s"/>
       <x:c r="C311" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -6287,8 +6211,8 @@
       <x:c r="H311" s="34" t="s"/>
     </x:row>
     <x:row r="312" spans="1:10" outlineLevel="3">
-      <x:c r="B312" s="40" t="s"/>
-      <x:c r="C312" s="41" t="s"/>
+      <x:c r="B312" s="35" t="s"/>
+      <x:c r="C312" s="36" t="s"/>
       <x:c r="D312" s="37" t="n">
         <x:v>1045</x:v>
       </x:c>
@@ -6306,8 +6230,8 @@
       </x:c>
     </x:row>
     <x:row r="313" spans="1:10" outlineLevel="3">
-      <x:c r="B313" s="40" t="s"/>
-      <x:c r="C313" s="42" t="s"/>
+      <x:c r="B313" s="35" t="s"/>
+      <x:c r="C313" s="36" t="s"/>
       <x:c r="D313" s="37" t="n">
         <x:v>1145</x:v>
       </x:c>
@@ -6325,7 +6249,7 @@
       </x:c>
     </x:row>
     <x:row r="314" spans="1:10" outlineLevel="2">
-      <x:c r="B314" s="40" t="s"/>
+      <x:c r="B314" s="35" t="s"/>
       <x:c r="C314" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -6342,7 +6266,7 @@
       </x:c>
     </x:row>
     <x:row r="315" spans="1:10" outlineLevel="2">
-      <x:c r="B315" s="40" t="s"/>
+      <x:c r="B315" s="35" t="s"/>
       <x:c r="C315" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -6353,8 +6277,8 @@
       <x:c r="H315" s="34" t="s"/>
     </x:row>
     <x:row r="316" spans="1:10" outlineLevel="3">
-      <x:c r="B316" s="40" t="s"/>
-      <x:c r="C316" s="41" t="s"/>
+      <x:c r="B316" s="35" t="s"/>
+      <x:c r="C316" s="36" t="s"/>
       <x:c r="D316" s="37" t="n">
         <x:v>1149</x:v>
       </x:c>
@@ -6372,8 +6296,8 @@
       </x:c>
     </x:row>
     <x:row r="317" spans="1:10" outlineLevel="3">
-      <x:c r="B317" s="40" t="s"/>
-      <x:c r="C317" s="42" t="s"/>
+      <x:c r="B317" s="35" t="s"/>
+      <x:c r="C317" s="36" t="s"/>
       <x:c r="D317" s="37" t="n">
         <x:v>1049</x:v>
       </x:c>
@@ -6391,7 +6315,7 @@
       </x:c>
     </x:row>
     <x:row r="318" spans="1:10" outlineLevel="2">
-      <x:c r="B318" s="43" t="s"/>
+      <x:c r="B318" s="35" t="s"/>
       <x:c r="C318" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -6436,7 +6360,7 @@
       <x:c r="H320" s="34" t="s"/>
     </x:row>
     <x:row r="321" spans="1:10" outlineLevel="2">
-      <x:c r="B321" s="39" t="s"/>
+      <x:c r="B321" s="35" t="s"/>
       <x:c r="C321" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -6447,7 +6371,7 @@
       <x:c r="H321" s="34" t="s"/>
     </x:row>
     <x:row r="322" spans="1:10" outlineLevel="3">
-      <x:c r="B322" s="40" t="s"/>
+      <x:c r="B322" s="35" t="s"/>
       <x:c r="C322" s="36" t="s"/>
       <x:c r="D322" s="37" t="n">
         <x:v>1092</x:v>
@@ -6466,7 +6390,7 @@
       </x:c>
     </x:row>
     <x:row r="323" spans="1:10" outlineLevel="2">
-      <x:c r="B323" s="43" t="s"/>
+      <x:c r="B323" s="35" t="s"/>
       <x:c r="C323" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -6511,7 +6435,7 @@
       <x:c r="H325" s="34" t="s"/>
     </x:row>
     <x:row r="326" spans="1:10" outlineLevel="2">
-      <x:c r="B326" s="39" t="s"/>
+      <x:c r="B326" s="35" t="s"/>
       <x:c r="C326" s="29" t="s">
         <x:v>34</x:v>
       </x:c>
@@ -6522,7 +6446,7 @@
       <x:c r="H326" s="34" t="s"/>
     </x:row>
     <x:row r="327" spans="1:10" outlineLevel="3">
-      <x:c r="B327" s="40" t="s"/>
+      <x:c r="B327" s="35" t="s"/>
       <x:c r="C327" s="36" t="s"/>
       <x:c r="D327" s="37" t="n">
         <x:v>1047</x:v>
@@ -6541,7 +6465,7 @@
       </x:c>
     </x:row>
     <x:row r="328" spans="1:10" outlineLevel="2">
-      <x:c r="B328" s="40" t="s"/>
+      <x:c r="B328" s="35" t="s"/>
       <x:c r="C328" s="29" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -6558,7 +6482,7 @@
       </x:c>
     </x:row>
     <x:row r="329" spans="1:10" outlineLevel="2">
-      <x:c r="B329" s="40" t="s"/>
+      <x:c r="B329" s="35" t="s"/>
       <x:c r="C329" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -6569,8 +6493,8 @@
       <x:c r="H329" s="34" t="s"/>
     </x:row>
     <x:row r="330" spans="1:10" outlineLevel="3">
-      <x:c r="B330" s="40" t="s"/>
-      <x:c r="C330" s="41" t="s"/>
+      <x:c r="B330" s="35" t="s"/>
+      <x:c r="C330" s="36" t="s"/>
       <x:c r="D330" s="37" t="n">
         <x:v>1144</x:v>
       </x:c>
@@ -6588,8 +6512,8 @@
       </x:c>
     </x:row>
     <x:row r="331" spans="1:10" outlineLevel="3">
-      <x:c r="B331" s="40" t="s"/>
-      <x:c r="C331" s="42" t="s"/>
+      <x:c r="B331" s="35" t="s"/>
+      <x:c r="C331" s="36" t="s"/>
       <x:c r="D331" s="37" t="n">
         <x:v>1044</x:v>
       </x:c>
@@ -6607,7 +6531,7 @@
       </x:c>
     </x:row>
     <x:row r="332" spans="1:10" outlineLevel="2">
-      <x:c r="B332" s="43" t="s"/>
+      <x:c r="B332" s="35" t="s"/>
       <x:c r="C332" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -6652,7 +6576,7 @@
       <x:c r="H334" s="34" t="s"/>
     </x:row>
     <x:row r="335" spans="1:10" outlineLevel="2">
-      <x:c r="B335" s="39" t="s"/>
+      <x:c r="B335" s="35" t="s"/>
       <x:c r="C335" s="29" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -6663,8 +6587,8 @@
       <x:c r="H335" s="34" t="s"/>
     </x:row>
     <x:row r="336" spans="1:10" outlineLevel="3">
-      <x:c r="B336" s="40" t="s"/>
-      <x:c r="C336" s="41" t="s"/>
+      <x:c r="B336" s="35" t="s"/>
+      <x:c r="C336" s="36" t="s"/>
       <x:c r="D336" s="37" t="n">
         <x:v>1025</x:v>
       </x:c>
@@ -6682,8 +6606,8 @@
       </x:c>
     </x:row>
     <x:row r="337" spans="1:10" outlineLevel="3">
-      <x:c r="B337" s="40" t="s"/>
-      <x:c r="C337" s="42" t="s"/>
+      <x:c r="B337" s="35" t="s"/>
+      <x:c r="C337" s="36" t="s"/>
       <x:c r="D337" s="37" t="n">
         <x:v>1125</x:v>
       </x:c>
@@ -6701,7 +6625,7 @@
       </x:c>
     </x:row>
     <x:row r="338" spans="1:10" outlineLevel="2">
-      <x:c r="B338" s="40" t="s"/>
+      <x:c r="B338" s="35" t="s"/>
       <x:c r="C338" s="29" t="s">
         <x:v>29</x:v>
       </x:c>
@@ -6718,7 +6642,7 @@
       </x:c>
     </x:row>
     <x:row r="339" spans="1:10" outlineLevel="2">
-      <x:c r="B339" s="40" t="s"/>
+      <x:c r="B339" s="35" t="s"/>
       <x:c r="C339" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -6729,8 +6653,8 @@
       <x:c r="H339" s="34" t="s"/>
     </x:row>
     <x:row r="340" spans="1:10" outlineLevel="3">
-      <x:c r="B340" s="40" t="s"/>
-      <x:c r="C340" s="41" t="s"/>
+      <x:c r="B340" s="35" t="s"/>
+      <x:c r="C340" s="36" t="s"/>
       <x:c r="D340" s="37" t="n">
         <x:v>1008</x:v>
       </x:c>
@@ -6748,8 +6672,8 @@
       </x:c>
     </x:row>
     <x:row r="341" spans="1:10" outlineLevel="3">
-      <x:c r="B341" s="40" t="s"/>
-      <x:c r="C341" s="42" t="s"/>
+      <x:c r="B341" s="35" t="s"/>
+      <x:c r="C341" s="36" t="s"/>
       <x:c r="D341" s="37" t="n">
         <x:v>1139</x:v>
       </x:c>
@@ -6767,7 +6691,7 @@
       </x:c>
     </x:row>
     <x:row r="342" spans="1:10" outlineLevel="2">
-      <x:c r="B342" s="43" t="s"/>
+      <x:c r="B342" s="35" t="s"/>
       <x:c r="C342" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -6812,7 +6736,7 @@
       <x:c r="H344" s="34" t="s"/>
     </x:row>
     <x:row r="345" spans="1:10" outlineLevel="2">
-      <x:c r="B345" s="39" t="s"/>
+      <x:c r="B345" s="35" t="s"/>
       <x:c r="C345" s="29" t="s">
         <x:v>34</x:v>
       </x:c>
@@ -6823,7 +6747,7 @@
       <x:c r="H345" s="34" t="s"/>
     </x:row>
     <x:row r="346" spans="1:10" outlineLevel="3">
-      <x:c r="B346" s="40" t="s"/>
+      <x:c r="B346" s="35" t="s"/>
       <x:c r="C346" s="36" t="s"/>
       <x:c r="D346" s="37" t="n">
         <x:v>1183</x:v>
@@ -6842,7 +6766,7 @@
       </x:c>
     </x:row>
     <x:row r="347" spans="1:10" outlineLevel="2">
-      <x:c r="B347" s="40" t="s"/>
+      <x:c r="B347" s="35" t="s"/>
       <x:c r="C347" s="29" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -6859,7 +6783,7 @@
       </x:c>
     </x:row>
     <x:row r="348" spans="1:10" outlineLevel="2">
-      <x:c r="B348" s="40" t="s"/>
+      <x:c r="B348" s="35" t="s"/>
       <x:c r="C348" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -6870,7 +6794,7 @@
       <x:c r="H348" s="34" t="s"/>
     </x:row>
     <x:row r="349" spans="1:10" outlineLevel="3">
-      <x:c r="B349" s="40" t="s"/>
+      <x:c r="B349" s="35" t="s"/>
       <x:c r="C349" s="36" t="s"/>
       <x:c r="D349" s="37" t="n">
         <x:v>1112</x:v>
@@ -6889,7 +6813,7 @@
       </x:c>
     </x:row>
     <x:row r="350" spans="1:10" outlineLevel="2">
-      <x:c r="B350" s="40" t="s"/>
+      <x:c r="B350" s="35" t="s"/>
       <x:c r="C350" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -6906,7 +6830,7 @@
       </x:c>
     </x:row>
     <x:row r="351" spans="1:10" outlineLevel="2">
-      <x:c r="B351" s="40" t="s"/>
+      <x:c r="B351" s="35" t="s"/>
       <x:c r="C351" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -6917,7 +6841,7 @@
       <x:c r="H351" s="34" t="s"/>
     </x:row>
     <x:row r="352" spans="1:10" outlineLevel="3">
-      <x:c r="B352" s="40" t="s"/>
+      <x:c r="B352" s="35" t="s"/>
       <x:c r="C352" s="36" t="s"/>
       <x:c r="D352" s="37" t="n">
         <x:v>1068</x:v>
@@ -6936,7 +6860,7 @@
       </x:c>
     </x:row>
     <x:row r="353" spans="1:10" outlineLevel="2">
-      <x:c r="B353" s="43" t="s"/>
+      <x:c r="B353" s="35" t="s"/>
       <x:c r="C353" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -6981,7 +6905,7 @@
       <x:c r="H355" s="34" t="s"/>
     </x:row>
     <x:row r="356" spans="1:10" outlineLevel="2">
-      <x:c r="B356" s="39" t="s"/>
+      <x:c r="B356" s="35" t="s"/>
       <x:c r="C356" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -6992,8 +6916,8 @@
       <x:c r="H356" s="34" t="s"/>
     </x:row>
     <x:row r="357" spans="1:10" outlineLevel="3">
-      <x:c r="B357" s="40" t="s"/>
-      <x:c r="C357" s="41" t="s"/>
+      <x:c r="B357" s="35" t="s"/>
+      <x:c r="C357" s="36" t="s"/>
       <x:c r="D357" s="37" t="n">
         <x:v>1043</x:v>
       </x:c>
@@ -7011,8 +6935,8 @@
       </x:c>
     </x:row>
     <x:row r="358" spans="1:10" outlineLevel="3">
-      <x:c r="B358" s="40" t="s"/>
-      <x:c r="C358" s="42" t="s"/>
+      <x:c r="B358" s="35" t="s"/>
+      <x:c r="C358" s="36" t="s"/>
       <x:c r="D358" s="37" t="n">
         <x:v>1143</x:v>
       </x:c>
@@ -7030,7 +6954,7 @@
       </x:c>
     </x:row>
     <x:row r="359" spans="1:10" outlineLevel="2">
-      <x:c r="B359" s="43" t="s"/>
+      <x:c r="B359" s="35" t="s"/>
       <x:c r="C359" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -7075,7 +6999,7 @@
       <x:c r="H361" s="34" t="s"/>
     </x:row>
     <x:row r="362" spans="1:10" outlineLevel="2">
-      <x:c r="B362" s="39" t="s"/>
+      <x:c r="B362" s="35" t="s"/>
       <x:c r="C362" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -7086,7 +7010,7 @@
       <x:c r="H362" s="34" t="s"/>
     </x:row>
     <x:row r="363" spans="1:10" outlineLevel="3">
-      <x:c r="B363" s="40" t="s"/>
+      <x:c r="B363" s="35" t="s"/>
       <x:c r="C363" s="36" t="s"/>
       <x:c r="D363" s="37" t="n">
         <x:v>1201</x:v>
@@ -7105,7 +7029,7 @@
       </x:c>
     </x:row>
     <x:row r="364" spans="1:10" outlineLevel="2">
-      <x:c r="B364" s="43" t="s"/>
+      <x:c r="B364" s="35" t="s"/>
       <x:c r="C364" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -7150,7 +7074,7 @@
       <x:c r="H366" s="34" t="s"/>
     </x:row>
     <x:row r="367" spans="1:10" outlineLevel="2">
-      <x:c r="B367" s="39" t="s"/>
+      <x:c r="B367" s="35" t="s"/>
       <x:c r="C367" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -7161,7 +7085,7 @@
       <x:c r="H367" s="34" t="s"/>
     </x:row>
     <x:row r="368" spans="1:10" outlineLevel="3">
-      <x:c r="B368" s="40" t="s"/>
+      <x:c r="B368" s="35" t="s"/>
       <x:c r="C368" s="36" t="s"/>
       <x:c r="D368" s="37" t="n">
         <x:v>1199</x:v>
@@ -7180,7 +7104,7 @@
       </x:c>
     </x:row>
     <x:row r="369" spans="1:10" outlineLevel="2">
-      <x:c r="B369" s="40" t="s"/>
+      <x:c r="B369" s="35" t="s"/>
       <x:c r="C369" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -7197,7 +7121,7 @@
       </x:c>
     </x:row>
     <x:row r="370" spans="1:10" outlineLevel="2">
-      <x:c r="B370" s="40" t="s"/>
+      <x:c r="B370" s="35" t="s"/>
       <x:c r="C370" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -7208,7 +7132,7 @@
       <x:c r="H370" s="34" t="s"/>
     </x:row>
     <x:row r="371" spans="1:10" outlineLevel="3">
-      <x:c r="B371" s="40" t="s"/>
+      <x:c r="B371" s="35" t="s"/>
       <x:c r="C371" s="36" t="s"/>
       <x:c r="D371" s="37" t="n">
         <x:v>1094</x:v>
@@ -7227,7 +7151,7 @@
       </x:c>
     </x:row>
     <x:row r="372" spans="1:10" outlineLevel="2">
-      <x:c r="B372" s="43" t="s"/>
+      <x:c r="B372" s="35" t="s"/>
       <x:c r="C372" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -7272,7 +7196,7 @@
       <x:c r="H374" s="34" t="s"/>
     </x:row>
     <x:row r="375" spans="1:10" outlineLevel="2">
-      <x:c r="B375" s="39" t="s"/>
+      <x:c r="B375" s="35" t="s"/>
       <x:c r="C375" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -7283,7 +7207,7 @@
       <x:c r="H375" s="34" t="s"/>
     </x:row>
     <x:row r="376" spans="1:10" outlineLevel="3">
-      <x:c r="B376" s="40" t="s"/>
+      <x:c r="B376" s="35" t="s"/>
       <x:c r="C376" s="36" t="s"/>
       <x:c r="D376" s="37" t="n">
         <x:v>1175</x:v>
@@ -7302,7 +7226,7 @@
       </x:c>
     </x:row>
     <x:row r="377" spans="1:10" outlineLevel="2">
-      <x:c r="B377" s="43" t="s"/>
+      <x:c r="B377" s="35" t="s"/>
       <x:c r="C377" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -7347,7 +7271,7 @@
       <x:c r="H379" s="34" t="s"/>
     </x:row>
     <x:row r="380" spans="1:10" outlineLevel="2">
-      <x:c r="B380" s="39" t="s"/>
+      <x:c r="B380" s="35" t="s"/>
       <x:c r="C380" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -7358,8 +7282,8 @@
       <x:c r="H380" s="34" t="s"/>
     </x:row>
     <x:row r="381" spans="1:10" outlineLevel="3">
-      <x:c r="B381" s="40" t="s"/>
-      <x:c r="C381" s="41" t="s"/>
+      <x:c r="B381" s="35" t="s"/>
+      <x:c r="C381" s="36" t="s"/>
       <x:c r="D381" s="37" t="n">
         <x:v>1132</x:v>
       </x:c>
@@ -7377,8 +7301,8 @@
       </x:c>
     </x:row>
     <x:row r="382" spans="1:10" outlineLevel="3">
-      <x:c r="B382" s="40" t="s"/>
-      <x:c r="C382" s="44" t="s"/>
+      <x:c r="B382" s="35" t="s"/>
+      <x:c r="C382" s="36" t="s"/>
       <x:c r="D382" s="37" t="n">
         <x:v>1221</x:v>
       </x:c>
@@ -7396,8 +7320,8 @@
       </x:c>
     </x:row>
     <x:row r="383" spans="1:10" outlineLevel="3">
-      <x:c r="B383" s="40" t="s"/>
-      <x:c r="C383" s="44" t="s"/>
+      <x:c r="B383" s="35" t="s"/>
+      <x:c r="C383" s="36" t="s"/>
       <x:c r="D383" s="37" t="n">
         <x:v>1136</x:v>
       </x:c>
@@ -7415,8 +7339,8 @@
       </x:c>
     </x:row>
     <x:row r="384" spans="1:10" outlineLevel="3">
-      <x:c r="B384" s="40" t="s"/>
-      <x:c r="C384" s="44" t="s"/>
+      <x:c r="B384" s="35" t="s"/>
+      <x:c r="C384" s="36" t="s"/>
       <x:c r="D384" s="37" t="n">
         <x:v>1021</x:v>
       </x:c>
@@ -7434,8 +7358,8 @@
       </x:c>
     </x:row>
     <x:row r="385" spans="1:10" outlineLevel="3">
-      <x:c r="B385" s="40" t="s"/>
-      <x:c r="C385" s="44" t="s"/>
+      <x:c r="B385" s="35" t="s"/>
+      <x:c r="C385" s="36" t="s"/>
       <x:c r="D385" s="37" t="n">
         <x:v>1032</x:v>
       </x:c>
@@ -7453,8 +7377,8 @@
       </x:c>
     </x:row>
     <x:row r="386" spans="1:10" outlineLevel="3">
-      <x:c r="B386" s="40" t="s"/>
-      <x:c r="C386" s="44" t="s"/>
+      <x:c r="B386" s="35" t="s"/>
+      <x:c r="C386" s="36" t="s"/>
       <x:c r="D386" s="37" t="n">
         <x:v>1122</x:v>
       </x:c>
@@ -7472,8 +7396,8 @@
       </x:c>
     </x:row>
     <x:row r="387" spans="1:10" outlineLevel="3">
-      <x:c r="B387" s="40" t="s"/>
-      <x:c r="C387" s="44" t="s"/>
+      <x:c r="B387" s="35" t="s"/>
+      <x:c r="C387" s="36" t="s"/>
       <x:c r="D387" s="37" t="n">
         <x:v>1121</x:v>
       </x:c>
@@ -7491,8 +7415,8 @@
       </x:c>
     </x:row>
     <x:row r="388" spans="1:10" outlineLevel="3">
-      <x:c r="B388" s="40" t="s"/>
-      <x:c r="C388" s="42" t="s"/>
+      <x:c r="B388" s="35" t="s"/>
+      <x:c r="C388" s="36" t="s"/>
       <x:c r="D388" s="37" t="n">
         <x:v>1022</x:v>
       </x:c>
@@ -7510,7 +7434,7 @@
       </x:c>
     </x:row>
     <x:row r="389" spans="1:10" outlineLevel="2">
-      <x:c r="B389" s="43" t="s"/>
+      <x:c r="B389" s="35" t="s"/>
       <x:c r="C389" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -7555,7 +7479,7 @@
       <x:c r="H391" s="34" t="s"/>
     </x:row>
     <x:row r="392" spans="1:10" outlineLevel="2">
-      <x:c r="B392" s="39" t="s"/>
+      <x:c r="B392" s="35" t="s"/>
       <x:c r="C392" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -7566,8 +7490,8 @@
       <x:c r="H392" s="34" t="s"/>
     </x:row>
     <x:row r="393" spans="1:10" outlineLevel="3">
-      <x:c r="B393" s="40" t="s"/>
-      <x:c r="C393" s="41" t="s"/>
+      <x:c r="B393" s="35" t="s"/>
+      <x:c r="C393" s="36" t="s"/>
       <x:c r="D393" s="37" t="n">
         <x:v>1101</x:v>
       </x:c>
@@ -7585,8 +7509,8 @@
       </x:c>
     </x:row>
     <x:row r="394" spans="1:10" outlineLevel="3">
-      <x:c r="B394" s="40" t="s"/>
-      <x:c r="C394" s="42" t="s"/>
+      <x:c r="B394" s="35" t="s"/>
+      <x:c r="C394" s="36" t="s"/>
       <x:c r="D394" s="37" t="n">
         <x:v>1051</x:v>
       </x:c>
@@ -7604,7 +7528,7 @@
       </x:c>
     </x:row>
     <x:row r="395" spans="1:10" outlineLevel="2">
-      <x:c r="B395" s="43" t="s"/>
+      <x:c r="B395" s="35" t="s"/>
       <x:c r="C395" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -7649,7 +7573,7 @@
       <x:c r="H397" s="34" t="s"/>
     </x:row>
     <x:row r="398" spans="1:10" outlineLevel="2">
-      <x:c r="B398" s="39" t="s"/>
+      <x:c r="B398" s="35" t="s"/>
       <x:c r="C398" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -7660,8 +7584,8 @@
       <x:c r="H398" s="34" t="s"/>
     </x:row>
     <x:row r="399" spans="1:10" outlineLevel="3">
-      <x:c r="B399" s="40" t="s"/>
-      <x:c r="C399" s="41" t="s"/>
+      <x:c r="B399" s="35" t="s"/>
+      <x:c r="C399" s="36" t="s"/>
       <x:c r="D399" s="37" t="n">
         <x:v>1052</x:v>
       </x:c>
@@ -7679,8 +7603,8 @@
       </x:c>
     </x:row>
     <x:row r="400" spans="1:10" outlineLevel="3">
-      <x:c r="B400" s="40" t="s"/>
-      <x:c r="C400" s="44" t="s"/>
+      <x:c r="B400" s="35" t="s"/>
+      <x:c r="C400" s="36" t="s"/>
       <x:c r="D400" s="37" t="n">
         <x:v>1155</x:v>
       </x:c>
@@ -7698,8 +7622,8 @@
       </x:c>
     </x:row>
     <x:row r="401" spans="1:10" outlineLevel="3">
-      <x:c r="B401" s="40" t="s"/>
-      <x:c r="C401" s="44" t="s"/>
+      <x:c r="B401" s="35" t="s"/>
+      <x:c r="C401" s="36" t="s"/>
       <x:c r="D401" s="37" t="n">
         <x:v>1152</x:v>
       </x:c>
@@ -7717,8 +7641,8 @@
       </x:c>
     </x:row>
     <x:row r="402" spans="1:10" outlineLevel="3">
-      <x:c r="B402" s="40" t="s"/>
-      <x:c r="C402" s="44" t="s"/>
+      <x:c r="B402" s="35" t="s"/>
+      <x:c r="C402" s="36" t="s"/>
       <x:c r="D402" s="37" t="n">
         <x:v>1163</x:v>
       </x:c>
@@ -7736,8 +7660,8 @@
       </x:c>
     </x:row>
     <x:row r="403" spans="1:10" outlineLevel="3">
-      <x:c r="B403" s="40" t="s"/>
-      <x:c r="C403" s="44" t="s"/>
+      <x:c r="B403" s="35" t="s"/>
+      <x:c r="C403" s="36" t="s"/>
       <x:c r="D403" s="37" t="n">
         <x:v>1087</x:v>
       </x:c>
@@ -7755,8 +7679,8 @@
       </x:c>
     </x:row>
     <x:row r="404" spans="1:10" outlineLevel="3">
-      <x:c r="B404" s="40" t="s"/>
-      <x:c r="C404" s="44" t="s"/>
+      <x:c r="B404" s="35" t="s"/>
+      <x:c r="C404" s="36" t="s"/>
       <x:c r="D404" s="37" t="n">
         <x:v>1055</x:v>
       </x:c>
@@ -7774,8 +7698,8 @@
       </x:c>
     </x:row>
     <x:row r="405" spans="1:10" outlineLevel="3">
-      <x:c r="B405" s="40" t="s"/>
-      <x:c r="C405" s="44" t="s"/>
+      <x:c r="B405" s="35" t="s"/>
+      <x:c r="C405" s="36" t="s"/>
       <x:c r="D405" s="37" t="n">
         <x:v>1003</x:v>
       </x:c>
@@ -7793,8 +7717,8 @@
       </x:c>
     </x:row>
     <x:row r="406" spans="1:10" outlineLevel="3">
-      <x:c r="B406" s="40" t="s"/>
-      <x:c r="C406" s="42" t="s"/>
+      <x:c r="B406" s="35" t="s"/>
+      <x:c r="C406" s="36" t="s"/>
       <x:c r="D406" s="37" t="n">
         <x:v>1255</x:v>
       </x:c>
@@ -7812,7 +7736,7 @@
       </x:c>
     </x:row>
     <x:row r="407" spans="1:10" outlineLevel="2">
-      <x:c r="B407" s="40" t="s"/>
+      <x:c r="B407" s="35" t="s"/>
       <x:c r="C407" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -7829,7 +7753,7 @@
       </x:c>
     </x:row>
     <x:row r="408" spans="1:10" outlineLevel="2">
-      <x:c r="B408" s="40" t="s"/>
+      <x:c r="B408" s="35" t="s"/>
       <x:c r="C408" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -7840,8 +7764,8 @@
       <x:c r="H408" s="34" t="s"/>
     </x:row>
     <x:row r="409" spans="1:10" outlineLevel="3">
-      <x:c r="B409" s="40" t="s"/>
-      <x:c r="C409" s="41" t="s"/>
+      <x:c r="B409" s="35" t="s"/>
+      <x:c r="C409" s="36" t="s"/>
       <x:c r="D409" s="37" t="n">
         <x:v>1275</x:v>
       </x:c>
@@ -7859,8 +7783,8 @@
       </x:c>
     </x:row>
     <x:row r="410" spans="1:10" outlineLevel="3">
-      <x:c r="B410" s="40" t="s"/>
-      <x:c r="C410" s="42" t="s"/>
+      <x:c r="B410" s="35" t="s"/>
+      <x:c r="C410" s="36" t="s"/>
       <x:c r="D410" s="37" t="n">
         <x:v>1075</x:v>
       </x:c>
@@ -7878,7 +7802,7 @@
       </x:c>
     </x:row>
     <x:row r="411" spans="1:10" outlineLevel="2">
-      <x:c r="B411" s="40" t="s"/>
+      <x:c r="B411" s="35" t="s"/>
       <x:c r="C411" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -7895,7 +7819,7 @@
       </x:c>
     </x:row>
     <x:row r="412" spans="1:10" outlineLevel="2">
-      <x:c r="B412" s="40" t="s"/>
+      <x:c r="B412" s="35" t="s"/>
       <x:c r="C412" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -7906,7 +7830,7 @@
       <x:c r="H412" s="34" t="s"/>
     </x:row>
     <x:row r="413" spans="1:10" outlineLevel="3">
-      <x:c r="B413" s="40" t="s"/>
+      <x:c r="B413" s="35" t="s"/>
       <x:c r="C413" s="36" t="s"/>
       <x:c r="D413" s="37" t="n">
         <x:v>1067</x:v>
@@ -7925,7 +7849,7 @@
       </x:c>
     </x:row>
     <x:row r="414" spans="1:10" outlineLevel="2">
-      <x:c r="B414" s="43" t="s"/>
+      <x:c r="B414" s="35" t="s"/>
       <x:c r="C414" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -7970,7 +7894,7 @@
       <x:c r="H416" s="34" t="s"/>
     </x:row>
     <x:row r="417" spans="1:10" outlineLevel="2">
-      <x:c r="B417" s="39" t="s"/>
+      <x:c r="B417" s="35" t="s"/>
       <x:c r="C417" s="29" t="s">
         <x:v>34</x:v>
       </x:c>
@@ -7981,8 +7905,8 @@
       <x:c r="H417" s="34" t="s"/>
     </x:row>
     <x:row r="418" spans="1:10" outlineLevel="3">
-      <x:c r="B418" s="40" t="s"/>
-      <x:c r="C418" s="41" t="s"/>
+      <x:c r="B418" s="35" t="s"/>
+      <x:c r="C418" s="36" t="s"/>
       <x:c r="D418" s="37" t="n">
         <x:v>1171</x:v>
       </x:c>
@@ -8000,8 +7924,8 @@
       </x:c>
     </x:row>
     <x:row r="419" spans="1:10" outlineLevel="3">
-      <x:c r="B419" s="40" t="s"/>
-      <x:c r="C419" s="44" t="s"/>
+      <x:c r="B419" s="35" t="s"/>
+      <x:c r="C419" s="36" t="s"/>
       <x:c r="D419" s="37" t="n">
         <x:v>1271</x:v>
       </x:c>
@@ -8019,8 +7943,8 @@
       </x:c>
     </x:row>
     <x:row r="420" spans="1:10" outlineLevel="3">
-      <x:c r="B420" s="40" t="s"/>
-      <x:c r="C420" s="42" t="s"/>
+      <x:c r="B420" s="35" t="s"/>
+      <x:c r="C420" s="36" t="s"/>
       <x:c r="D420" s="37" t="n">
         <x:v>1071</x:v>
       </x:c>
@@ -8038,7 +7962,7 @@
       </x:c>
     </x:row>
     <x:row r="421" spans="1:10" outlineLevel="2">
-      <x:c r="B421" s="40" t="s"/>
+      <x:c r="B421" s="35" t="s"/>
       <x:c r="C421" s="29" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -8055,7 +7979,7 @@
       </x:c>
     </x:row>
     <x:row r="422" spans="1:10" outlineLevel="2">
-      <x:c r="B422" s="40" t="s"/>
+      <x:c r="B422" s="35" t="s"/>
       <x:c r="C422" s="29" t="s">
         <x:v>56</x:v>
       </x:c>
@@ -8066,8 +7990,8 @@
       <x:c r="H422" s="34" t="s"/>
     </x:row>
     <x:row r="423" spans="1:10" outlineLevel="3">
-      <x:c r="B423" s="40" t="s"/>
-      <x:c r="C423" s="41" t="s"/>
+      <x:c r="B423" s="35" t="s"/>
+      <x:c r="C423" s="36" t="s"/>
       <x:c r="D423" s="37" t="n">
         <x:v>1011</x:v>
       </x:c>
@@ -8085,8 +8009,8 @@
       </x:c>
     </x:row>
     <x:row r="424" spans="1:10" outlineLevel="3">
-      <x:c r="B424" s="40" t="s"/>
-      <x:c r="C424" s="42" t="s"/>
+      <x:c r="B424" s="35" t="s"/>
+      <x:c r="C424" s="36" t="s"/>
       <x:c r="D424" s="37" t="n">
         <x:v>1111</x:v>
       </x:c>
@@ -8104,7 +8028,7 @@
       </x:c>
     </x:row>
     <x:row r="425" spans="1:10" outlineLevel="2">
-      <x:c r="B425" s="40" t="s"/>
+      <x:c r="B425" s="35" t="s"/>
       <x:c r="C425" s="29" t="s">
         <x:v>57</x:v>
       </x:c>
@@ -8121,7 +8045,7 @@
       </x:c>
     </x:row>
     <x:row r="426" spans="1:10" outlineLevel="2">
-      <x:c r="B426" s="40" t="s"/>
+      <x:c r="B426" s="35" t="s"/>
       <x:c r="C426" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -8132,7 +8056,7 @@
       <x:c r="H426" s="34" t="s"/>
     </x:row>
     <x:row r="427" spans="1:10" outlineLevel="3">
-      <x:c r="B427" s="40" t="s"/>
+      <x:c r="B427" s="35" t="s"/>
       <x:c r="C427" s="36" t="s"/>
       <x:c r="D427" s="37" t="n">
         <x:v>1035</x:v>
@@ -8151,7 +8075,7 @@
       </x:c>
     </x:row>
     <x:row r="428" spans="1:10" outlineLevel="2">
-      <x:c r="B428" s="40" t="s"/>
+      <x:c r="B428" s="35" t="s"/>
       <x:c r="C428" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -8168,7 +8092,7 @@
       </x:c>
     </x:row>
     <x:row r="429" spans="1:10" outlineLevel="2">
-      <x:c r="B429" s="40" t="s"/>
+      <x:c r="B429" s="35" t="s"/>
       <x:c r="C429" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -8179,7 +8103,7 @@
       <x:c r="H429" s="34" t="s"/>
     </x:row>
     <x:row r="430" spans="1:10" outlineLevel="3">
-      <x:c r="B430" s="40" t="s"/>
+      <x:c r="B430" s="35" t="s"/>
       <x:c r="C430" s="36" t="s"/>
       <x:c r="D430" s="37" t="n">
         <x:v>1154</x:v>
@@ -8198,7 +8122,7 @@
       </x:c>
     </x:row>
     <x:row r="431" spans="1:10" outlineLevel="2">
-      <x:c r="B431" s="43" t="s"/>
+      <x:c r="B431" s="35" t="s"/>
       <x:c r="C431" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -8243,7 +8167,7 @@
       <x:c r="H433" s="34" t="s"/>
     </x:row>
     <x:row r="434" spans="1:10" outlineLevel="2">
-      <x:c r="B434" s="39" t="s"/>
+      <x:c r="B434" s="35" t="s"/>
       <x:c r="C434" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -8254,7 +8178,7 @@
       <x:c r="H434" s="34" t="s"/>
     </x:row>
     <x:row r="435" spans="1:10" outlineLevel="3">
-      <x:c r="B435" s="40" t="s"/>
+      <x:c r="B435" s="35" t="s"/>
       <x:c r="C435" s="36" t="s"/>
       <x:c r="D435" s="37" t="n">
         <x:v>1053</x:v>
@@ -8273,7 +8197,7 @@
       </x:c>
     </x:row>
     <x:row r="436" spans="1:10" outlineLevel="2">
-      <x:c r="B436" s="43" t="s"/>
+      <x:c r="B436" s="35" t="s"/>
       <x:c r="C436" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -8318,7 +8242,7 @@
       <x:c r="H438" s="34" t="s"/>
     </x:row>
     <x:row r="439" spans="1:10" outlineLevel="2">
-      <x:c r="B439" s="39" t="s"/>
+      <x:c r="B439" s="35" t="s"/>
       <x:c r="C439" s="29" t="s">
         <x:v>34</x:v>
       </x:c>
@@ -8329,8 +8253,8 @@
       <x:c r="H439" s="34" t="s"/>
     </x:row>
     <x:row r="440" spans="1:10" outlineLevel="3">
-      <x:c r="B440" s="40" t="s"/>
-      <x:c r="C440" s="41" t="s"/>
+      <x:c r="B440" s="35" t="s"/>
+      <x:c r="C440" s="36" t="s"/>
       <x:c r="D440" s="37" t="n">
         <x:v>1059</x:v>
       </x:c>
@@ -8348,8 +8272,8 @@
       </x:c>
     </x:row>
     <x:row r="441" spans="1:10" outlineLevel="3">
-      <x:c r="B441" s="40" t="s"/>
-      <x:c r="C441" s="42" t="s"/>
+      <x:c r="B441" s="35" t="s"/>
+      <x:c r="C441" s="36" t="s"/>
       <x:c r="D441" s="37" t="n">
         <x:v>1072</x:v>
       </x:c>
@@ -8367,7 +8291,7 @@
       </x:c>
     </x:row>
     <x:row r="442" spans="1:10" outlineLevel="2">
-      <x:c r="B442" s="40" t="s"/>
+      <x:c r="B442" s="35" t="s"/>
       <x:c r="C442" s="29" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -8384,7 +8308,7 @@
       </x:c>
     </x:row>
     <x:row r="443" spans="1:10" outlineLevel="2">
-      <x:c r="B443" s="40" t="s"/>
+      <x:c r="B443" s="35" t="s"/>
       <x:c r="C443" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -8395,8 +8319,8 @@
       <x:c r="H443" s="34" t="s"/>
     </x:row>
     <x:row r="444" spans="1:10" outlineLevel="3">
-      <x:c r="B444" s="40" t="s"/>
-      <x:c r="C444" s="41" t="s"/>
+      <x:c r="B444" s="35" t="s"/>
+      <x:c r="C444" s="36" t="s"/>
       <x:c r="D444" s="37" t="n">
         <x:v>1280</x:v>
       </x:c>
@@ -8414,8 +8338,8 @@
       </x:c>
     </x:row>
     <x:row r="445" spans="1:10" outlineLevel="3">
-      <x:c r="B445" s="40" t="s"/>
-      <x:c r="C445" s="44" t="s"/>
+      <x:c r="B445" s="35" t="s"/>
+      <x:c r="C445" s="36" t="s"/>
       <x:c r="D445" s="37" t="n">
         <x:v>1080</x:v>
       </x:c>
@@ -8433,8 +8357,8 @@
       </x:c>
     </x:row>
     <x:row r="446" spans="1:10" outlineLevel="3">
-      <x:c r="B446" s="40" t="s"/>
-      <x:c r="C446" s="42" t="s"/>
+      <x:c r="B446" s="35" t="s"/>
+      <x:c r="C446" s="36" t="s"/>
       <x:c r="D446" s="37" t="n">
         <x:v>1180</x:v>
       </x:c>
@@ -8452,7 +8376,7 @@
       </x:c>
     </x:row>
     <x:row r="447" spans="1:10" outlineLevel="2">
-      <x:c r="B447" s="40" t="s"/>
+      <x:c r="B447" s="35" t="s"/>
       <x:c r="C447" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -8469,7 +8393,7 @@
       </x:c>
     </x:row>
     <x:row r="448" spans="1:10" outlineLevel="2">
-      <x:c r="B448" s="40" t="s"/>
+      <x:c r="B448" s="35" t="s"/>
       <x:c r="C448" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -8480,8 +8404,8 @@
       <x:c r="H448" s="34" t="s"/>
     </x:row>
     <x:row r="449" spans="1:10" outlineLevel="3">
-      <x:c r="B449" s="40" t="s"/>
-      <x:c r="C449" s="41" t="s"/>
+      <x:c r="B449" s="35" t="s"/>
+      <x:c r="C449" s="36" t="s"/>
       <x:c r="D449" s="37" t="n">
         <x:v>1105</x:v>
       </x:c>
@@ -8499,8 +8423,8 @@
       </x:c>
     </x:row>
     <x:row r="450" spans="1:10" outlineLevel="3">
-      <x:c r="B450" s="40" t="s"/>
-      <x:c r="C450" s="44" t="s"/>
+      <x:c r="B450" s="35" t="s"/>
+      <x:c r="C450" s="36" t="s"/>
       <x:c r="D450" s="37" t="n">
         <x:v>1005</x:v>
       </x:c>
@@ -8518,8 +8442,8 @@
       </x:c>
     </x:row>
     <x:row r="451" spans="1:10" outlineLevel="3">
-      <x:c r="B451" s="40" t="s"/>
-      <x:c r="C451" s="44" t="s"/>
+      <x:c r="B451" s="35" t="s"/>
+      <x:c r="C451" s="36" t="s"/>
       <x:c r="D451" s="37" t="n">
         <x:v>1305</x:v>
       </x:c>
@@ -8537,8 +8461,8 @@
       </x:c>
     </x:row>
     <x:row r="452" spans="1:10" outlineLevel="3">
-      <x:c r="B452" s="40" t="s"/>
-      <x:c r="C452" s="42" t="s"/>
+      <x:c r="B452" s="35" t="s"/>
+      <x:c r="C452" s="36" t="s"/>
       <x:c r="D452" s="37" t="n">
         <x:v>1266</x:v>
       </x:c>
@@ -8556,7 +8480,7 @@
       </x:c>
     </x:row>
     <x:row r="453" spans="1:10" outlineLevel="2">
-      <x:c r="B453" s="43" t="s"/>
+      <x:c r="B453" s="35" t="s"/>
       <x:c r="C453" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -8601,7 +8525,7 @@
       <x:c r="H455" s="34" t="s"/>
     </x:row>
     <x:row r="456" spans="1:10" outlineLevel="2">
-      <x:c r="B456" s="39" t="s"/>
+      <x:c r="B456" s="35" t="s"/>
       <x:c r="C456" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -8612,8 +8536,8 @@
       <x:c r="H456" s="34" t="s"/>
     </x:row>
     <x:row r="457" spans="1:10" outlineLevel="3">
-      <x:c r="B457" s="40" t="s"/>
-      <x:c r="C457" s="41" t="s"/>
+      <x:c r="B457" s="35" t="s"/>
+      <x:c r="C457" s="36" t="s"/>
       <x:c r="D457" s="37" t="n">
         <x:v>1119</x:v>
       </x:c>
@@ -8631,8 +8555,8 @@
       </x:c>
     </x:row>
     <x:row r="458" spans="1:10" outlineLevel="3">
-      <x:c r="B458" s="40" t="s"/>
-      <x:c r="C458" s="42" t="s"/>
+      <x:c r="B458" s="35" t="s"/>
+      <x:c r="C458" s="36" t="s"/>
       <x:c r="D458" s="37" t="n">
         <x:v>1036</x:v>
       </x:c>
@@ -8650,7 +8574,7 @@
       </x:c>
     </x:row>
     <x:row r="459" spans="1:10" outlineLevel="2">
-      <x:c r="B459" s="40" t="s"/>
+      <x:c r="B459" s="35" t="s"/>
       <x:c r="C459" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -8667,7 +8591,7 @@
       </x:c>
     </x:row>
     <x:row r="460" spans="1:10" outlineLevel="2">
-      <x:c r="B460" s="40" t="s"/>
+      <x:c r="B460" s="35" t="s"/>
       <x:c r="C460" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -8678,7 +8602,7 @@
       <x:c r="H460" s="34" t="s"/>
     </x:row>
     <x:row r="461" spans="1:10" outlineLevel="3">
-      <x:c r="B461" s="40" t="s"/>
+      <x:c r="B461" s="35" t="s"/>
       <x:c r="C461" s="36" t="s"/>
       <x:c r="D461" s="37" t="n">
         <x:v>1195</x:v>
@@ -8697,7 +8621,7 @@
       </x:c>
     </x:row>
     <x:row r="462" spans="1:10" outlineLevel="2">
-      <x:c r="B462" s="43" t="s"/>
+      <x:c r="B462" s="35" t="s"/>
       <x:c r="C462" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -8742,7 +8666,7 @@
       <x:c r="H464" s="34" t="s"/>
     </x:row>
     <x:row r="465" spans="1:10" outlineLevel="2">
-      <x:c r="B465" s="39" t="s"/>
+      <x:c r="B465" s="35" t="s"/>
       <x:c r="C465" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -8753,7 +8677,7 @@
       <x:c r="H465" s="34" t="s"/>
     </x:row>
     <x:row r="466" spans="1:10" outlineLevel="3">
-      <x:c r="B466" s="40" t="s"/>
+      <x:c r="B466" s="35" t="s"/>
       <x:c r="C466" s="36" t="s"/>
       <x:c r="D466" s="37" t="n">
         <x:v>1115</x:v>
@@ -8772,7 +8696,7 @@
       </x:c>
     </x:row>
     <x:row r="467" spans="1:10" outlineLevel="2">
-      <x:c r="B467" s="43" t="s"/>
+      <x:c r="B467" s="35" t="s"/>
       <x:c r="C467" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -8817,7 +8741,7 @@
       <x:c r="H469" s="34" t="s"/>
     </x:row>
     <x:row r="470" spans="1:10" outlineLevel="2">
-      <x:c r="B470" s="39" t="s"/>
+      <x:c r="B470" s="35" t="s"/>
       <x:c r="C470" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -8828,7 +8752,7 @@
       <x:c r="H470" s="34" t="s"/>
     </x:row>
     <x:row r="471" spans="1:10" outlineLevel="3">
-      <x:c r="B471" s="40" t="s"/>
+      <x:c r="B471" s="35" t="s"/>
       <x:c r="C471" s="36" t="s"/>
       <x:c r="D471" s="37" t="n">
         <x:v>1070</x:v>
@@ -8847,7 +8771,7 @@
       </x:c>
     </x:row>
     <x:row r="472" spans="1:10" outlineLevel="2">
-      <x:c r="B472" s="43" t="s"/>
+      <x:c r="B472" s="35" t="s"/>
       <x:c r="C472" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -8892,7 +8816,7 @@
       <x:c r="H474" s="34" t="s"/>
     </x:row>
     <x:row r="475" spans="1:10" outlineLevel="2">
-      <x:c r="B475" s="39" t="s"/>
+      <x:c r="B475" s="35" t="s"/>
       <x:c r="C475" s="29" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -8903,8 +8827,8 @@
       <x:c r="H475" s="34" t="s"/>
     </x:row>
     <x:row r="476" spans="1:10" outlineLevel="3">
-      <x:c r="B476" s="40" t="s"/>
-      <x:c r="C476" s="41" t="s"/>
+      <x:c r="B476" s="35" t="s"/>
+      <x:c r="C476" s="36" t="s"/>
       <x:c r="D476" s="37" t="n">
         <x:v>1250</x:v>
       </x:c>
@@ -8922,8 +8846,8 @@
       </x:c>
     </x:row>
     <x:row r="477" spans="1:10" outlineLevel="3">
-      <x:c r="B477" s="40" t="s"/>
-      <x:c r="C477" s="44" t="s"/>
+      <x:c r="B477" s="35" t="s"/>
+      <x:c r="C477" s="36" t="s"/>
       <x:c r="D477" s="37" t="n">
         <x:v>1350</x:v>
       </x:c>
@@ -8941,8 +8865,8 @@
       </x:c>
     </x:row>
     <x:row r="478" spans="1:10" outlineLevel="3">
-      <x:c r="B478" s="40" t="s"/>
-      <x:c r="C478" s="44" t="s"/>
+      <x:c r="B478" s="35" t="s"/>
+      <x:c r="C478" s="36" t="s"/>
       <x:c r="D478" s="37" t="n">
         <x:v>1050</x:v>
       </x:c>
@@ -8960,8 +8884,8 @@
       </x:c>
     </x:row>
     <x:row r="479" spans="1:10" outlineLevel="3">
-      <x:c r="B479" s="40" t="s"/>
-      <x:c r="C479" s="42" t="s"/>
+      <x:c r="B479" s="35" t="s"/>
+      <x:c r="C479" s="36" t="s"/>
       <x:c r="D479" s="37" t="n">
         <x:v>1150</x:v>
       </x:c>
@@ -8979,7 +8903,7 @@
       </x:c>
     </x:row>
     <x:row r="480" spans="1:10" outlineLevel="2">
-      <x:c r="B480" s="43" t="s"/>
+      <x:c r="B480" s="35" t="s"/>
       <x:c r="C480" s="29" t="s">
         <x:v>29</x:v>
       </x:c>
@@ -9024,7 +8948,7 @@
       <x:c r="H482" s="34" t="s"/>
     </x:row>
     <x:row r="483" spans="1:10" outlineLevel="2">
-      <x:c r="B483" s="39" t="s"/>
+      <x:c r="B483" s="35" t="s"/>
       <x:c r="C483" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -9035,8 +8959,8 @@
       <x:c r="H483" s="34" t="s"/>
     </x:row>
     <x:row r="484" spans="1:10" outlineLevel="3">
-      <x:c r="B484" s="40" t="s"/>
-      <x:c r="C484" s="41" t="s"/>
+      <x:c r="B484" s="35" t="s"/>
+      <x:c r="C484" s="36" t="s"/>
       <x:c r="D484" s="37" t="n">
         <x:v>1060</x:v>
       </x:c>
@@ -9054,8 +8978,8 @@
       </x:c>
     </x:row>
     <x:row r="485" spans="1:10" outlineLevel="3">
-      <x:c r="B485" s="40" t="s"/>
-      <x:c r="C485" s="42" t="s"/>
+      <x:c r="B485" s="35" t="s"/>
+      <x:c r="C485" s="36" t="s"/>
       <x:c r="D485" s="37" t="n">
         <x:v>1160</x:v>
       </x:c>
@@ -9073,7 +8997,7 @@
       </x:c>
     </x:row>
     <x:row r="486" spans="1:10" outlineLevel="2">
-      <x:c r="B486" s="40" t="s"/>
+      <x:c r="B486" s="35" t="s"/>
       <x:c r="C486" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -9090,7 +9014,7 @@
       </x:c>
     </x:row>
     <x:row r="487" spans="1:10" outlineLevel="2">
-      <x:c r="B487" s="40" t="s"/>
+      <x:c r="B487" s="35" t="s"/>
       <x:c r="C487" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -9101,8 +9025,8 @@
       <x:c r="H487" s="34" t="s"/>
     </x:row>
     <x:row r="488" spans="1:10" outlineLevel="3">
-      <x:c r="B488" s="40" t="s"/>
-      <x:c r="C488" s="41" t="s"/>
+      <x:c r="B488" s="35" t="s"/>
+      <x:c r="C488" s="36" t="s"/>
       <x:c r="D488" s="37" t="n">
         <x:v>1202</x:v>
       </x:c>
@@ -9120,8 +9044,8 @@
       </x:c>
     </x:row>
     <x:row r="489" spans="1:10" outlineLevel="3">
-      <x:c r="B489" s="40" t="s"/>
-      <x:c r="C489" s="44" t="s"/>
+      <x:c r="B489" s="35" t="s"/>
+      <x:c r="C489" s="36" t="s"/>
       <x:c r="D489" s="37" t="n">
         <x:v>1178</x:v>
       </x:c>
@@ -9139,8 +9063,8 @@
       </x:c>
     </x:row>
     <x:row r="490" spans="1:10" outlineLevel="3">
-      <x:c r="B490" s="40" t="s"/>
-      <x:c r="C490" s="44" t="s"/>
+      <x:c r="B490" s="35" t="s"/>
+      <x:c r="C490" s="36" t="s"/>
       <x:c r="D490" s="37" t="n">
         <x:v>1302</x:v>
       </x:c>
@@ -9158,8 +9082,8 @@
       </x:c>
     </x:row>
     <x:row r="491" spans="1:10" outlineLevel="3">
-      <x:c r="B491" s="40" t="s"/>
-      <x:c r="C491" s="44" t="s"/>
+      <x:c r="B491" s="35" t="s"/>
+      <x:c r="C491" s="36" t="s"/>
       <x:c r="D491" s="37" t="n">
         <x:v>1278</x:v>
       </x:c>
@@ -9177,8 +9101,8 @@
       </x:c>
     </x:row>
     <x:row r="492" spans="1:10" outlineLevel="3">
-      <x:c r="B492" s="40" t="s"/>
-      <x:c r="C492" s="42" t="s"/>
+      <x:c r="B492" s="35" t="s"/>
+      <x:c r="C492" s="36" t="s"/>
       <x:c r="D492" s="37" t="n">
         <x:v>1102</x:v>
       </x:c>
@@ -9196,7 +9120,7 @@
       </x:c>
     </x:row>
     <x:row r="493" spans="1:10" outlineLevel="2">
-      <x:c r="B493" s="40" t="s"/>
+      <x:c r="B493" s="35" t="s"/>
       <x:c r="C493" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -9213,7 +9137,7 @@
       </x:c>
     </x:row>
     <x:row r="494" spans="1:10" outlineLevel="2">
-      <x:c r="B494" s="40" t="s"/>
+      <x:c r="B494" s="35" t="s"/>
       <x:c r="C494" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -9224,8 +9148,8 @@
       <x:c r="H494" s="34" t="s"/>
     </x:row>
     <x:row r="495" spans="1:10" outlineLevel="3">
-      <x:c r="B495" s="40" t="s"/>
-      <x:c r="C495" s="41" t="s"/>
+      <x:c r="B495" s="35" t="s"/>
+      <x:c r="C495" s="36" t="s"/>
       <x:c r="D495" s="37" t="n">
         <x:v>1073</x:v>
       </x:c>
@@ -9243,8 +9167,8 @@
       </x:c>
     </x:row>
     <x:row r="496" spans="1:10" outlineLevel="3">
-      <x:c r="B496" s="40" t="s"/>
-      <x:c r="C496" s="42" t="s"/>
+      <x:c r="B496" s="35" t="s"/>
+      <x:c r="C496" s="36" t="s"/>
       <x:c r="D496" s="37" t="n">
         <x:v>1173</x:v>
       </x:c>
@@ -9262,7 +9186,7 @@
       </x:c>
     </x:row>
     <x:row r="497" spans="1:10" outlineLevel="2">
-      <x:c r="B497" s="43" t="s"/>
+      <x:c r="B497" s="35" t="s"/>
       <x:c r="C497" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -9307,7 +9231,7 @@
       <x:c r="H499" s="34" t="s"/>
     </x:row>
     <x:row r="500" spans="1:10" outlineLevel="2">
-      <x:c r="B500" s="39" t="s"/>
+      <x:c r="B500" s="35" t="s"/>
       <x:c r="C500" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -9318,7 +9242,7 @@
       <x:c r="H500" s="34" t="s"/>
     </x:row>
     <x:row r="501" spans="1:10" outlineLevel="3">
-      <x:c r="B501" s="40" t="s"/>
+      <x:c r="B501" s="35" t="s"/>
       <x:c r="C501" s="36" t="s"/>
       <x:c r="D501" s="37" t="n">
         <x:v>1296</x:v>
@@ -9337,7 +9261,7 @@
       </x:c>
     </x:row>
     <x:row r="502" spans="1:10" outlineLevel="2">
-      <x:c r="B502" s="43" t="s"/>
+      <x:c r="B502" s="35" t="s"/>
       <x:c r="C502" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -9382,7 +9306,7 @@
       <x:c r="H504" s="34" t="s"/>
     </x:row>
     <x:row r="505" spans="1:10" outlineLevel="2">
-      <x:c r="B505" s="39" t="s"/>
+      <x:c r="B505" s="35" t="s"/>
       <x:c r="C505" s="29" t="s">
         <x:v>34</x:v>
       </x:c>
@@ -9393,7 +9317,7 @@
       <x:c r="H505" s="34" t="s"/>
     </x:row>
     <x:row r="506" spans="1:10" outlineLevel="3">
-      <x:c r="B506" s="40" t="s"/>
+      <x:c r="B506" s="35" t="s"/>
       <x:c r="C506" s="36" t="s"/>
       <x:c r="D506" s="37" t="n">
         <x:v>1033</x:v>
@@ -9412,7 +9336,7 @@
       </x:c>
     </x:row>
     <x:row r="507" spans="1:10" outlineLevel="2">
-      <x:c r="B507" s="40" t="s"/>
+      <x:c r="B507" s="35" t="s"/>
       <x:c r="C507" s="29" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -9429,7 +9353,7 @@
       </x:c>
     </x:row>
     <x:row r="508" spans="1:10" outlineLevel="2">
-      <x:c r="B508" s="40" t="s"/>
+      <x:c r="B508" s="35" t="s"/>
       <x:c r="C508" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -9440,7 +9364,7 @@
       <x:c r="H508" s="34" t="s"/>
     </x:row>
     <x:row r="509" spans="1:10" outlineLevel="3">
-      <x:c r="B509" s="40" t="s"/>
+      <x:c r="B509" s="35" t="s"/>
       <x:c r="C509" s="36" t="s"/>
       <x:c r="D509" s="37" t="n">
         <x:v>1124</x:v>
@@ -9459,7 +9383,7 @@
       </x:c>
     </x:row>
     <x:row r="510" spans="1:10" outlineLevel="2">
-      <x:c r="B510" s="40" t="s"/>
+      <x:c r="B510" s="35" t="s"/>
       <x:c r="C510" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -9476,7 +9400,7 @@
       </x:c>
     </x:row>
     <x:row r="511" spans="1:10" outlineLevel="2">
-      <x:c r="B511" s="40" t="s"/>
+      <x:c r="B511" s="35" t="s"/>
       <x:c r="C511" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -9487,8 +9411,8 @@
       <x:c r="H511" s="34" t="s"/>
     </x:row>
     <x:row r="512" spans="1:10" outlineLevel="3">
-      <x:c r="B512" s="40" t="s"/>
-      <x:c r="C512" s="41" t="s"/>
+      <x:c r="B512" s="35" t="s"/>
+      <x:c r="C512" s="36" t="s"/>
       <x:c r="D512" s="37" t="n">
         <x:v>1200</x:v>
       </x:c>
@@ -9506,8 +9430,8 @@
       </x:c>
     </x:row>
     <x:row r="513" spans="1:10" outlineLevel="3">
-      <x:c r="B513" s="40" t="s"/>
-      <x:c r="C513" s="44" t="s"/>
+      <x:c r="B513" s="35" t="s"/>
+      <x:c r="C513" s="36" t="s"/>
       <x:c r="D513" s="37" t="n">
         <x:v>1300</x:v>
       </x:c>
@@ -9525,8 +9449,8 @@
       </x:c>
     </x:row>
     <x:row r="514" spans="1:10" outlineLevel="3">
-      <x:c r="B514" s="40" t="s"/>
-      <x:c r="C514" s="42" t="s"/>
+      <x:c r="B514" s="35" t="s"/>
+      <x:c r="C514" s="36" t="s"/>
       <x:c r="D514" s="37" t="n">
         <x:v>1100</x:v>
       </x:c>
@@ -9544,7 +9468,7 @@
       </x:c>
     </x:row>
     <x:row r="515" spans="1:10" outlineLevel="2">
-      <x:c r="B515" s="40" t="s"/>
+      <x:c r="B515" s="35" t="s"/>
       <x:c r="C515" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -9561,7 +9485,7 @@
       </x:c>
     </x:row>
     <x:row r="516" spans="1:10" outlineLevel="2">
-      <x:c r="B516" s="40" t="s"/>
+      <x:c r="B516" s="35" t="s"/>
       <x:c r="C516" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -9572,8 +9496,8 @@
       <x:c r="H516" s="34" t="s"/>
     </x:row>
     <x:row r="517" spans="1:10" outlineLevel="3">
-      <x:c r="B517" s="40" t="s"/>
-      <x:c r="C517" s="41" t="s"/>
+      <x:c r="B517" s="35" t="s"/>
+      <x:c r="C517" s="36" t="s"/>
       <x:c r="D517" s="37" t="n">
         <x:v>1127</x:v>
       </x:c>
@@ -9591,8 +9515,8 @@
       </x:c>
     </x:row>
     <x:row r="518" spans="1:10" outlineLevel="3">
-      <x:c r="B518" s="40" t="s"/>
-      <x:c r="C518" s="44" t="s"/>
+      <x:c r="B518" s="35" t="s"/>
+      <x:c r="C518" s="36" t="s"/>
       <x:c r="D518" s="37" t="n">
         <x:v>1207</x:v>
       </x:c>
@@ -9610,8 +9534,8 @@
       </x:c>
     </x:row>
     <x:row r="519" spans="1:10" outlineLevel="3">
-      <x:c r="B519" s="40" t="s"/>
-      <x:c r="C519" s="44" t="s"/>
+      <x:c r="B519" s="35" t="s"/>
+      <x:c r="C519" s="36" t="s"/>
       <x:c r="D519" s="37" t="n">
         <x:v>1027</x:v>
       </x:c>
@@ -9629,8 +9553,8 @@
       </x:c>
     </x:row>
     <x:row r="520" spans="1:10" outlineLevel="3">
-      <x:c r="B520" s="40" t="s"/>
-      <x:c r="C520" s="44" t="s"/>
+      <x:c r="B520" s="35" t="s"/>
+      <x:c r="C520" s="36" t="s"/>
       <x:c r="D520" s="37" t="n">
         <x:v>1107</x:v>
       </x:c>
@@ -9648,8 +9572,8 @@
       </x:c>
     </x:row>
     <x:row r="521" spans="1:10" outlineLevel="3">
-      <x:c r="B521" s="40" t="s"/>
-      <x:c r="C521" s="42" t="s"/>
+      <x:c r="B521" s="35" t="s"/>
+      <x:c r="C521" s="36" t="s"/>
       <x:c r="D521" s="37" t="n">
         <x:v>1007</x:v>
       </x:c>
@@ -9667,7 +9591,7 @@
       </x:c>
     </x:row>
     <x:row r="522" spans="1:10" outlineLevel="2">
-      <x:c r="B522" s="43" t="s"/>
+      <x:c r="B522" s="35" t="s"/>
       <x:c r="C522" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -9712,7 +9636,7 @@
       <x:c r="H524" s="34" t="s"/>
     </x:row>
     <x:row r="525" spans="1:10" outlineLevel="2">
-      <x:c r="B525" s="39" t="s"/>
+      <x:c r="B525" s="35" t="s"/>
       <x:c r="C525" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -9723,8 +9647,8 @@
       <x:c r="H525" s="34" t="s"/>
     </x:row>
     <x:row r="526" spans="1:10" outlineLevel="3">
-      <x:c r="B526" s="40" t="s"/>
-      <x:c r="C526" s="41" t="s"/>
+      <x:c r="B526" s="35" t="s"/>
+      <x:c r="C526" s="36" t="s"/>
       <x:c r="D526" s="37" t="n">
         <x:v>1140</x:v>
       </x:c>
@@ -9742,8 +9666,8 @@
       </x:c>
     </x:row>
     <x:row r="527" spans="1:10" outlineLevel="3">
-      <x:c r="B527" s="40" t="s"/>
-      <x:c r="C527" s="42" t="s"/>
+      <x:c r="B527" s="35" t="s"/>
+      <x:c r="C527" s="36" t="s"/>
       <x:c r="D527" s="37" t="n">
         <x:v>1040</x:v>
       </x:c>
@@ -9761,7 +9685,7 @@
       </x:c>
     </x:row>
     <x:row r="528" spans="1:10" outlineLevel="2">
-      <x:c r="B528" s="43" t="s"/>
+      <x:c r="B528" s="35" t="s"/>
       <x:c r="C528" s="29" t="s">
         <x:v>15</x:v>
       </x:c>

</xml_diff>

<commit_message>
Upgrade ClosedXML to 0.95.0 (#135)
* Upgrade to ClosedXML 0.95

* Update reference files: contents of merged cells (except the first one) cleared (see https://github.com/ClosedXML/ClosedXML/issues/1229)

* Update reference files: styles of merged cells slightly differ, though visually they are the same
</commit_message>
<xml_diff>
--- a/tests/Gauges/GroupTagTests_WithHeader.xlsx
+++ b/tests/Gauges/GroupTagTests_WithHeader.xlsx
@@ -532,7 +532,7 @@
       </x:patternFill>
     </x:fill>
   </x:fills>
-  <x:borders count="8">
+  <x:borders count="6">
     <x:border>
       <x:left/>
       <x:right/>
@@ -605,42 +605,8 @@
       </x:bottom>
       <x:diagonal/>
     </x:border>
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="thin">
-        <x:color indexed="64"/>
-      </x:left>
-      <x:right style="thin">
-        <x:color indexed="64"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
-    </x:border>
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="thin">
-        <x:color indexed="64"/>
-      </x:left>
-      <x:right style="thin">
-        <x:color indexed="64"/>
-      </x:right>
-      <x:top style="none">
-        <x:color indexed="64"/>
-      </x:top>
-      <x:bottom style="thin">
-        <x:color indexed="64"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
-    </x:border>
   </x:borders>
-  <x:cellStyleXfs count="22">
+  <x:cellStyleXfs count="16">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
@@ -687,26 +653,8 @@
     <x:xf numFmtId="4" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="6" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="45">
+  <x:cellXfs count="39">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <x:alignment vertical="center"/>
@@ -824,30 +772,6 @@
     </x:xf>
     <x:xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
@@ -1418,7 +1342,7 @@
       </x:c>
     </x:row>
     <x:row r="6" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
-      <x:c r="B6" s="39" t="s"/>
+      <x:c r="B6" s="35" t="s"/>
       <x:c r="C6" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -1432,7 +1356,7 @@
       </x:c>
     </x:row>
     <x:row r="7" spans="1:10" outlineLevel="3" x14ac:dyDescent="0.2">
-      <x:c r="B7" s="40" t="s"/>
+      <x:c r="B7" s="35" t="s"/>
       <x:c r="C7" s="36" t="s"/>
       <x:c r="D7" s="37" t="n">
         <x:v>1014</x:v>
@@ -1454,7 +1378,7 @@
       </x:c>
     </x:row>
     <x:row r="8" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
-      <x:c r="B8" s="40" t="s"/>
+      <x:c r="B8" s="35" t="s"/>
       <x:c r="C8" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -1474,7 +1398,7 @@
       </x:c>
     </x:row>
     <x:row r="9" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
-      <x:c r="B9" s="40" t="s"/>
+      <x:c r="B9" s="35" t="s"/>
       <x:c r="C9" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -1491,8 +1415,8 @@
       </x:c>
     </x:row>
     <x:row r="10" spans="1:10" outlineLevel="3">
-      <x:c r="B10" s="40" t="s"/>
-      <x:c r="C10" s="41" t="s"/>
+      <x:c r="B10" s="35" t="s"/>
+      <x:c r="C10" s="36" t="s"/>
       <x:c r="D10" s="37" t="n">
         <x:v>1129</x:v>
       </x:c>
@@ -1510,8 +1434,8 @@
       </x:c>
     </x:row>
     <x:row r="11" spans="1:10" outlineLevel="3">
-      <x:c r="B11" s="40" t="s"/>
-      <x:c r="C11" s="42" t="s"/>
+      <x:c r="B11" s="35" t="s"/>
+      <x:c r="C11" s="36" t="s"/>
       <x:c r="D11" s="37" t="n">
         <x:v>1029</x:v>
       </x:c>
@@ -1529,7 +1453,7 @@
       </x:c>
     </x:row>
     <x:row r="12" spans="1:10" outlineLevel="2">
-      <x:c r="B12" s="40" t="s"/>
+      <x:c r="B12" s="35" t="s"/>
       <x:c r="C12" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -1546,7 +1470,7 @@
       </x:c>
     </x:row>
     <x:row r="13" spans="1:10" outlineLevel="2">
-      <x:c r="B13" s="40" t="s"/>
+      <x:c r="B13" s="35" t="s"/>
       <x:c r="C13" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -1557,7 +1481,7 @@
       <x:c r="H13" s="34" t="s"/>
     </x:row>
     <x:row r="14" spans="1:10" outlineLevel="3">
-      <x:c r="B14" s="40" t="s"/>
+      <x:c r="B14" s="35" t="s"/>
       <x:c r="C14" s="36" t="s"/>
       <x:c r="D14" s="37" t="n">
         <x:v>1038</x:v>
@@ -1576,7 +1500,7 @@
       </x:c>
     </x:row>
     <x:row r="15" spans="1:10" outlineLevel="2">
-      <x:c r="B15" s="43" t="s"/>
+      <x:c r="B15" s="35" t="s"/>
       <x:c r="C15" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -1621,7 +1545,7 @@
       <x:c r="H17" s="34" t="s"/>
     </x:row>
     <x:row r="18" spans="1:10" outlineLevel="2">
-      <x:c r="B18" s="39" t="s"/>
+      <x:c r="B18" s="35" t="s"/>
       <x:c r="C18" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -1632,7 +1556,7 @@
       <x:c r="H18" s="34" t="s"/>
     </x:row>
     <x:row r="19" spans="1:10" outlineLevel="3">
-      <x:c r="B19" s="40" t="s"/>
+      <x:c r="B19" s="35" t="s"/>
       <x:c r="C19" s="36" t="s"/>
       <x:c r="D19" s="37" t="n">
         <x:v>1039</x:v>
@@ -1651,7 +1575,7 @@
       </x:c>
     </x:row>
     <x:row r="20" spans="1:10" outlineLevel="2">
-      <x:c r="B20" s="43" t="s"/>
+      <x:c r="B20" s="35" t="s"/>
       <x:c r="C20" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -1696,7 +1620,7 @@
       <x:c r="H22" s="34" t="s"/>
     </x:row>
     <x:row r="23" spans="1:10" outlineLevel="2">
-      <x:c r="B23" s="39" t="s"/>
+      <x:c r="B23" s="35" t="s"/>
       <x:c r="C23" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1707,8 +1631,8 @@
       <x:c r="H23" s="34" t="s"/>
     </x:row>
     <x:row r="24" spans="1:10" outlineLevel="3">
-      <x:c r="B24" s="40" t="s"/>
-      <x:c r="C24" s="41" t="s"/>
+      <x:c r="B24" s="35" t="s"/>
+      <x:c r="C24" s="36" t="s"/>
       <x:c r="D24" s="37" t="n">
         <x:v>1017</x:v>
       </x:c>
@@ -1726,8 +1650,8 @@
       </x:c>
     </x:row>
     <x:row r="25" spans="1:10" outlineLevel="3">
-      <x:c r="B25" s="40" t="s"/>
-      <x:c r="C25" s="44" t="s"/>
+      <x:c r="B25" s="35" t="s"/>
+      <x:c r="C25" s="36" t="s"/>
       <x:c r="D25" s="37" t="n">
         <x:v>1217</x:v>
       </x:c>
@@ -1745,8 +1669,8 @@
       </x:c>
     </x:row>
     <x:row r="26" spans="1:10" outlineLevel="3">
-      <x:c r="B26" s="40" t="s"/>
-      <x:c r="C26" s="44" t="s"/>
+      <x:c r="B26" s="35" t="s"/>
+      <x:c r="C26" s="36" t="s"/>
       <x:c r="D26" s="37" t="n">
         <x:v>1117</x:v>
       </x:c>
@@ -1764,8 +1688,8 @@
       </x:c>
     </x:row>
     <x:row r="27" spans="1:10" outlineLevel="3">
-      <x:c r="B27" s="40" t="s"/>
-      <x:c r="C27" s="42" t="s"/>
+      <x:c r="B27" s="35" t="s"/>
+      <x:c r="C27" s="36" t="s"/>
       <x:c r="D27" s="37" t="n">
         <x:v>1317</x:v>
       </x:c>
@@ -1783,7 +1707,7 @@
       </x:c>
     </x:row>
     <x:row r="28" spans="1:10" outlineLevel="2">
-      <x:c r="B28" s="40" t="s"/>
+      <x:c r="B28" s="35" t="s"/>
       <x:c r="C28" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -1800,7 +1724,7 @@
       </x:c>
     </x:row>
     <x:row r="29" spans="1:10" outlineLevel="2">
-      <x:c r="B29" s="40" t="s"/>
+      <x:c r="B29" s="35" t="s"/>
       <x:c r="C29" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -1811,8 +1735,8 @@
       <x:c r="H29" s="34" t="s"/>
     </x:row>
     <x:row r="30" spans="1:10" outlineLevel="3">
-      <x:c r="B30" s="40" t="s"/>
-      <x:c r="C30" s="41" t="s"/>
+      <x:c r="B30" s="35" t="s"/>
+      <x:c r="C30" s="36" t="s"/>
       <x:c r="D30" s="37" t="n">
         <x:v>1137</x:v>
       </x:c>
@@ -1830,8 +1754,8 @@
       </x:c>
     </x:row>
     <x:row r="31" spans="1:10" outlineLevel="3">
-      <x:c r="B31" s="40" t="s"/>
-      <x:c r="C31" s="44" t="s"/>
+      <x:c r="B31" s="35" t="s"/>
+      <x:c r="C31" s="36" t="s"/>
       <x:c r="D31" s="37" t="n">
         <x:v>1037</x:v>
       </x:c>
@@ -1849,8 +1773,8 @@
       </x:c>
     </x:row>
     <x:row r="32" spans="1:10" outlineLevel="3">
-      <x:c r="B32" s="40" t="s"/>
-      <x:c r="C32" s="42" t="s"/>
+      <x:c r="B32" s="35" t="s"/>
+      <x:c r="C32" s="36" t="s"/>
       <x:c r="D32" s="37" t="n">
         <x:v>1099</x:v>
       </x:c>
@@ -1868,7 +1792,7 @@
       </x:c>
     </x:row>
     <x:row r="33" spans="1:10" outlineLevel="2">
-      <x:c r="B33" s="40" t="s"/>
+      <x:c r="B33" s="35" t="s"/>
       <x:c r="C33" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -1885,7 +1809,7 @@
       </x:c>
     </x:row>
     <x:row r="34" spans="1:10" outlineLevel="2">
-      <x:c r="B34" s="40" t="s"/>
+      <x:c r="B34" s="35" t="s"/>
       <x:c r="C34" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -1896,8 +1820,8 @@
       <x:c r="H34" s="34" t="s"/>
     </x:row>
     <x:row r="35" spans="1:10" outlineLevel="3">
-      <x:c r="B35" s="40" t="s"/>
-      <x:c r="C35" s="41" t="s"/>
+      <x:c r="B35" s="35" t="s"/>
+      <x:c r="C35" s="36" t="s"/>
       <x:c r="D35" s="37" t="n">
         <x:v>1294</x:v>
       </x:c>
@@ -1915,8 +1839,8 @@
       </x:c>
     </x:row>
     <x:row r="36" spans="1:10" outlineLevel="3">
-      <x:c r="B36" s="40" t="s"/>
-      <x:c r="C36" s="42" t="s"/>
+      <x:c r="B36" s="35" t="s"/>
+      <x:c r="C36" s="36" t="s"/>
       <x:c r="D36" s="37" t="n">
         <x:v>1074</x:v>
       </x:c>
@@ -1934,7 +1858,7 @@
       </x:c>
     </x:row>
     <x:row r="37" spans="1:10" outlineLevel="2">
-      <x:c r="B37" s="43" t="s"/>
+      <x:c r="B37" s="35" t="s"/>
       <x:c r="C37" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -1979,7 +1903,7 @@
       <x:c r="H39" s="34" t="s"/>
     </x:row>
     <x:row r="40" spans="1:10" outlineLevel="2">
-      <x:c r="B40" s="39" t="s"/>
+      <x:c r="B40" s="35" t="s"/>
       <x:c r="C40" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1990,7 +1914,7 @@
       <x:c r="H40" s="34" t="s"/>
     </x:row>
     <x:row r="41" spans="1:10" outlineLevel="3">
-      <x:c r="B41" s="40" t="s"/>
+      <x:c r="B41" s="35" t="s"/>
       <x:c r="C41" s="36" t="s"/>
       <x:c r="D41" s="37" t="n">
         <x:v>1204</x:v>
@@ -2009,7 +1933,7 @@
       </x:c>
     </x:row>
     <x:row r="42" spans="1:10" outlineLevel="2">
-      <x:c r="B42" s="40" t="s"/>
+      <x:c r="B42" s="35" t="s"/>
       <x:c r="C42" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -2026,7 +1950,7 @@
       </x:c>
     </x:row>
     <x:row r="43" spans="1:10" outlineLevel="2">
-      <x:c r="B43" s="40" t="s"/>
+      <x:c r="B43" s="35" t="s"/>
       <x:c r="C43" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -2037,8 +1961,8 @@
       <x:c r="H43" s="34" t="s"/>
     </x:row>
     <x:row r="44" spans="1:10" outlineLevel="3">
-      <x:c r="B44" s="40" t="s"/>
-      <x:c r="C44" s="41" t="s"/>
+      <x:c r="B44" s="35" t="s"/>
+      <x:c r="C44" s="36" t="s"/>
       <x:c r="D44" s="37" t="n">
         <x:v>1355</x:v>
       </x:c>
@@ -2056,8 +1980,8 @@
       </x:c>
     </x:row>
     <x:row r="45" spans="1:10" outlineLevel="3">
-      <x:c r="B45" s="40" t="s"/>
-      <x:c r="C45" s="42" t="s"/>
+      <x:c r="B45" s="35" t="s"/>
+      <x:c r="C45" s="36" t="s"/>
       <x:c r="D45" s="37" t="n">
         <x:v>1263</x:v>
       </x:c>
@@ -2075,7 +1999,7 @@
       </x:c>
     </x:row>
     <x:row r="46" spans="1:10" outlineLevel="2">
-      <x:c r="B46" s="43" t="s"/>
+      <x:c r="B46" s="35" t="s"/>
       <x:c r="C46" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -2120,7 +2044,7 @@
       <x:c r="H48" s="34" t="s"/>
     </x:row>
     <x:row r="49" spans="1:10" outlineLevel="2">
-      <x:c r="B49" s="39" t="s"/>
+      <x:c r="B49" s="35" t="s"/>
       <x:c r="C49" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -2131,7 +2055,7 @@
       <x:c r="H49" s="34" t="s"/>
     </x:row>
     <x:row r="50" spans="1:10" outlineLevel="3">
-      <x:c r="B50" s="40" t="s"/>
+      <x:c r="B50" s="35" t="s"/>
       <x:c r="C50" s="36" t="s"/>
       <x:c r="D50" s="37" t="n">
         <x:v>1065</x:v>
@@ -2150,7 +2074,7 @@
       </x:c>
     </x:row>
     <x:row r="51" spans="1:10" outlineLevel="2">
-      <x:c r="B51" s="43" t="s"/>
+      <x:c r="B51" s="35" t="s"/>
       <x:c r="C51" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -2195,7 +2119,7 @@
       <x:c r="H53" s="34" t="s"/>
     </x:row>
     <x:row r="54" spans="1:10" outlineLevel="2">
-      <x:c r="B54" s="39" t="s"/>
+      <x:c r="B54" s="35" t="s"/>
       <x:c r="C54" s="29" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -2206,8 +2130,8 @@
       <x:c r="H54" s="34" t="s"/>
     </x:row>
     <x:row r="55" spans="1:10" outlineLevel="3">
-      <x:c r="B55" s="40" t="s"/>
-      <x:c r="C55" s="41" t="s"/>
+      <x:c r="B55" s="35" t="s"/>
+      <x:c r="C55" s="36" t="s"/>
       <x:c r="D55" s="37" t="n">
         <x:v>1042</x:v>
       </x:c>
@@ -2225,8 +2149,8 @@
       </x:c>
     </x:row>
     <x:row r="56" spans="1:10" outlineLevel="3">
-      <x:c r="B56" s="40" t="s"/>
-      <x:c r="C56" s="42" t="s"/>
+      <x:c r="B56" s="35" t="s"/>
+      <x:c r="C56" s="36" t="s"/>
       <x:c r="D56" s="37" t="n">
         <x:v>1142</x:v>
       </x:c>
@@ -2244,7 +2168,7 @@
       </x:c>
     </x:row>
     <x:row r="57" spans="1:10" outlineLevel="2">
-      <x:c r="B57" s="43" t="s"/>
+      <x:c r="B57" s="35" t="s"/>
       <x:c r="C57" s="29" t="s">
         <x:v>29</x:v>
       </x:c>
@@ -2289,7 +2213,7 @@
       <x:c r="H59" s="34" t="s"/>
     </x:row>
     <x:row r="60" spans="1:10" outlineLevel="2">
-      <x:c r="B60" s="39" t="s"/>
+      <x:c r="B60" s="35" t="s"/>
       <x:c r="C60" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -2300,8 +2224,8 @@
       <x:c r="H60" s="34" t="s"/>
     </x:row>
     <x:row r="61" spans="1:10" outlineLevel="3">
-      <x:c r="B61" s="40" t="s"/>
-      <x:c r="C61" s="41" t="s"/>
+      <x:c r="B61" s="35" t="s"/>
+      <x:c r="C61" s="36" t="s"/>
       <x:c r="D61" s="37" t="n">
         <x:v>1079</x:v>
       </x:c>
@@ -2319,8 +2243,8 @@
       </x:c>
     </x:row>
     <x:row r="62" spans="1:10" outlineLevel="3">
-      <x:c r="B62" s="40" t="s"/>
-      <x:c r="C62" s="44" t="s"/>
+      <x:c r="B62" s="35" t="s"/>
+      <x:c r="C62" s="36" t="s"/>
       <x:c r="D62" s="37" t="n">
         <x:v>1153</x:v>
       </x:c>
@@ -2338,8 +2262,8 @@
       </x:c>
     </x:row>
     <x:row r="63" spans="1:10" outlineLevel="3">
-      <x:c r="B63" s="40" t="s"/>
-      <x:c r="C63" s="42" t="s"/>
+      <x:c r="B63" s="35" t="s"/>
+      <x:c r="C63" s="36" t="s"/>
       <x:c r="D63" s="37" t="n">
         <x:v>1253</x:v>
       </x:c>
@@ -2357,7 +2281,7 @@
       </x:c>
     </x:row>
     <x:row r="64" spans="1:10" outlineLevel="2">
-      <x:c r="B64" s="40" t="s"/>
+      <x:c r="B64" s="35" t="s"/>
       <x:c r="C64" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -2374,7 +2298,7 @@
       </x:c>
     </x:row>
     <x:row r="65" spans="1:10" outlineLevel="2">
-      <x:c r="B65" s="40" t="s"/>
+      <x:c r="B65" s="35" t="s"/>
       <x:c r="C65" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -2385,8 +2309,8 @@
       <x:c r="H65" s="34" t="s"/>
     </x:row>
     <x:row r="66" spans="1:10" outlineLevel="3">
-      <x:c r="B66" s="40" t="s"/>
-      <x:c r="C66" s="41" t="s"/>
+      <x:c r="B66" s="35" t="s"/>
+      <x:c r="C66" s="36" t="s"/>
       <x:c r="D66" s="37" t="n">
         <x:v>1106</x:v>
       </x:c>
@@ -2404,8 +2328,8 @@
       </x:c>
     </x:row>
     <x:row r="67" spans="1:10" outlineLevel="3">
-      <x:c r="B67" s="40" t="s"/>
-      <x:c r="C67" s="42" t="s"/>
+      <x:c r="B67" s="35" t="s"/>
+      <x:c r="C67" s="36" t="s"/>
       <x:c r="D67" s="37" t="n">
         <x:v>1006</x:v>
       </x:c>
@@ -2423,7 +2347,7 @@
       </x:c>
     </x:row>
     <x:row r="68" spans="1:10" outlineLevel="2">
-      <x:c r="B68" s="43" t="s"/>
+      <x:c r="B68" s="35" t="s"/>
       <x:c r="C68" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -2468,7 +2392,7 @@
       <x:c r="H70" s="34" t="s"/>
     </x:row>
     <x:row r="71" spans="1:10" outlineLevel="2">
-      <x:c r="B71" s="39" t="s"/>
+      <x:c r="B71" s="35" t="s"/>
       <x:c r="C71" s="29" t="s">
         <x:v>34</x:v>
       </x:c>
@@ -2479,8 +2403,8 @@
       <x:c r="H71" s="34" t="s"/>
     </x:row>
     <x:row r="72" spans="1:10" outlineLevel="3">
-      <x:c r="B72" s="40" t="s"/>
-      <x:c r="C72" s="41" t="s"/>
+      <x:c r="B72" s="35" t="s"/>
+      <x:c r="C72" s="36" t="s"/>
       <x:c r="D72" s="37" t="n">
         <x:v>1283</x:v>
       </x:c>
@@ -2498,8 +2422,8 @@
       </x:c>
     </x:row>
     <x:row r="73" spans="1:10" outlineLevel="3">
-      <x:c r="B73" s="40" t="s"/>
-      <x:c r="C73" s="42" t="s"/>
+      <x:c r="B73" s="35" t="s"/>
+      <x:c r="C73" s="36" t="s"/>
       <x:c r="D73" s="37" t="n">
         <x:v>1083</x:v>
       </x:c>
@@ -2517,7 +2441,7 @@
       </x:c>
     </x:row>
     <x:row r="74" spans="1:10" outlineLevel="2">
-      <x:c r="B74" s="40" t="s"/>
+      <x:c r="B74" s="35" t="s"/>
       <x:c r="C74" s="29" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -2534,7 +2458,7 @@
       </x:c>
     </x:row>
     <x:row r="75" spans="1:10" outlineLevel="2">
-      <x:c r="B75" s="40" t="s"/>
+      <x:c r="B75" s="35" t="s"/>
       <x:c r="C75" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -2545,8 +2469,8 @@
       <x:c r="H75" s="34" t="s"/>
     </x:row>
     <x:row r="76" spans="1:10" outlineLevel="3">
-      <x:c r="B76" s="40" t="s"/>
-      <x:c r="C76" s="41" t="s"/>
+      <x:c r="B76" s="35" t="s"/>
+      <x:c r="C76" s="36" t="s"/>
       <x:c r="D76" s="37" t="n">
         <x:v>1061</x:v>
       </x:c>
@@ -2564,8 +2488,8 @@
       </x:c>
     </x:row>
     <x:row r="77" spans="1:10" outlineLevel="3">
-      <x:c r="B77" s="40" t="s"/>
-      <x:c r="C77" s="44" t="s"/>
+      <x:c r="B77" s="35" t="s"/>
+      <x:c r="C77" s="36" t="s"/>
       <x:c r="D77" s="37" t="n">
         <x:v>1057</x:v>
       </x:c>
@@ -2583,8 +2507,8 @@
       </x:c>
     </x:row>
     <x:row r="78" spans="1:10" outlineLevel="3">
-      <x:c r="B78" s="40" t="s"/>
-      <x:c r="C78" s="44" t="s"/>
+      <x:c r="B78" s="35" t="s"/>
+      <x:c r="C78" s="36" t="s"/>
       <x:c r="D78" s="37" t="n">
         <x:v>1212</x:v>
       </x:c>
@@ -2602,8 +2526,8 @@
       </x:c>
     </x:row>
     <x:row r="79" spans="1:10" outlineLevel="3">
-      <x:c r="B79" s="40" t="s"/>
-      <x:c r="C79" s="44" t="s"/>
+      <x:c r="B79" s="35" t="s"/>
+      <x:c r="C79" s="36" t="s"/>
       <x:c r="D79" s="37" t="n">
         <x:v>1091</x:v>
       </x:c>
@@ -2621,8 +2545,8 @@
       </x:c>
     </x:row>
     <x:row r="80" spans="1:10" outlineLevel="3">
-      <x:c r="B80" s="40" t="s"/>
-      <x:c r="C80" s="44" t="s"/>
+      <x:c r="B80" s="35" t="s"/>
+      <x:c r="C80" s="36" t="s"/>
       <x:c r="D80" s="37" t="n">
         <x:v>1261</x:v>
       </x:c>
@@ -2640,8 +2564,8 @@
       </x:c>
     </x:row>
     <x:row r="81" spans="1:10" outlineLevel="3">
-      <x:c r="B81" s="40" t="s"/>
-      <x:c r="C81" s="44" t="s"/>
+      <x:c r="B81" s="35" t="s"/>
+      <x:c r="C81" s="36" t="s"/>
       <x:c r="D81" s="37" t="n">
         <x:v>1012</x:v>
       </x:c>
@@ -2659,8 +2583,8 @@
       </x:c>
     </x:row>
     <x:row r="82" spans="1:10" outlineLevel="3">
-      <x:c r="B82" s="40" t="s"/>
-      <x:c r="C82" s="42" t="s"/>
+      <x:c r="B82" s="35" t="s"/>
+      <x:c r="C82" s="36" t="s"/>
       <x:c r="D82" s="37" t="n">
         <x:v>1161</x:v>
       </x:c>
@@ -2678,7 +2602,7 @@
       </x:c>
     </x:row>
     <x:row r="83" spans="1:10" outlineLevel="2">
-      <x:c r="B83" s="40" t="s"/>
+      <x:c r="B83" s="35" t="s"/>
       <x:c r="C83" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -2695,7 +2619,7 @@
       </x:c>
     </x:row>
     <x:row r="84" spans="1:10" outlineLevel="2">
-      <x:c r="B84" s="40" t="s"/>
+      <x:c r="B84" s="35" t="s"/>
       <x:c r="C84" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -2706,7 +2630,7 @@
       <x:c r="H84" s="34" t="s"/>
     </x:row>
     <x:row r="85" spans="1:10" outlineLevel="3">
-      <x:c r="B85" s="40" t="s"/>
+      <x:c r="B85" s="35" t="s"/>
       <x:c r="C85" s="36" t="s"/>
       <x:c r="D85" s="37" t="n">
         <x:v>1168</x:v>
@@ -2725,7 +2649,7 @@
       </x:c>
     </x:row>
     <x:row r="86" spans="1:10" outlineLevel="2">
-      <x:c r="B86" s="40" t="s"/>
+      <x:c r="B86" s="35" t="s"/>
       <x:c r="C86" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -2742,7 +2666,7 @@
       </x:c>
     </x:row>
     <x:row r="87" spans="1:10" outlineLevel="2">
-      <x:c r="B87" s="40" t="s"/>
+      <x:c r="B87" s="35" t="s"/>
       <x:c r="C87" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -2753,7 +2677,7 @@
       <x:c r="H87" s="34" t="s"/>
     </x:row>
     <x:row r="88" spans="1:10" outlineLevel="3">
-      <x:c r="B88" s="40" t="s"/>
+      <x:c r="B88" s="35" t="s"/>
       <x:c r="C88" s="36" t="s"/>
       <x:c r="D88" s="37" t="n">
         <x:v>1148</x:v>
@@ -2772,7 +2696,7 @@
       </x:c>
     </x:row>
     <x:row r="89" spans="1:10" outlineLevel="2">
-      <x:c r="B89" s="43" t="s"/>
+      <x:c r="B89" s="35" t="s"/>
       <x:c r="C89" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -2817,7 +2741,7 @@
       <x:c r="H91" s="34" t="s"/>
     </x:row>
     <x:row r="92" spans="1:10" outlineLevel="2">
-      <x:c r="B92" s="39" t="s"/>
+      <x:c r="B92" s="35" t="s"/>
       <x:c r="C92" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2828,8 +2752,8 @@
       <x:c r="H92" s="34" t="s"/>
     </x:row>
     <x:row r="93" spans="1:10" outlineLevel="3">
-      <x:c r="B93" s="40" t="s"/>
-      <x:c r="C93" s="41" t="s"/>
+      <x:c r="B93" s="35" t="s"/>
+      <x:c r="C93" s="36" t="s"/>
       <x:c r="D93" s="37" t="n">
         <x:v>1018</x:v>
       </x:c>
@@ -2847,8 +2771,8 @@
       </x:c>
     </x:row>
     <x:row r="94" spans="1:10" outlineLevel="3">
-      <x:c r="B94" s="40" t="s"/>
-      <x:c r="C94" s="42" t="s"/>
+      <x:c r="B94" s="35" t="s"/>
+      <x:c r="C94" s="36" t="s"/>
       <x:c r="D94" s="37" t="n">
         <x:v>1118</x:v>
       </x:c>
@@ -2866,7 +2790,7 @@
       </x:c>
     </x:row>
     <x:row r="95" spans="1:10" outlineLevel="2">
-      <x:c r="B95" s="40" t="s"/>
+      <x:c r="B95" s="35" t="s"/>
       <x:c r="C95" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -2883,7 +2807,7 @@
       </x:c>
     </x:row>
     <x:row r="96" spans="1:10" outlineLevel="2">
-      <x:c r="B96" s="40" t="s"/>
+      <x:c r="B96" s="35" t="s"/>
       <x:c r="C96" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -2894,8 +2818,8 @@
       <x:c r="H96" s="34" t="s"/>
     </x:row>
     <x:row r="97" spans="1:10" outlineLevel="3">
-      <x:c r="B97" s="40" t="s"/>
-      <x:c r="C97" s="41" t="s"/>
+      <x:c r="B97" s="35" t="s"/>
+      <x:c r="C97" s="36" t="s"/>
       <x:c r="D97" s="37" t="n">
         <x:v>1162</x:v>
       </x:c>
@@ -2913,8 +2837,8 @@
       </x:c>
     </x:row>
     <x:row r="98" spans="1:10" outlineLevel="3">
-      <x:c r="B98" s="40" t="s"/>
-      <x:c r="C98" s="44" t="s"/>
+      <x:c r="B98" s="35" t="s"/>
+      <x:c r="C98" s="36" t="s"/>
       <x:c r="D98" s="37" t="n">
         <x:v>1031</x:v>
       </x:c>
@@ -2932,8 +2856,8 @@
       </x:c>
     </x:row>
     <x:row r="99" spans="1:10" outlineLevel="3">
-      <x:c r="B99" s="40" t="s"/>
-      <x:c r="C99" s="44" t="s"/>
+      <x:c r="B99" s="35" t="s"/>
+      <x:c r="C99" s="36" t="s"/>
       <x:c r="D99" s="37" t="n">
         <x:v>1064</x:v>
       </x:c>
@@ -2951,8 +2875,8 @@
       </x:c>
     </x:row>
     <x:row r="100" spans="1:10" outlineLevel="3">
-      <x:c r="B100" s="40" t="s"/>
-      <x:c r="C100" s="44" t="s"/>
+      <x:c r="B100" s="35" t="s"/>
+      <x:c r="C100" s="36" t="s"/>
       <x:c r="D100" s="37" t="n">
         <x:v>1131</x:v>
       </x:c>
@@ -2970,8 +2894,8 @@
       </x:c>
     </x:row>
     <x:row r="101" spans="1:10" outlineLevel="3">
-      <x:c r="B101" s="40" t="s"/>
-      <x:c r="C101" s="44" t="s"/>
+      <x:c r="B101" s="35" t="s"/>
+      <x:c r="C101" s="36" t="s"/>
       <x:c r="D101" s="37" t="n">
         <x:v>1058</x:v>
       </x:c>
@@ -2989,8 +2913,8 @@
       </x:c>
     </x:row>
     <x:row r="102" spans="1:10" outlineLevel="3">
-      <x:c r="B102" s="40" t="s"/>
-      <x:c r="C102" s="42" t="s"/>
+      <x:c r="B102" s="35" t="s"/>
+      <x:c r="C102" s="36" t="s"/>
       <x:c r="D102" s="37" t="n">
         <x:v>1062</x:v>
       </x:c>
@@ -3008,7 +2932,7 @@
       </x:c>
     </x:row>
     <x:row r="103" spans="1:10" outlineLevel="2">
-      <x:c r="B103" s="43" t="s"/>
+      <x:c r="B103" s="35" t="s"/>
       <x:c r="C103" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -3053,7 +2977,7 @@
       <x:c r="H105" s="34" t="s"/>
     </x:row>
     <x:row r="106" spans="1:10" outlineLevel="2">
-      <x:c r="B106" s="39" t="s"/>
+      <x:c r="B106" s="35" t="s"/>
       <x:c r="C106" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -3064,8 +2988,8 @@
       <x:c r="H106" s="34" t="s"/>
     </x:row>
     <x:row r="107" spans="1:10" outlineLevel="3">
-      <x:c r="B107" s="40" t="s"/>
-      <x:c r="C107" s="41" t="s"/>
+      <x:c r="B107" s="35" t="s"/>
+      <x:c r="C107" s="36" t="s"/>
       <x:c r="D107" s="37" t="n">
         <x:v>1066</x:v>
       </x:c>
@@ -3083,8 +3007,8 @@
       </x:c>
     </x:row>
     <x:row r="108" spans="1:10" outlineLevel="3">
-      <x:c r="B108" s="40" t="s"/>
-      <x:c r="C108" s="44" t="s"/>
+      <x:c r="B108" s="35" t="s"/>
+      <x:c r="C108" s="36" t="s"/>
       <x:c r="D108" s="37" t="n">
         <x:v>1205</x:v>
       </x:c>
@@ -3102,8 +3026,8 @@
       </x:c>
     </x:row>
     <x:row r="109" spans="1:10" outlineLevel="3">
-      <x:c r="B109" s="40" t="s"/>
-      <x:c r="C109" s="42" t="s"/>
+      <x:c r="B109" s="35" t="s"/>
+      <x:c r="C109" s="36" t="s"/>
       <x:c r="D109" s="37" t="n">
         <x:v>1166</x:v>
       </x:c>
@@ -3121,7 +3045,7 @@
       </x:c>
     </x:row>
     <x:row r="110" spans="1:10" outlineLevel="2">
-      <x:c r="B110" s="43" t="s"/>
+      <x:c r="B110" s="35" t="s"/>
       <x:c r="C110" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -3166,7 +3090,7 @@
       <x:c r="H112" s="34" t="s"/>
     </x:row>
     <x:row r="113" spans="1:10" outlineLevel="2">
-      <x:c r="B113" s="39" t="s"/>
+      <x:c r="B113" s="35" t="s"/>
       <x:c r="C113" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3177,7 +3101,7 @@
       <x:c r="H113" s="34" t="s"/>
     </x:row>
     <x:row r="114" spans="1:10" outlineLevel="3">
-      <x:c r="B114" s="40" t="s"/>
+      <x:c r="B114" s="35" t="s"/>
       <x:c r="C114" s="36" t="s"/>
       <x:c r="D114" s="37" t="n">
         <x:v>1104</x:v>
@@ -3196,7 +3120,7 @@
       </x:c>
     </x:row>
     <x:row r="115" spans="1:10" outlineLevel="2">
-      <x:c r="B115" s="40" t="s"/>
+      <x:c r="B115" s="35" t="s"/>
       <x:c r="C115" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -3213,7 +3137,7 @@
       </x:c>
     </x:row>
     <x:row r="116" spans="1:10" outlineLevel="2">
-      <x:c r="B116" s="40" t="s"/>
+      <x:c r="B116" s="35" t="s"/>
       <x:c r="C116" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -3224,7 +3148,7 @@
       <x:c r="H116" s="34" t="s"/>
     </x:row>
     <x:row r="117" spans="1:10" outlineLevel="3">
-      <x:c r="B117" s="40" t="s"/>
+      <x:c r="B117" s="35" t="s"/>
       <x:c r="C117" s="36" t="s"/>
       <x:c r="D117" s="37" t="n">
         <x:v>1292</x:v>
@@ -3243,7 +3167,7 @@
       </x:c>
     </x:row>
     <x:row r="118" spans="1:10" outlineLevel="2">
-      <x:c r="B118" s="43" t="s"/>
+      <x:c r="B118" s="35" t="s"/>
       <x:c r="C118" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -3288,7 +3212,7 @@
       <x:c r="H120" s="34" t="s"/>
     </x:row>
     <x:row r="121" spans="1:10" outlineLevel="2">
-      <x:c r="B121" s="39" t="s"/>
+      <x:c r="B121" s="35" t="s"/>
       <x:c r="C121" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3299,7 +3223,7 @@
       <x:c r="H121" s="34" t="s"/>
     </x:row>
     <x:row r="122" spans="1:10" outlineLevel="3">
-      <x:c r="B122" s="40" t="s"/>
+      <x:c r="B122" s="35" t="s"/>
       <x:c r="C122" s="36" t="s"/>
       <x:c r="D122" s="37" t="n">
         <x:v>1134</x:v>
@@ -3318,7 +3242,7 @@
       </x:c>
     </x:row>
     <x:row r="123" spans="1:10" outlineLevel="2">
-      <x:c r="B123" s="43" t="s"/>
+      <x:c r="B123" s="35" t="s"/>
       <x:c r="C123" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -3363,7 +3287,7 @@
       <x:c r="H125" s="34" t="s"/>
     </x:row>
     <x:row r="126" spans="1:10" outlineLevel="2">
-      <x:c r="B126" s="39" t="s"/>
+      <x:c r="B126" s="35" t="s"/>
       <x:c r="C126" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3374,7 +3298,7 @@
       <x:c r="H126" s="34" t="s"/>
     </x:row>
     <x:row r="127" spans="1:10" outlineLevel="3">
-      <x:c r="B127" s="40" t="s"/>
+      <x:c r="B127" s="35" t="s"/>
       <x:c r="C127" s="36" t="s"/>
       <x:c r="D127" s="37" t="n">
         <x:v>1004</x:v>
@@ -3393,7 +3317,7 @@
       </x:c>
     </x:row>
     <x:row r="128" spans="1:10" outlineLevel="2">
-      <x:c r="B128" s="40" t="s"/>
+      <x:c r="B128" s="35" t="s"/>
       <x:c r="C128" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -3410,7 +3334,7 @@
       </x:c>
     </x:row>
     <x:row r="129" spans="1:10" outlineLevel="2">
-      <x:c r="B129" s="40" t="s"/>
+      <x:c r="B129" s="35" t="s"/>
       <x:c r="C129" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -3421,8 +3345,8 @@
       <x:c r="H129" s="34" t="s"/>
     </x:row>
     <x:row r="130" spans="1:10" outlineLevel="3">
-      <x:c r="B130" s="40" t="s"/>
-      <x:c r="C130" s="41" t="s"/>
+      <x:c r="B130" s="35" t="s"/>
+      <x:c r="C130" s="36" t="s"/>
       <x:c r="D130" s="37" t="n">
         <x:v>1020</x:v>
       </x:c>
@@ -3440,8 +3364,8 @@
       </x:c>
     </x:row>
     <x:row r="131" spans="1:10" outlineLevel="3">
-      <x:c r="B131" s="40" t="s"/>
-      <x:c r="C131" s="42" t="s"/>
+      <x:c r="B131" s="35" t="s"/>
+      <x:c r="C131" s="36" t="s"/>
       <x:c r="D131" s="37" t="n">
         <x:v>1120</x:v>
       </x:c>
@@ -3459,7 +3383,7 @@
       </x:c>
     </x:row>
     <x:row r="132" spans="1:10" outlineLevel="2">
-      <x:c r="B132" s="40" t="s"/>
+      <x:c r="B132" s="35" t="s"/>
       <x:c r="C132" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -3476,7 +3400,7 @@
       </x:c>
     </x:row>
     <x:row r="133" spans="1:10" outlineLevel="2">
-      <x:c r="B133" s="40" t="s"/>
+      <x:c r="B133" s="35" t="s"/>
       <x:c r="C133" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -3487,8 +3411,8 @@
       <x:c r="H133" s="34" t="s"/>
     </x:row>
     <x:row r="134" spans="1:10" outlineLevel="3">
-      <x:c r="B134" s="40" t="s"/>
-      <x:c r="C134" s="41" t="s"/>
+      <x:c r="B134" s="35" t="s"/>
+      <x:c r="C134" s="36" t="s"/>
       <x:c r="D134" s="37" t="n">
         <x:v>1295</x:v>
       </x:c>
@@ -3506,8 +3430,8 @@
       </x:c>
     </x:row>
     <x:row r="135" spans="1:10" outlineLevel="3">
-      <x:c r="B135" s="40" t="s"/>
-      <x:c r="C135" s="42" t="s"/>
+      <x:c r="B135" s="35" t="s"/>
+      <x:c r="C135" s="36" t="s"/>
       <x:c r="D135" s="37" t="n">
         <x:v>1095</x:v>
       </x:c>
@@ -3525,7 +3449,7 @@
       </x:c>
     </x:row>
     <x:row r="136" spans="1:10" outlineLevel="2">
-      <x:c r="B136" s="43" t="s"/>
+      <x:c r="B136" s="35" t="s"/>
       <x:c r="C136" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -3570,7 +3494,7 @@
       <x:c r="H138" s="34" t="s"/>
     </x:row>
     <x:row r="139" spans="1:10" outlineLevel="2">
-      <x:c r="B139" s="39" t="s"/>
+      <x:c r="B139" s="35" t="s"/>
       <x:c r="C139" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3581,7 +3505,7 @@
       <x:c r="H139" s="34" t="s"/>
     </x:row>
     <x:row r="140" spans="1:10" outlineLevel="3">
-      <x:c r="B140" s="40" t="s"/>
+      <x:c r="B140" s="35" t="s"/>
       <x:c r="C140" s="36" t="s"/>
       <x:c r="D140" s="37" t="n">
         <x:v>1260</x:v>
@@ -3600,7 +3524,7 @@
       </x:c>
     </x:row>
     <x:row r="141" spans="1:10" outlineLevel="2">
-      <x:c r="B141" s="40" t="s"/>
+      <x:c r="B141" s="35" t="s"/>
       <x:c r="C141" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -3617,7 +3541,7 @@
       </x:c>
     </x:row>
     <x:row r="142" spans="1:10" outlineLevel="2">
-      <x:c r="B142" s="40" t="s"/>
+      <x:c r="B142" s="35" t="s"/>
       <x:c r="C142" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -3628,7 +3552,7 @@
       <x:c r="H142" s="34" t="s"/>
     </x:row>
     <x:row r="143" spans="1:10" outlineLevel="3">
-      <x:c r="B143" s="40" t="s"/>
+      <x:c r="B143" s="35" t="s"/>
       <x:c r="C143" s="36" t="s"/>
       <x:c r="D143" s="37" t="n">
         <x:v>1078</x:v>
@@ -3647,7 +3571,7 @@
       </x:c>
     </x:row>
     <x:row r="144" spans="1:10" outlineLevel="2">
-      <x:c r="B144" s="43" t="s"/>
+      <x:c r="B144" s="35" t="s"/>
       <x:c r="C144" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -3692,7 +3616,7 @@
       <x:c r="H146" s="34" t="s"/>
     </x:row>
     <x:row r="147" spans="1:10" outlineLevel="2">
-      <x:c r="B147" s="39" t="s"/>
+      <x:c r="B147" s="35" t="s"/>
       <x:c r="C147" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3703,8 +3627,8 @@
       <x:c r="H147" s="34" t="s"/>
     </x:row>
     <x:row r="148" spans="1:10" outlineLevel="3">
-      <x:c r="B148" s="40" t="s"/>
-      <x:c r="C148" s="41" t="s"/>
+      <x:c r="B148" s="35" t="s"/>
+      <x:c r="C148" s="36" t="s"/>
       <x:c r="D148" s="37" t="n">
         <x:v>1046</x:v>
       </x:c>
@@ -3722,8 +3646,8 @@
       </x:c>
     </x:row>
     <x:row r="149" spans="1:10" outlineLevel="3">
-      <x:c r="B149" s="40" t="s"/>
-      <x:c r="C149" s="42" t="s"/>
+      <x:c r="B149" s="35" t="s"/>
+      <x:c r="C149" s="36" t="s"/>
       <x:c r="D149" s="37" t="n">
         <x:v>1146</x:v>
       </x:c>
@@ -3741,7 +3665,7 @@
       </x:c>
     </x:row>
     <x:row r="150" spans="1:10" outlineLevel="2">
-      <x:c r="B150" s="40" t="s"/>
+      <x:c r="B150" s="35" t="s"/>
       <x:c r="C150" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -3758,7 +3682,7 @@
       </x:c>
     </x:row>
     <x:row r="151" spans="1:10" outlineLevel="2">
-      <x:c r="B151" s="40" t="s"/>
+      <x:c r="B151" s="35" t="s"/>
       <x:c r="C151" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -3769,8 +3693,8 @@
       <x:c r="H151" s="34" t="s"/>
     </x:row>
     <x:row r="152" spans="1:10" outlineLevel="3">
-      <x:c r="B152" s="40" t="s"/>
-      <x:c r="C152" s="41" t="s"/>
+      <x:c r="B152" s="35" t="s"/>
+      <x:c r="C152" s="36" t="s"/>
       <x:c r="D152" s="37" t="n">
         <x:v>1098</x:v>
       </x:c>
@@ -3788,8 +3712,8 @@
       </x:c>
     </x:row>
     <x:row r="153" spans="1:10" outlineLevel="3">
-      <x:c r="B153" s="40" t="s"/>
-      <x:c r="C153" s="44" t="s"/>
+      <x:c r="B153" s="35" t="s"/>
+      <x:c r="C153" s="36" t="s"/>
       <x:c r="D153" s="37" t="n">
         <x:v>1298</x:v>
       </x:c>
@@ -3807,8 +3731,8 @@
       </x:c>
     </x:row>
     <x:row r="154" spans="1:10" outlineLevel="3">
-      <x:c r="B154" s="40" t="s"/>
-      <x:c r="C154" s="42" t="s"/>
+      <x:c r="B154" s="35" t="s"/>
+      <x:c r="C154" s="36" t="s"/>
       <x:c r="D154" s="37" t="n">
         <x:v>1198</x:v>
       </x:c>
@@ -3826,7 +3750,7 @@
       </x:c>
     </x:row>
     <x:row r="155" spans="1:10" outlineLevel="2">
-      <x:c r="B155" s="43" t="s"/>
+      <x:c r="B155" s="35" t="s"/>
       <x:c r="C155" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -3871,7 +3795,7 @@
       <x:c r="H157" s="34" t="s"/>
     </x:row>
     <x:row r="158" spans="1:10" outlineLevel="2">
-      <x:c r="B158" s="39" t="s"/>
+      <x:c r="B158" s="35" t="s"/>
       <x:c r="C158" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -3882,7 +3806,7 @@
       <x:c r="H158" s="34" t="s"/>
     </x:row>
     <x:row r="159" spans="1:10" outlineLevel="3">
-      <x:c r="B159" s="40" t="s"/>
+      <x:c r="B159" s="35" t="s"/>
       <x:c r="C159" s="36" t="s"/>
       <x:c r="D159" s="37" t="n">
         <x:v>1130</x:v>
@@ -3901,7 +3825,7 @@
       </x:c>
     </x:row>
     <x:row r="160" spans="1:10" outlineLevel="2">
-      <x:c r="B160" s="43" t="s"/>
+      <x:c r="B160" s="35" t="s"/>
       <x:c r="C160" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -3946,7 +3870,7 @@
       <x:c r="H162" s="34" t="s"/>
     </x:row>
     <x:row r="163" spans="1:10" outlineLevel="2">
-      <x:c r="B163" s="39" t="s"/>
+      <x:c r="B163" s="35" t="s"/>
       <x:c r="C163" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -3957,8 +3881,8 @@
       <x:c r="H163" s="34" t="s"/>
     </x:row>
     <x:row r="164" spans="1:10" outlineLevel="3">
-      <x:c r="B164" s="40" t="s"/>
-      <x:c r="C164" s="41" t="s"/>
+      <x:c r="B164" s="35" t="s"/>
+      <x:c r="C164" s="36" t="s"/>
       <x:c r="D164" s="37" t="n">
         <x:v>1048</x:v>
       </x:c>
@@ -3976,8 +3900,8 @@
       </x:c>
     </x:row>
     <x:row r="165" spans="1:10" outlineLevel="3">
-      <x:c r="B165" s="40" t="s"/>
-      <x:c r="C165" s="42" t="s"/>
+      <x:c r="B165" s="35" t="s"/>
+      <x:c r="C165" s="36" t="s"/>
       <x:c r="D165" s="37" t="n">
         <x:v>1054</x:v>
       </x:c>
@@ -3995,7 +3919,7 @@
       </x:c>
     </x:row>
     <x:row r="166" spans="1:10" outlineLevel="2">
-      <x:c r="B166" s="43" t="s"/>
+      <x:c r="B166" s="35" t="s"/>
       <x:c r="C166" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -4040,7 +3964,7 @@
       <x:c r="H168" s="34" t="s"/>
     </x:row>
     <x:row r="169" spans="1:10" outlineLevel="2">
-      <x:c r="B169" s="39" t="s"/>
+      <x:c r="B169" s="35" t="s"/>
       <x:c r="C169" s="29" t="s">
         <x:v>34</x:v>
       </x:c>
@@ -4051,7 +3975,7 @@
       <x:c r="H169" s="34" t="s"/>
     </x:row>
     <x:row r="170" spans="1:10" outlineLevel="3">
-      <x:c r="B170" s="40" t="s"/>
+      <x:c r="B170" s="35" t="s"/>
       <x:c r="C170" s="36" t="s"/>
       <x:c r="D170" s="37" t="n">
         <x:v>1086</x:v>
@@ -4070,7 +3994,7 @@
       </x:c>
     </x:row>
     <x:row r="171" spans="1:10" outlineLevel="2">
-      <x:c r="B171" s="40" t="s"/>
+      <x:c r="B171" s="35" t="s"/>
       <x:c r="C171" s="29" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -4087,7 +4011,7 @@
       </x:c>
     </x:row>
     <x:row r="172" spans="1:10" outlineLevel="2">
-      <x:c r="B172" s="40" t="s"/>
+      <x:c r="B172" s="35" t="s"/>
       <x:c r="C172" s="29" t="s">
         <x:v>56</x:v>
       </x:c>
@@ -4098,8 +4022,8 @@
       <x:c r="H172" s="34" t="s"/>
     </x:row>
     <x:row r="173" spans="1:10" outlineLevel="3">
-      <x:c r="B173" s="40" t="s"/>
-      <x:c r="C173" s="41" t="s"/>
+      <x:c r="B173" s="35" t="s"/>
+      <x:c r="C173" s="36" t="s"/>
       <x:c r="D173" s="37" t="n">
         <x:v>1209</x:v>
       </x:c>
@@ -4117,8 +4041,8 @@
       </x:c>
     </x:row>
     <x:row r="174" spans="1:10" outlineLevel="3">
-      <x:c r="B174" s="40" t="s"/>
-      <x:c r="C174" s="44" t="s"/>
+      <x:c r="B174" s="35" t="s"/>
+      <x:c r="C174" s="36" t="s"/>
       <x:c r="D174" s="37" t="n">
         <x:v>1109</x:v>
       </x:c>
@@ -4136,8 +4060,8 @@
       </x:c>
     </x:row>
     <x:row r="175" spans="1:10" outlineLevel="3">
-      <x:c r="B175" s="40" t="s"/>
-      <x:c r="C175" s="42" t="s"/>
+      <x:c r="B175" s="35" t="s"/>
+      <x:c r="C175" s="36" t="s"/>
       <x:c r="D175" s="37" t="n">
         <x:v>1009</x:v>
       </x:c>
@@ -4155,7 +4079,7 @@
       </x:c>
     </x:row>
     <x:row r="176" spans="1:10" outlineLevel="2">
-      <x:c r="B176" s="40" t="s"/>
+      <x:c r="B176" s="35" t="s"/>
       <x:c r="C176" s="29" t="s">
         <x:v>57</x:v>
       </x:c>
@@ -4172,7 +4096,7 @@
       </x:c>
     </x:row>
     <x:row r="177" spans="1:10" outlineLevel="2">
-      <x:c r="B177" s="40" t="s"/>
+      <x:c r="B177" s="35" t="s"/>
       <x:c r="C177" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -4183,7 +4107,7 @@
       <x:c r="H177" s="34" t="s"/>
     </x:row>
     <x:row r="178" spans="1:10" outlineLevel="3">
-      <x:c r="B178" s="40" t="s"/>
+      <x:c r="B178" s="35" t="s"/>
       <x:c r="C178" s="36" t="s"/>
       <x:c r="D178" s="37" t="n">
         <x:v>1090</x:v>
@@ -4202,7 +4126,7 @@
       </x:c>
     </x:row>
     <x:row r="179" spans="1:10" outlineLevel="2">
-      <x:c r="B179" s="40" t="s"/>
+      <x:c r="B179" s="35" t="s"/>
       <x:c r="C179" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -4219,7 +4143,7 @@
       </x:c>
     </x:row>
     <x:row r="180" spans="1:10" outlineLevel="2">
-      <x:c r="B180" s="40" t="s"/>
+      <x:c r="B180" s="35" t="s"/>
       <x:c r="C180" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -4230,8 +4154,8 @@
       <x:c r="H180" s="34" t="s"/>
     </x:row>
     <x:row r="181" spans="1:10" outlineLevel="3">
-      <x:c r="B181" s="40" t="s"/>
-      <x:c r="C181" s="41" t="s"/>
+      <x:c r="B181" s="35" t="s"/>
+      <x:c r="C181" s="36" t="s"/>
       <x:c r="D181" s="37" t="n">
         <x:v>1056</x:v>
       </x:c>
@@ -4249,8 +4173,8 @@
       </x:c>
     </x:row>
     <x:row r="182" spans="1:10" outlineLevel="3">
-      <x:c r="B182" s="40" t="s"/>
-      <x:c r="C182" s="44" t="s"/>
+      <x:c r="B182" s="35" t="s"/>
+      <x:c r="C182" s="36" t="s"/>
       <x:c r="D182" s="37" t="n">
         <x:v>1197</x:v>
       </x:c>
@@ -4268,8 +4192,8 @@
       </x:c>
     </x:row>
     <x:row r="183" spans="1:10" outlineLevel="3">
-      <x:c r="B183" s="40" t="s"/>
-      <x:c r="C183" s="42" t="s"/>
+      <x:c r="B183" s="35" t="s"/>
+      <x:c r="C183" s="36" t="s"/>
       <x:c r="D183" s="37" t="n">
         <x:v>1156</x:v>
       </x:c>
@@ -4287,7 +4211,7 @@
       </x:c>
     </x:row>
     <x:row r="184" spans="1:10" outlineLevel="2">
-      <x:c r="B184" s="40" t="s"/>
+      <x:c r="B184" s="35" t="s"/>
       <x:c r="C184" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -4304,7 +4228,7 @@
       </x:c>
     </x:row>
     <x:row r="185" spans="1:10" outlineLevel="2">
-      <x:c r="B185" s="40" t="s"/>
+      <x:c r="B185" s="35" t="s"/>
       <x:c r="C185" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -4315,7 +4239,7 @@
       <x:c r="H185" s="34" t="s"/>
     </x:row>
     <x:row r="186" spans="1:10" outlineLevel="3">
-      <x:c r="B186" s="40" t="s"/>
+      <x:c r="B186" s="35" t="s"/>
       <x:c r="C186" s="36" t="s"/>
       <x:c r="D186" s="37" t="n">
         <x:v>1165</x:v>
@@ -4334,7 +4258,7 @@
       </x:c>
     </x:row>
     <x:row r="187" spans="1:10" outlineLevel="2">
-      <x:c r="B187" s="43" t="s"/>
+      <x:c r="B187" s="35" t="s"/>
       <x:c r="C187" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -4379,7 +4303,7 @@
       <x:c r="H189" s="34" t="s"/>
     </x:row>
     <x:row r="190" spans="1:10" outlineLevel="2">
-      <x:c r="B190" s="39" t="s"/>
+      <x:c r="B190" s="35" t="s"/>
       <x:c r="C190" s="29" t="s">
         <x:v>34</x:v>
       </x:c>
@@ -4390,7 +4314,7 @@
       <x:c r="H190" s="34" t="s"/>
     </x:row>
     <x:row r="191" spans="1:10" outlineLevel="3">
-      <x:c r="B191" s="40" t="s"/>
+      <x:c r="B191" s="35" t="s"/>
       <x:c r="C191" s="36" t="s"/>
       <x:c r="D191" s="37" t="n">
         <x:v>1133</x:v>
@@ -4409,7 +4333,7 @@
       </x:c>
     </x:row>
     <x:row r="192" spans="1:10" outlineLevel="2">
-      <x:c r="B192" s="40" t="s"/>
+      <x:c r="B192" s="35" t="s"/>
       <x:c r="C192" s="29" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -4426,7 +4350,7 @@
       </x:c>
     </x:row>
     <x:row r="193" spans="1:10" outlineLevel="2">
-      <x:c r="B193" s="40" t="s"/>
+      <x:c r="B193" s="35" t="s"/>
       <x:c r="C193" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -4437,7 +4361,7 @@
       <x:c r="H193" s="34" t="s"/>
     </x:row>
     <x:row r="194" spans="1:10" outlineLevel="3">
-      <x:c r="B194" s="40" t="s"/>
+      <x:c r="B194" s="35" t="s"/>
       <x:c r="C194" s="36" t="s"/>
       <x:c r="D194" s="37" t="n">
         <x:v>1024</x:v>
@@ -4456,7 +4380,7 @@
       </x:c>
     </x:row>
     <x:row r="195" spans="1:10" outlineLevel="2">
-      <x:c r="B195" s="40" t="s"/>
+      <x:c r="B195" s="35" t="s"/>
       <x:c r="C195" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -4473,7 +4397,7 @@
       </x:c>
     </x:row>
     <x:row r="196" spans="1:10" outlineLevel="2">
-      <x:c r="B196" s="40" t="s"/>
+      <x:c r="B196" s="35" t="s"/>
       <x:c r="C196" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -4484,7 +4408,7 @@
       <x:c r="H196" s="34" t="s"/>
     </x:row>
     <x:row r="197" spans="1:10" outlineLevel="3">
-      <x:c r="B197" s="40" t="s"/>
+      <x:c r="B197" s="35" t="s"/>
       <x:c r="C197" s="36" t="s"/>
       <x:c r="D197" s="37" t="n">
         <x:v>1089</x:v>
@@ -4503,7 +4427,7 @@
       </x:c>
     </x:row>
     <x:row r="198" spans="1:10" outlineLevel="2">
-      <x:c r="B198" s="43" t="s"/>
+      <x:c r="B198" s="35" t="s"/>
       <x:c r="C198" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -4548,7 +4472,7 @@
       <x:c r="H200" s="34" t="s"/>
     </x:row>
     <x:row r="201" spans="1:10" outlineLevel="2">
-      <x:c r="B201" s="39" t="s"/>
+      <x:c r="B201" s="35" t="s"/>
       <x:c r="C201" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -4559,7 +4483,7 @@
       <x:c r="H201" s="34" t="s"/>
     </x:row>
     <x:row r="202" spans="1:10" outlineLevel="3">
-      <x:c r="B202" s="40" t="s"/>
+      <x:c r="B202" s="35" t="s"/>
       <x:c r="C202" s="36" t="s"/>
       <x:c r="D202" s="37" t="n">
         <x:v>1019</x:v>
@@ -4578,7 +4502,7 @@
       </x:c>
     </x:row>
     <x:row r="203" spans="1:10" outlineLevel="2">
-      <x:c r="B203" s="43" t="s"/>
+      <x:c r="B203" s="35" t="s"/>
       <x:c r="C203" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -4623,7 +4547,7 @@
       <x:c r="H205" s="34" t="s"/>
     </x:row>
     <x:row r="206" spans="1:10" outlineLevel="2">
-      <x:c r="B206" s="39" t="s"/>
+      <x:c r="B206" s="35" t="s"/>
       <x:c r="C206" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -4634,7 +4558,7 @@
       <x:c r="H206" s="34" t="s"/>
     </x:row>
     <x:row r="207" spans="1:10" outlineLevel="3">
-      <x:c r="B207" s="40" t="s"/>
+      <x:c r="B207" s="35" t="s"/>
       <x:c r="C207" s="36" t="s"/>
       <x:c r="D207" s="37" t="n">
         <x:v>1069</x:v>
@@ -4653,7 +4577,7 @@
       </x:c>
     </x:row>
     <x:row r="208" spans="1:10" outlineLevel="2">
-      <x:c r="B208" s="43" t="s"/>
+      <x:c r="B208" s="35" t="s"/>
       <x:c r="C208" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -4698,7 +4622,7 @@
       <x:c r="H210" s="34" t="s"/>
     </x:row>
     <x:row r="211" spans="1:10" outlineLevel="2">
-      <x:c r="B211" s="39" t="s"/>
+      <x:c r="B211" s="35" t="s"/>
       <x:c r="C211" s="29" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -4709,7 +4633,7 @@
       <x:c r="H211" s="34" t="s"/>
     </x:row>
     <x:row r="212" spans="1:10" outlineLevel="3">
-      <x:c r="B212" s="40" t="s"/>
+      <x:c r="B212" s="35" t="s"/>
       <x:c r="C212" s="36" t="s"/>
       <x:c r="D212" s="37" t="n">
         <x:v>1081</x:v>
@@ -4728,7 +4652,7 @@
       </x:c>
     </x:row>
     <x:row r="213" spans="1:10" outlineLevel="2">
-      <x:c r="B213" s="40" t="s"/>
+      <x:c r="B213" s="35" t="s"/>
       <x:c r="C213" s="29" t="s">
         <x:v>29</x:v>
       </x:c>
@@ -4745,7 +4669,7 @@
       </x:c>
     </x:row>
     <x:row r="214" spans="1:10" outlineLevel="2">
-      <x:c r="B214" s="40" t="s"/>
+      <x:c r="B214" s="35" t="s"/>
       <x:c r="C214" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -4756,8 +4680,8 @@
       <x:c r="H214" s="34" t="s"/>
     </x:row>
     <x:row r="215" spans="1:10" outlineLevel="3">
-      <x:c r="B215" s="40" t="s"/>
-      <x:c r="C215" s="41" t="s"/>
+      <x:c r="B215" s="35" t="s"/>
+      <x:c r="C215" s="36" t="s"/>
       <x:c r="D215" s="37" t="n">
         <x:v>1103</x:v>
       </x:c>
@@ -4775,8 +4699,8 @@
       </x:c>
     </x:row>
     <x:row r="216" spans="1:10" outlineLevel="3">
-      <x:c r="B216" s="40" t="s"/>
-      <x:c r="C216" s="42" t="s"/>
+      <x:c r="B216" s="35" t="s"/>
+      <x:c r="C216" s="36" t="s"/>
       <x:c r="D216" s="37" t="n">
         <x:v>1063</x:v>
       </x:c>
@@ -4794,7 +4718,7 @@
       </x:c>
     </x:row>
     <x:row r="217" spans="1:10" outlineLevel="2">
-      <x:c r="B217" s="43" t="s"/>
+      <x:c r="B217" s="35" t="s"/>
       <x:c r="C217" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -4839,7 +4763,7 @@
       <x:c r="H219" s="34" t="s"/>
     </x:row>
     <x:row r="220" spans="1:10" outlineLevel="2">
-      <x:c r="B220" s="39" t="s"/>
+      <x:c r="B220" s="35" t="s"/>
       <x:c r="C220" s="29" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -4850,8 +4774,8 @@
       <x:c r="H220" s="34" t="s"/>
     </x:row>
     <x:row r="221" spans="1:10" outlineLevel="3">
-      <x:c r="B221" s="40" t="s"/>
-      <x:c r="C221" s="41" t="s"/>
+      <x:c r="B221" s="35" t="s"/>
+      <x:c r="C221" s="36" t="s"/>
       <x:c r="D221" s="37" t="n">
         <x:v>1016</x:v>
       </x:c>
@@ -4869,8 +4793,8 @@
       </x:c>
     </x:row>
     <x:row r="222" spans="1:10" outlineLevel="3">
-      <x:c r="B222" s="40" t="s"/>
-      <x:c r="C222" s="42" t="s"/>
+      <x:c r="B222" s="35" t="s"/>
+      <x:c r="C222" s="36" t="s"/>
       <x:c r="D222" s="37" t="n">
         <x:v>1116</x:v>
       </x:c>
@@ -4888,7 +4812,7 @@
       </x:c>
     </x:row>
     <x:row r="223" spans="1:10" outlineLevel="2">
-      <x:c r="B223" s="40" t="s"/>
+      <x:c r="B223" s="35" t="s"/>
       <x:c r="C223" s="29" t="s">
         <x:v>29</x:v>
       </x:c>
@@ -4905,7 +4829,7 @@
       </x:c>
     </x:row>
     <x:row r="224" spans="1:10" outlineLevel="2">
-      <x:c r="B224" s="40" t="s"/>
+      <x:c r="B224" s="35" t="s"/>
       <x:c r="C224" s="29" t="s">
         <x:v>34</x:v>
       </x:c>
@@ -4916,7 +4840,7 @@
       <x:c r="H224" s="34" t="s"/>
     </x:row>
     <x:row r="225" spans="1:10" outlineLevel="3">
-      <x:c r="B225" s="40" t="s"/>
+      <x:c r="B225" s="35" t="s"/>
       <x:c r="C225" s="36" t="s"/>
       <x:c r="D225" s="37" t="n">
         <x:v>1084</x:v>
@@ -4935,7 +4859,7 @@
       </x:c>
     </x:row>
     <x:row r="226" spans="1:10" outlineLevel="2">
-      <x:c r="B226" s="40" t="s"/>
+      <x:c r="B226" s="35" t="s"/>
       <x:c r="C226" s="29" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -4952,7 +4876,7 @@
       </x:c>
     </x:row>
     <x:row r="227" spans="1:10" outlineLevel="2">
-      <x:c r="B227" s="40" t="s"/>
+      <x:c r="B227" s="35" t="s"/>
       <x:c r="C227" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -4963,7 +4887,7 @@
       <x:c r="H227" s="34" t="s"/>
     </x:row>
     <x:row r="228" spans="1:10" outlineLevel="3">
-      <x:c r="B228" s="40" t="s"/>
+      <x:c r="B228" s="35" t="s"/>
       <x:c r="C228" s="36" t="s"/>
       <x:c r="D228" s="37" t="n">
         <x:v>1034</x:v>
@@ -4982,7 +4906,7 @@
       </x:c>
     </x:row>
     <x:row r="229" spans="1:10" outlineLevel="2">
-      <x:c r="B229" s="40" t="s"/>
+      <x:c r="B229" s="35" t="s"/>
       <x:c r="C229" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -4999,7 +4923,7 @@
       </x:c>
     </x:row>
     <x:row r="230" spans="1:10" outlineLevel="2">
-      <x:c r="B230" s="40" t="s"/>
+      <x:c r="B230" s="35" t="s"/>
       <x:c r="C230" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -5010,7 +4934,7 @@
       <x:c r="H230" s="34" t="s"/>
     </x:row>
     <x:row r="231" spans="1:10" outlineLevel="3">
-      <x:c r="B231" s="40" t="s"/>
+      <x:c r="B231" s="35" t="s"/>
       <x:c r="C231" s="36" t="s"/>
       <x:c r="D231" s="37" t="n">
         <x:v>1093</x:v>
@@ -5029,7 +4953,7 @@
       </x:c>
     </x:row>
     <x:row r="232" spans="1:10" outlineLevel="2">
-      <x:c r="B232" s="43" t="s"/>
+      <x:c r="B232" s="35" t="s"/>
       <x:c r="C232" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -5074,7 +4998,7 @@
       <x:c r="H234" s="34" t="s"/>
     </x:row>
     <x:row r="235" spans="1:10" outlineLevel="2">
-      <x:c r="B235" s="39" t="s"/>
+      <x:c r="B235" s="35" t="s"/>
       <x:c r="C235" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -5085,8 +5009,8 @@
       <x:c r="H235" s="34" t="s"/>
     </x:row>
     <x:row r="236" spans="1:10" outlineLevel="3">
-      <x:c r="B236" s="40" t="s"/>
-      <x:c r="C236" s="41" t="s"/>
+      <x:c r="B236" s="35" t="s"/>
+      <x:c r="C236" s="36" t="s"/>
       <x:c r="D236" s="37" t="n">
         <x:v>1015</x:v>
       </x:c>
@@ -5104,8 +5028,8 @@
       </x:c>
     </x:row>
     <x:row r="237" spans="1:10" outlineLevel="3">
-      <x:c r="B237" s="40" t="s"/>
-      <x:c r="C237" s="44" t="s"/>
+      <x:c r="B237" s="35" t="s"/>
+      <x:c r="C237" s="36" t="s"/>
       <x:c r="D237" s="37" t="n">
         <x:v>1315</x:v>
       </x:c>
@@ -5123,8 +5047,8 @@
       </x:c>
     </x:row>
     <x:row r="238" spans="1:10" outlineLevel="3">
-      <x:c r="B238" s="40" t="s"/>
-      <x:c r="C238" s="42" t="s"/>
+      <x:c r="B238" s="35" t="s"/>
+      <x:c r="C238" s="36" t="s"/>
       <x:c r="D238" s="37" t="n">
         <x:v>1215</x:v>
       </x:c>
@@ -5142,7 +5066,7 @@
       </x:c>
     </x:row>
     <x:row r="239" spans="1:10" outlineLevel="2">
-      <x:c r="B239" s="40" t="s"/>
+      <x:c r="B239" s="35" t="s"/>
       <x:c r="C239" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -5159,7 +5083,7 @@
       </x:c>
     </x:row>
     <x:row r="240" spans="1:10" outlineLevel="2">
-      <x:c r="B240" s="40" t="s"/>
+      <x:c r="B240" s="35" t="s"/>
       <x:c r="C240" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -5170,8 +5094,8 @@
       <x:c r="H240" s="34" t="s"/>
     </x:row>
     <x:row r="241" spans="1:10" outlineLevel="3">
-      <x:c r="B241" s="40" t="s"/>
-      <x:c r="C241" s="41" t="s"/>
+      <x:c r="B241" s="35" t="s"/>
+      <x:c r="C241" s="36" t="s"/>
       <x:c r="D241" s="37" t="n">
         <x:v>1128</x:v>
       </x:c>
@@ -5189,8 +5113,8 @@
       </x:c>
     </x:row>
     <x:row r="242" spans="1:10" outlineLevel="3">
-      <x:c r="B242" s="40" t="s"/>
-      <x:c r="C242" s="42" t="s"/>
+      <x:c r="B242" s="35" t="s"/>
+      <x:c r="C242" s="36" t="s"/>
       <x:c r="D242" s="37" t="n">
         <x:v>1028</x:v>
       </x:c>
@@ -5208,7 +5132,7 @@
       </x:c>
     </x:row>
     <x:row r="243" spans="1:10" outlineLevel="2">
-      <x:c r="B243" s="43" t="s"/>
+      <x:c r="B243" s="35" t="s"/>
       <x:c r="C243" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -5253,7 +5177,7 @@
       <x:c r="H245" s="34" t="s"/>
     </x:row>
     <x:row r="246" spans="1:10" outlineLevel="2">
-      <x:c r="B246" s="39" t="s"/>
+      <x:c r="B246" s="35" t="s"/>
       <x:c r="C246" s="29" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -5264,8 +5188,8 @@
       <x:c r="H246" s="34" t="s"/>
     </x:row>
     <x:row r="247" spans="1:10" outlineLevel="3">
-      <x:c r="B247" s="40" t="s"/>
-      <x:c r="C247" s="41" t="s"/>
+      <x:c r="B247" s="35" t="s"/>
+      <x:c r="C247" s="36" t="s"/>
       <x:c r="D247" s="37" t="n">
         <x:v>1141</x:v>
       </x:c>
@@ -5283,8 +5207,8 @@
       </x:c>
     </x:row>
     <x:row r="248" spans="1:10" outlineLevel="3">
-      <x:c r="B248" s="40" t="s"/>
-      <x:c r="C248" s="42" t="s"/>
+      <x:c r="B248" s="35" t="s"/>
+      <x:c r="C248" s="36" t="s"/>
       <x:c r="D248" s="37" t="n">
         <x:v>1041</x:v>
       </x:c>
@@ -5302,7 +5226,7 @@
       </x:c>
     </x:row>
     <x:row r="249" spans="1:10" outlineLevel="2">
-      <x:c r="B249" s="43" t="s"/>
+      <x:c r="B249" s="35" t="s"/>
       <x:c r="C249" s="29" t="s">
         <x:v>29</x:v>
       </x:c>
@@ -5347,7 +5271,7 @@
       <x:c r="H251" s="34" t="s"/>
     </x:row>
     <x:row r="252" spans="1:10" outlineLevel="2">
-      <x:c r="B252" s="39" t="s"/>
+      <x:c r="B252" s="35" t="s"/>
       <x:c r="C252" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -5358,8 +5282,8 @@
       <x:c r="H252" s="34" t="s"/>
     </x:row>
     <x:row r="253" spans="1:10" outlineLevel="3">
-      <x:c r="B253" s="40" t="s"/>
-      <x:c r="C253" s="41" t="s"/>
+      <x:c r="B253" s="35" t="s"/>
+      <x:c r="C253" s="36" t="s"/>
       <x:c r="D253" s="37" t="n">
         <x:v>1023</x:v>
       </x:c>
@@ -5377,8 +5301,8 @@
       </x:c>
     </x:row>
     <x:row r="254" spans="1:10" outlineLevel="3">
-      <x:c r="B254" s="40" t="s"/>
-      <x:c r="C254" s="42" t="s"/>
+      <x:c r="B254" s="35" t="s"/>
+      <x:c r="C254" s="36" t="s"/>
       <x:c r="D254" s="37" t="n">
         <x:v>1123</x:v>
       </x:c>
@@ -5396,7 +5320,7 @@
       </x:c>
     </x:row>
     <x:row r="255" spans="1:10" outlineLevel="2">
-      <x:c r="B255" s="40" t="s"/>
+      <x:c r="B255" s="35" t="s"/>
       <x:c r="C255" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -5413,7 +5337,7 @@
       </x:c>
     </x:row>
     <x:row r="256" spans="1:10" outlineLevel="2">
-      <x:c r="B256" s="40" t="s"/>
+      <x:c r="B256" s="35" t="s"/>
       <x:c r="C256" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -5424,8 +5348,8 @@
       <x:c r="H256" s="34" t="s"/>
     </x:row>
     <x:row r="257" spans="1:10" outlineLevel="3">
-      <x:c r="B257" s="40" t="s"/>
-      <x:c r="C257" s="41" t="s"/>
+      <x:c r="B257" s="35" t="s"/>
+      <x:c r="C257" s="36" t="s"/>
       <x:c r="D257" s="37" t="n">
         <x:v>1269</x:v>
       </x:c>
@@ -5443,8 +5367,8 @@
       </x:c>
     </x:row>
     <x:row r="258" spans="1:10" outlineLevel="3">
-      <x:c r="B258" s="40" t="s"/>
-      <x:c r="C258" s="42" t="s"/>
+      <x:c r="B258" s="35" t="s"/>
+      <x:c r="C258" s="36" t="s"/>
       <x:c r="D258" s="37" t="n">
         <x:v>1169</x:v>
       </x:c>
@@ -5462,7 +5386,7 @@
       </x:c>
     </x:row>
     <x:row r="259" spans="1:10" outlineLevel="2">
-      <x:c r="B259" s="40" t="s"/>
+      <x:c r="B259" s="35" t="s"/>
       <x:c r="C259" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -5479,7 +5403,7 @@
       </x:c>
     </x:row>
     <x:row r="260" spans="1:10" outlineLevel="2">
-      <x:c r="B260" s="40" t="s"/>
+      <x:c r="B260" s="35" t="s"/>
       <x:c r="C260" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -5490,8 +5414,8 @@
       <x:c r="H260" s="34" t="s"/>
     </x:row>
     <x:row r="261" spans="1:10" outlineLevel="3">
-      <x:c r="B261" s="40" t="s"/>
-      <x:c r="C261" s="41" t="s"/>
+      <x:c r="B261" s="35" t="s"/>
+      <x:c r="C261" s="36" t="s"/>
       <x:c r="D261" s="37" t="n">
         <x:v>1076</x:v>
       </x:c>
@@ -5509,8 +5433,8 @@
       </x:c>
     </x:row>
     <x:row r="262" spans="1:10" outlineLevel="3">
-      <x:c r="B262" s="40" t="s"/>
-      <x:c r="C262" s="42" t="s"/>
+      <x:c r="B262" s="35" t="s"/>
+      <x:c r="C262" s="36" t="s"/>
       <x:c r="D262" s="37" t="n">
         <x:v>1176</x:v>
       </x:c>
@@ -5528,7 +5452,7 @@
       </x:c>
     </x:row>
     <x:row r="263" spans="1:10" outlineLevel="2">
-      <x:c r="B263" s="43" t="s"/>
+      <x:c r="B263" s="35" t="s"/>
       <x:c r="C263" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -5573,7 +5497,7 @@
       <x:c r="H265" s="34" t="s"/>
     </x:row>
     <x:row r="266" spans="1:10" outlineLevel="2">
-      <x:c r="B266" s="39" t="s"/>
+      <x:c r="B266" s="35" t="s"/>
       <x:c r="C266" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -5584,8 +5508,8 @@
       <x:c r="H266" s="34" t="s"/>
     </x:row>
     <x:row r="267" spans="1:10" outlineLevel="3">
-      <x:c r="B267" s="40" t="s"/>
-      <x:c r="C267" s="41" t="s"/>
+      <x:c r="B267" s="35" t="s"/>
+      <x:c r="C267" s="36" t="s"/>
       <x:c r="D267" s="37" t="n">
         <x:v>1096</x:v>
       </x:c>
@@ -5603,8 +5527,8 @@
       </x:c>
     </x:row>
     <x:row r="268" spans="1:10" outlineLevel="3">
-      <x:c r="B268" s="40" t="s"/>
-      <x:c r="C268" s="42" t="s"/>
+      <x:c r="B268" s="35" t="s"/>
+      <x:c r="C268" s="36" t="s"/>
       <x:c r="D268" s="37" t="n">
         <x:v>1196</x:v>
       </x:c>
@@ -5622,7 +5546,7 @@
       </x:c>
     </x:row>
     <x:row r="269" spans="1:10" outlineLevel="2">
-      <x:c r="B269" s="43" t="s"/>
+      <x:c r="B269" s="35" t="s"/>
       <x:c r="C269" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -5667,7 +5591,7 @@
       <x:c r="H271" s="34" t="s"/>
     </x:row>
     <x:row r="272" spans="1:10" outlineLevel="2">
-      <x:c r="B272" s="39" t="s"/>
+      <x:c r="B272" s="35" t="s"/>
       <x:c r="C272" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -5678,7 +5602,7 @@
       <x:c r="H272" s="34" t="s"/>
     </x:row>
     <x:row r="273" spans="1:10" outlineLevel="3">
-      <x:c r="B273" s="40" t="s"/>
+      <x:c r="B273" s="35" t="s"/>
       <x:c r="C273" s="36" t="s"/>
       <x:c r="D273" s="37" t="n">
         <x:v>1158</x:v>
@@ -5697,7 +5621,7 @@
       </x:c>
     </x:row>
     <x:row r="274" spans="1:10" outlineLevel="2">
-      <x:c r="B274" s="43" t="s"/>
+      <x:c r="B274" s="35" t="s"/>
       <x:c r="C274" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -5742,7 +5666,7 @@
       <x:c r="H276" s="34" t="s"/>
     </x:row>
     <x:row r="277" spans="1:10" outlineLevel="2">
-      <x:c r="B277" s="39" t="s"/>
+      <x:c r="B277" s="35" t="s"/>
       <x:c r="C277" s="29" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -5753,8 +5677,8 @@
       <x:c r="H277" s="34" t="s"/>
     </x:row>
     <x:row r="278" spans="1:10" outlineLevel="3">
-      <x:c r="B278" s="40" t="s"/>
-      <x:c r="C278" s="41" t="s"/>
+      <x:c r="B278" s="35" t="s"/>
+      <x:c r="C278" s="36" t="s"/>
       <x:c r="D278" s="37" t="n">
         <x:v>1026</x:v>
       </x:c>
@@ -5772,8 +5696,8 @@
       </x:c>
     </x:row>
     <x:row r="279" spans="1:10" outlineLevel="3">
-      <x:c r="B279" s="40" t="s"/>
-      <x:c r="C279" s="42" t="s"/>
+      <x:c r="B279" s="35" t="s"/>
+      <x:c r="C279" s="36" t="s"/>
       <x:c r="D279" s="37" t="n">
         <x:v>1126</x:v>
       </x:c>
@@ -5791,7 +5715,7 @@
       </x:c>
     </x:row>
     <x:row r="280" spans="1:10" outlineLevel="2">
-      <x:c r="B280" s="40" t="s"/>
+      <x:c r="B280" s="35" t="s"/>
       <x:c r="C280" s="29" t="s">
         <x:v>29</x:v>
       </x:c>
@@ -5808,7 +5732,7 @@
       </x:c>
     </x:row>
     <x:row r="281" spans="1:10" outlineLevel="2">
-      <x:c r="B281" s="40" t="s"/>
+      <x:c r="B281" s="35" t="s"/>
       <x:c r="C281" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -5819,8 +5743,8 @@
       <x:c r="H281" s="34" t="s"/>
     </x:row>
     <x:row r="282" spans="1:10" outlineLevel="3">
-      <x:c r="B282" s="40" t="s"/>
-      <x:c r="C282" s="41" t="s"/>
+      <x:c r="B282" s="35" t="s"/>
+      <x:c r="C282" s="36" t="s"/>
       <x:c r="D282" s="37" t="n">
         <x:v>1013</x:v>
       </x:c>
@@ -5838,8 +5762,8 @@
       </x:c>
     </x:row>
     <x:row r="283" spans="1:10" outlineLevel="3">
-      <x:c r="B283" s="40" t="s"/>
-      <x:c r="C283" s="42" t="s"/>
+      <x:c r="B283" s="35" t="s"/>
+      <x:c r="C283" s="36" t="s"/>
       <x:c r="D283" s="37" t="n">
         <x:v>1113</x:v>
       </x:c>
@@ -5857,7 +5781,7 @@
       </x:c>
     </x:row>
     <x:row r="284" spans="1:10" outlineLevel="2">
-      <x:c r="B284" s="43" t="s"/>
+      <x:c r="B284" s="35" t="s"/>
       <x:c r="C284" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -5902,7 +5826,7 @@
       <x:c r="H286" s="34" t="s"/>
     </x:row>
     <x:row r="287" spans="1:10" outlineLevel="2">
-      <x:c r="B287" s="39" t="s"/>
+      <x:c r="B287" s="35" t="s"/>
       <x:c r="C287" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -5913,7 +5837,7 @@
       <x:c r="H287" s="34" t="s"/>
     </x:row>
     <x:row r="288" spans="1:10" outlineLevel="3">
-      <x:c r="B288" s="40" t="s"/>
+      <x:c r="B288" s="35" t="s"/>
       <x:c r="C288" s="36" t="s"/>
       <x:c r="D288" s="37" t="n">
         <x:v>1860</x:v>
@@ -5930,7 +5854,7 @@
       </x:c>
     </x:row>
     <x:row r="289" spans="1:10" outlineLevel="2">
-      <x:c r="B289" s="40" t="s"/>
+      <x:c r="B289" s="35" t="s"/>
       <x:c r="C289" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -5947,7 +5871,7 @@
       </x:c>
     </x:row>
     <x:row r="290" spans="1:10" outlineLevel="2">
-      <x:c r="B290" s="40" t="s"/>
+      <x:c r="B290" s="35" t="s"/>
       <x:c r="C290" s="29" t="s">
         <x:v>56</x:v>
       </x:c>
@@ -5958,7 +5882,7 @@
       <x:c r="H290" s="34" t="s"/>
     </x:row>
     <x:row r="291" spans="1:10" outlineLevel="3">
-      <x:c r="B291" s="40" t="s"/>
+      <x:c r="B291" s="35" t="s"/>
       <x:c r="C291" s="36" t="s"/>
       <x:c r="D291" s="37" t="n">
         <x:v>1309</x:v>
@@ -5977,7 +5901,7 @@
       </x:c>
     </x:row>
     <x:row r="292" spans="1:10" outlineLevel="2">
-      <x:c r="B292" s="40" t="s"/>
+      <x:c r="B292" s="35" t="s"/>
       <x:c r="C292" s="29" t="s">
         <x:v>57</x:v>
       </x:c>
@@ -5994,7 +5918,7 @@
       </x:c>
     </x:row>
     <x:row r="293" spans="1:10" outlineLevel="2">
-      <x:c r="B293" s="40" t="s"/>
+      <x:c r="B293" s="35" t="s"/>
       <x:c r="C293" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -6005,8 +5929,8 @@
       <x:c r="H293" s="34" t="s"/>
     </x:row>
     <x:row r="294" spans="1:10" outlineLevel="3">
-      <x:c r="B294" s="40" t="s"/>
-      <x:c r="C294" s="41" t="s"/>
+      <x:c r="B294" s="35" t="s"/>
+      <x:c r="C294" s="36" t="s"/>
       <x:c r="D294" s="37" t="n">
         <x:v>1030</x:v>
       </x:c>
@@ -6024,8 +5948,8 @@
       </x:c>
     </x:row>
     <x:row r="295" spans="1:10" outlineLevel="3">
-      <x:c r="B295" s="40" t="s"/>
-      <x:c r="C295" s="42" t="s"/>
+      <x:c r="B295" s="35" t="s"/>
+      <x:c r="C295" s="36" t="s"/>
       <x:c r="D295" s="37" t="n">
         <x:v>1097</x:v>
       </x:c>
@@ -6043,7 +5967,7 @@
       </x:c>
     </x:row>
     <x:row r="296" spans="1:10" outlineLevel="2">
-      <x:c r="B296" s="43" t="s"/>
+      <x:c r="B296" s="35" t="s"/>
       <x:c r="C296" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -6088,7 +6012,7 @@
       <x:c r="H298" s="34" t="s"/>
     </x:row>
     <x:row r="299" spans="1:10" outlineLevel="2">
-      <x:c r="B299" s="39" t="s"/>
+      <x:c r="B299" s="35" t="s"/>
       <x:c r="C299" s="29" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -6099,7 +6023,7 @@
       <x:c r="H299" s="34" t="s"/>
     </x:row>
     <x:row r="300" spans="1:10" outlineLevel="3">
-      <x:c r="B300" s="40" t="s"/>
+      <x:c r="B300" s="35" t="s"/>
       <x:c r="C300" s="36" t="s"/>
       <x:c r="D300" s="37" t="n">
         <x:v>1082</x:v>
@@ -6118,7 +6042,7 @@
       </x:c>
     </x:row>
     <x:row r="301" spans="1:10" outlineLevel="2">
-      <x:c r="B301" s="40" t="s"/>
+      <x:c r="B301" s="35" t="s"/>
       <x:c r="C301" s="29" t="s">
         <x:v>29</x:v>
       </x:c>
@@ -6135,7 +6059,7 @@
       </x:c>
     </x:row>
     <x:row r="302" spans="1:10" outlineLevel="2">
-      <x:c r="B302" s="40" t="s"/>
+      <x:c r="B302" s="35" t="s"/>
       <x:c r="C302" s="29" t="s">
         <x:v>56</x:v>
       </x:c>
@@ -6146,7 +6070,7 @@
       <x:c r="H302" s="34" t="s"/>
     </x:row>
     <x:row r="303" spans="1:10" outlineLevel="3">
-      <x:c r="B303" s="40" t="s"/>
+      <x:c r="B303" s="35" t="s"/>
       <x:c r="C303" s="36" t="s"/>
       <x:c r="D303" s="37" t="n">
         <x:v>1010</x:v>
@@ -6165,7 +6089,7 @@
       </x:c>
     </x:row>
     <x:row r="304" spans="1:10" outlineLevel="2">
-      <x:c r="B304" s="40" t="s"/>
+      <x:c r="B304" s="35" t="s"/>
       <x:c r="C304" s="29" t="s">
         <x:v>57</x:v>
       </x:c>
@@ -6182,7 +6106,7 @@
       </x:c>
     </x:row>
     <x:row r="305" spans="1:10" outlineLevel="2">
-      <x:c r="B305" s="40" t="s"/>
+      <x:c r="B305" s="35" t="s"/>
       <x:c r="C305" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -6193,8 +6117,8 @@
       <x:c r="H305" s="34" t="s"/>
     </x:row>
     <x:row r="306" spans="1:10" outlineLevel="3">
-      <x:c r="B306" s="40" t="s"/>
-      <x:c r="C306" s="41" t="s"/>
+      <x:c r="B306" s="35" t="s"/>
+      <x:c r="C306" s="36" t="s"/>
       <x:c r="D306" s="37" t="n">
         <x:v>1170</x:v>
       </x:c>
@@ -6212,8 +6136,8 @@
       </x:c>
     </x:row>
     <x:row r="307" spans="1:10" outlineLevel="3">
-      <x:c r="B307" s="40" t="s"/>
-      <x:c r="C307" s="42" t="s"/>
+      <x:c r="B307" s="35" t="s"/>
+      <x:c r="C307" s="36" t="s"/>
       <x:c r="D307" s="37" t="n">
         <x:v>1077</x:v>
       </x:c>
@@ -6231,7 +6155,7 @@
       </x:c>
     </x:row>
     <x:row r="308" spans="1:10" outlineLevel="2">
-      <x:c r="B308" s="43" t="s"/>
+      <x:c r="B308" s="35" t="s"/>
       <x:c r="C308" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -6276,7 +6200,7 @@
       <x:c r="H310" s="34" t="s"/>
     </x:row>
     <x:row r="311" spans="1:10" outlineLevel="2">
-      <x:c r="B311" s="39" t="s"/>
+      <x:c r="B311" s="35" t="s"/>
       <x:c r="C311" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -6287,8 +6211,8 @@
       <x:c r="H311" s="34" t="s"/>
     </x:row>
     <x:row r="312" spans="1:10" outlineLevel="3">
-      <x:c r="B312" s="40" t="s"/>
-      <x:c r="C312" s="41" t="s"/>
+      <x:c r="B312" s="35" t="s"/>
+      <x:c r="C312" s="36" t="s"/>
       <x:c r="D312" s="37" t="n">
         <x:v>1045</x:v>
       </x:c>
@@ -6306,8 +6230,8 @@
       </x:c>
     </x:row>
     <x:row r="313" spans="1:10" outlineLevel="3">
-      <x:c r="B313" s="40" t="s"/>
-      <x:c r="C313" s="42" t="s"/>
+      <x:c r="B313" s="35" t="s"/>
+      <x:c r="C313" s="36" t="s"/>
       <x:c r="D313" s="37" t="n">
         <x:v>1145</x:v>
       </x:c>
@@ -6325,7 +6249,7 @@
       </x:c>
     </x:row>
     <x:row r="314" spans="1:10" outlineLevel="2">
-      <x:c r="B314" s="40" t="s"/>
+      <x:c r="B314" s="35" t="s"/>
       <x:c r="C314" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -6342,7 +6266,7 @@
       </x:c>
     </x:row>
     <x:row r="315" spans="1:10" outlineLevel="2">
-      <x:c r="B315" s="40" t="s"/>
+      <x:c r="B315" s="35" t="s"/>
       <x:c r="C315" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -6353,8 +6277,8 @@
       <x:c r="H315" s="34" t="s"/>
     </x:row>
     <x:row r="316" spans="1:10" outlineLevel="3">
-      <x:c r="B316" s="40" t="s"/>
-      <x:c r="C316" s="41" t="s"/>
+      <x:c r="B316" s="35" t="s"/>
+      <x:c r="C316" s="36" t="s"/>
       <x:c r="D316" s="37" t="n">
         <x:v>1149</x:v>
       </x:c>
@@ -6372,8 +6296,8 @@
       </x:c>
     </x:row>
     <x:row r="317" spans="1:10" outlineLevel="3">
-      <x:c r="B317" s="40" t="s"/>
-      <x:c r="C317" s="42" t="s"/>
+      <x:c r="B317" s="35" t="s"/>
+      <x:c r="C317" s="36" t="s"/>
       <x:c r="D317" s="37" t="n">
         <x:v>1049</x:v>
       </x:c>
@@ -6391,7 +6315,7 @@
       </x:c>
     </x:row>
     <x:row r="318" spans="1:10" outlineLevel="2">
-      <x:c r="B318" s="43" t="s"/>
+      <x:c r="B318" s="35" t="s"/>
       <x:c r="C318" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -6436,7 +6360,7 @@
       <x:c r="H320" s="34" t="s"/>
     </x:row>
     <x:row r="321" spans="1:10" outlineLevel="2">
-      <x:c r="B321" s="39" t="s"/>
+      <x:c r="B321" s="35" t="s"/>
       <x:c r="C321" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -6447,7 +6371,7 @@
       <x:c r="H321" s="34" t="s"/>
     </x:row>
     <x:row r="322" spans="1:10" outlineLevel="3">
-      <x:c r="B322" s="40" t="s"/>
+      <x:c r="B322" s="35" t="s"/>
       <x:c r="C322" s="36" t="s"/>
       <x:c r="D322" s="37" t="n">
         <x:v>1092</x:v>
@@ -6466,7 +6390,7 @@
       </x:c>
     </x:row>
     <x:row r="323" spans="1:10" outlineLevel="2">
-      <x:c r="B323" s="43" t="s"/>
+      <x:c r="B323" s="35" t="s"/>
       <x:c r="C323" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -6511,7 +6435,7 @@
       <x:c r="H325" s="34" t="s"/>
     </x:row>
     <x:row r="326" spans="1:10" outlineLevel="2">
-      <x:c r="B326" s="39" t="s"/>
+      <x:c r="B326" s="35" t="s"/>
       <x:c r="C326" s="29" t="s">
         <x:v>34</x:v>
       </x:c>
@@ -6522,7 +6446,7 @@
       <x:c r="H326" s="34" t="s"/>
     </x:row>
     <x:row r="327" spans="1:10" outlineLevel="3">
-      <x:c r="B327" s="40" t="s"/>
+      <x:c r="B327" s="35" t="s"/>
       <x:c r="C327" s="36" t="s"/>
       <x:c r="D327" s="37" t="n">
         <x:v>1047</x:v>
@@ -6541,7 +6465,7 @@
       </x:c>
     </x:row>
     <x:row r="328" spans="1:10" outlineLevel="2">
-      <x:c r="B328" s="40" t="s"/>
+      <x:c r="B328" s="35" t="s"/>
       <x:c r="C328" s="29" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -6558,7 +6482,7 @@
       </x:c>
     </x:row>
     <x:row r="329" spans="1:10" outlineLevel="2">
-      <x:c r="B329" s="40" t="s"/>
+      <x:c r="B329" s="35" t="s"/>
       <x:c r="C329" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -6569,8 +6493,8 @@
       <x:c r="H329" s="34" t="s"/>
     </x:row>
     <x:row r="330" spans="1:10" outlineLevel="3">
-      <x:c r="B330" s="40" t="s"/>
-      <x:c r="C330" s="41" t="s"/>
+      <x:c r="B330" s="35" t="s"/>
+      <x:c r="C330" s="36" t="s"/>
       <x:c r="D330" s="37" t="n">
         <x:v>1144</x:v>
       </x:c>
@@ -6588,8 +6512,8 @@
       </x:c>
     </x:row>
     <x:row r="331" spans="1:10" outlineLevel="3">
-      <x:c r="B331" s="40" t="s"/>
-      <x:c r="C331" s="42" t="s"/>
+      <x:c r="B331" s="35" t="s"/>
+      <x:c r="C331" s="36" t="s"/>
       <x:c r="D331" s="37" t="n">
         <x:v>1044</x:v>
       </x:c>
@@ -6607,7 +6531,7 @@
       </x:c>
     </x:row>
     <x:row r="332" spans="1:10" outlineLevel="2">
-      <x:c r="B332" s="43" t="s"/>
+      <x:c r="B332" s="35" t="s"/>
       <x:c r="C332" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -6652,7 +6576,7 @@
       <x:c r="H334" s="34" t="s"/>
     </x:row>
     <x:row r="335" spans="1:10" outlineLevel="2">
-      <x:c r="B335" s="39" t="s"/>
+      <x:c r="B335" s="35" t="s"/>
       <x:c r="C335" s="29" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -6663,8 +6587,8 @@
       <x:c r="H335" s="34" t="s"/>
     </x:row>
     <x:row r="336" spans="1:10" outlineLevel="3">
-      <x:c r="B336" s="40" t="s"/>
-      <x:c r="C336" s="41" t="s"/>
+      <x:c r="B336" s="35" t="s"/>
+      <x:c r="C336" s="36" t="s"/>
       <x:c r="D336" s="37" t="n">
         <x:v>1025</x:v>
       </x:c>
@@ -6682,8 +6606,8 @@
       </x:c>
     </x:row>
     <x:row r="337" spans="1:10" outlineLevel="3">
-      <x:c r="B337" s="40" t="s"/>
-      <x:c r="C337" s="42" t="s"/>
+      <x:c r="B337" s="35" t="s"/>
+      <x:c r="C337" s="36" t="s"/>
       <x:c r="D337" s="37" t="n">
         <x:v>1125</x:v>
       </x:c>
@@ -6701,7 +6625,7 @@
       </x:c>
     </x:row>
     <x:row r="338" spans="1:10" outlineLevel="2">
-      <x:c r="B338" s="40" t="s"/>
+      <x:c r="B338" s="35" t="s"/>
       <x:c r="C338" s="29" t="s">
         <x:v>29</x:v>
       </x:c>
@@ -6718,7 +6642,7 @@
       </x:c>
     </x:row>
     <x:row r="339" spans="1:10" outlineLevel="2">
-      <x:c r="B339" s="40" t="s"/>
+      <x:c r="B339" s="35" t="s"/>
       <x:c r="C339" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -6729,8 +6653,8 @@
       <x:c r="H339" s="34" t="s"/>
     </x:row>
     <x:row r="340" spans="1:10" outlineLevel="3">
-      <x:c r="B340" s="40" t="s"/>
-      <x:c r="C340" s="41" t="s"/>
+      <x:c r="B340" s="35" t="s"/>
+      <x:c r="C340" s="36" t="s"/>
       <x:c r="D340" s="37" t="n">
         <x:v>1008</x:v>
       </x:c>
@@ -6748,8 +6672,8 @@
       </x:c>
     </x:row>
     <x:row r="341" spans="1:10" outlineLevel="3">
-      <x:c r="B341" s="40" t="s"/>
-      <x:c r="C341" s="42" t="s"/>
+      <x:c r="B341" s="35" t="s"/>
+      <x:c r="C341" s="36" t="s"/>
       <x:c r="D341" s="37" t="n">
         <x:v>1139</x:v>
       </x:c>
@@ -6767,7 +6691,7 @@
       </x:c>
     </x:row>
     <x:row r="342" spans="1:10" outlineLevel="2">
-      <x:c r="B342" s="43" t="s"/>
+      <x:c r="B342" s="35" t="s"/>
       <x:c r="C342" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -6812,7 +6736,7 @@
       <x:c r="H344" s="34" t="s"/>
     </x:row>
     <x:row r="345" spans="1:10" outlineLevel="2">
-      <x:c r="B345" s="39" t="s"/>
+      <x:c r="B345" s="35" t="s"/>
       <x:c r="C345" s="29" t="s">
         <x:v>34</x:v>
       </x:c>
@@ -6823,7 +6747,7 @@
       <x:c r="H345" s="34" t="s"/>
     </x:row>
     <x:row r="346" spans="1:10" outlineLevel="3">
-      <x:c r="B346" s="40" t="s"/>
+      <x:c r="B346" s="35" t="s"/>
       <x:c r="C346" s="36" t="s"/>
       <x:c r="D346" s="37" t="n">
         <x:v>1183</x:v>
@@ -6842,7 +6766,7 @@
       </x:c>
     </x:row>
     <x:row r="347" spans="1:10" outlineLevel="2">
-      <x:c r="B347" s="40" t="s"/>
+      <x:c r="B347" s="35" t="s"/>
       <x:c r="C347" s="29" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -6859,7 +6783,7 @@
       </x:c>
     </x:row>
     <x:row r="348" spans="1:10" outlineLevel="2">
-      <x:c r="B348" s="40" t="s"/>
+      <x:c r="B348" s="35" t="s"/>
       <x:c r="C348" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -6870,7 +6794,7 @@
       <x:c r="H348" s="34" t="s"/>
     </x:row>
     <x:row r="349" spans="1:10" outlineLevel="3">
-      <x:c r="B349" s="40" t="s"/>
+      <x:c r="B349" s="35" t="s"/>
       <x:c r="C349" s="36" t="s"/>
       <x:c r="D349" s="37" t="n">
         <x:v>1112</x:v>
@@ -6889,7 +6813,7 @@
       </x:c>
     </x:row>
     <x:row r="350" spans="1:10" outlineLevel="2">
-      <x:c r="B350" s="40" t="s"/>
+      <x:c r="B350" s="35" t="s"/>
       <x:c r="C350" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -6906,7 +6830,7 @@
       </x:c>
     </x:row>
     <x:row r="351" spans="1:10" outlineLevel="2">
-      <x:c r="B351" s="40" t="s"/>
+      <x:c r="B351" s="35" t="s"/>
       <x:c r="C351" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -6917,7 +6841,7 @@
       <x:c r="H351" s="34" t="s"/>
     </x:row>
     <x:row r="352" spans="1:10" outlineLevel="3">
-      <x:c r="B352" s="40" t="s"/>
+      <x:c r="B352" s="35" t="s"/>
       <x:c r="C352" s="36" t="s"/>
       <x:c r="D352" s="37" t="n">
         <x:v>1068</x:v>
@@ -6936,7 +6860,7 @@
       </x:c>
     </x:row>
     <x:row r="353" spans="1:10" outlineLevel="2">
-      <x:c r="B353" s="43" t="s"/>
+      <x:c r="B353" s="35" t="s"/>
       <x:c r="C353" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -6981,7 +6905,7 @@
       <x:c r="H355" s="34" t="s"/>
     </x:row>
     <x:row r="356" spans="1:10" outlineLevel="2">
-      <x:c r="B356" s="39" t="s"/>
+      <x:c r="B356" s="35" t="s"/>
       <x:c r="C356" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -6992,8 +6916,8 @@
       <x:c r="H356" s="34" t="s"/>
     </x:row>
     <x:row r="357" spans="1:10" outlineLevel="3">
-      <x:c r="B357" s="40" t="s"/>
-      <x:c r="C357" s="41" t="s"/>
+      <x:c r="B357" s="35" t="s"/>
+      <x:c r="C357" s="36" t="s"/>
       <x:c r="D357" s="37" t="n">
         <x:v>1043</x:v>
       </x:c>
@@ -7011,8 +6935,8 @@
       </x:c>
     </x:row>
     <x:row r="358" spans="1:10" outlineLevel="3">
-      <x:c r="B358" s="40" t="s"/>
-      <x:c r="C358" s="42" t="s"/>
+      <x:c r="B358" s="35" t="s"/>
+      <x:c r="C358" s="36" t="s"/>
       <x:c r="D358" s="37" t="n">
         <x:v>1143</x:v>
       </x:c>
@@ -7030,7 +6954,7 @@
       </x:c>
     </x:row>
     <x:row r="359" spans="1:10" outlineLevel="2">
-      <x:c r="B359" s="43" t="s"/>
+      <x:c r="B359" s="35" t="s"/>
       <x:c r="C359" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -7075,7 +6999,7 @@
       <x:c r="H361" s="34" t="s"/>
     </x:row>
     <x:row r="362" spans="1:10" outlineLevel="2">
-      <x:c r="B362" s="39" t="s"/>
+      <x:c r="B362" s="35" t="s"/>
       <x:c r="C362" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -7086,7 +7010,7 @@
       <x:c r="H362" s="34" t="s"/>
     </x:row>
     <x:row r="363" spans="1:10" outlineLevel="3">
-      <x:c r="B363" s="40" t="s"/>
+      <x:c r="B363" s="35" t="s"/>
       <x:c r="C363" s="36" t="s"/>
       <x:c r="D363" s="37" t="n">
         <x:v>1201</x:v>
@@ -7105,7 +7029,7 @@
       </x:c>
     </x:row>
     <x:row r="364" spans="1:10" outlineLevel="2">
-      <x:c r="B364" s="43" t="s"/>
+      <x:c r="B364" s="35" t="s"/>
       <x:c r="C364" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -7150,7 +7074,7 @@
       <x:c r="H366" s="34" t="s"/>
     </x:row>
     <x:row r="367" spans="1:10" outlineLevel="2">
-      <x:c r="B367" s="39" t="s"/>
+      <x:c r="B367" s="35" t="s"/>
       <x:c r="C367" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -7161,7 +7085,7 @@
       <x:c r="H367" s="34" t="s"/>
     </x:row>
     <x:row r="368" spans="1:10" outlineLevel="3">
-      <x:c r="B368" s="40" t="s"/>
+      <x:c r="B368" s="35" t="s"/>
       <x:c r="C368" s="36" t="s"/>
       <x:c r="D368" s="37" t="n">
         <x:v>1199</x:v>
@@ -7180,7 +7104,7 @@
       </x:c>
     </x:row>
     <x:row r="369" spans="1:10" outlineLevel="2">
-      <x:c r="B369" s="40" t="s"/>
+      <x:c r="B369" s="35" t="s"/>
       <x:c r="C369" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -7197,7 +7121,7 @@
       </x:c>
     </x:row>
     <x:row r="370" spans="1:10" outlineLevel="2">
-      <x:c r="B370" s="40" t="s"/>
+      <x:c r="B370" s="35" t="s"/>
       <x:c r="C370" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -7208,7 +7132,7 @@
       <x:c r="H370" s="34" t="s"/>
     </x:row>
     <x:row r="371" spans="1:10" outlineLevel="3">
-      <x:c r="B371" s="40" t="s"/>
+      <x:c r="B371" s="35" t="s"/>
       <x:c r="C371" s="36" t="s"/>
       <x:c r="D371" s="37" t="n">
         <x:v>1094</x:v>
@@ -7227,7 +7151,7 @@
       </x:c>
     </x:row>
     <x:row r="372" spans="1:10" outlineLevel="2">
-      <x:c r="B372" s="43" t="s"/>
+      <x:c r="B372" s="35" t="s"/>
       <x:c r="C372" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -7272,7 +7196,7 @@
       <x:c r="H374" s="34" t="s"/>
     </x:row>
     <x:row r="375" spans="1:10" outlineLevel="2">
-      <x:c r="B375" s="39" t="s"/>
+      <x:c r="B375" s="35" t="s"/>
       <x:c r="C375" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -7283,7 +7207,7 @@
       <x:c r="H375" s="34" t="s"/>
     </x:row>
     <x:row r="376" spans="1:10" outlineLevel="3">
-      <x:c r="B376" s="40" t="s"/>
+      <x:c r="B376" s="35" t="s"/>
       <x:c r="C376" s="36" t="s"/>
       <x:c r="D376" s="37" t="n">
         <x:v>1175</x:v>
@@ -7302,7 +7226,7 @@
       </x:c>
     </x:row>
     <x:row r="377" spans="1:10" outlineLevel="2">
-      <x:c r="B377" s="43" t="s"/>
+      <x:c r="B377" s="35" t="s"/>
       <x:c r="C377" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -7347,7 +7271,7 @@
       <x:c r="H379" s="34" t="s"/>
     </x:row>
     <x:row r="380" spans="1:10" outlineLevel="2">
-      <x:c r="B380" s="39" t="s"/>
+      <x:c r="B380" s="35" t="s"/>
       <x:c r="C380" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -7358,8 +7282,8 @@
       <x:c r="H380" s="34" t="s"/>
     </x:row>
     <x:row r="381" spans="1:10" outlineLevel="3">
-      <x:c r="B381" s="40" t="s"/>
-      <x:c r="C381" s="41" t="s"/>
+      <x:c r="B381" s="35" t="s"/>
+      <x:c r="C381" s="36" t="s"/>
       <x:c r="D381" s="37" t="n">
         <x:v>1132</x:v>
       </x:c>
@@ -7377,8 +7301,8 @@
       </x:c>
     </x:row>
     <x:row r="382" spans="1:10" outlineLevel="3">
-      <x:c r="B382" s="40" t="s"/>
-      <x:c r="C382" s="44" t="s"/>
+      <x:c r="B382" s="35" t="s"/>
+      <x:c r="C382" s="36" t="s"/>
       <x:c r="D382" s="37" t="n">
         <x:v>1221</x:v>
       </x:c>
@@ -7396,8 +7320,8 @@
       </x:c>
     </x:row>
     <x:row r="383" spans="1:10" outlineLevel="3">
-      <x:c r="B383" s="40" t="s"/>
-      <x:c r="C383" s="44" t="s"/>
+      <x:c r="B383" s="35" t="s"/>
+      <x:c r="C383" s="36" t="s"/>
       <x:c r="D383" s="37" t="n">
         <x:v>1136</x:v>
       </x:c>
@@ -7415,8 +7339,8 @@
       </x:c>
     </x:row>
     <x:row r="384" spans="1:10" outlineLevel="3">
-      <x:c r="B384" s="40" t="s"/>
-      <x:c r="C384" s="44" t="s"/>
+      <x:c r="B384" s="35" t="s"/>
+      <x:c r="C384" s="36" t="s"/>
       <x:c r="D384" s="37" t="n">
         <x:v>1021</x:v>
       </x:c>
@@ -7434,8 +7358,8 @@
       </x:c>
     </x:row>
     <x:row r="385" spans="1:10" outlineLevel="3">
-      <x:c r="B385" s="40" t="s"/>
-      <x:c r="C385" s="44" t="s"/>
+      <x:c r="B385" s="35" t="s"/>
+      <x:c r="C385" s="36" t="s"/>
       <x:c r="D385" s="37" t="n">
         <x:v>1032</x:v>
       </x:c>
@@ -7453,8 +7377,8 @@
       </x:c>
     </x:row>
     <x:row r="386" spans="1:10" outlineLevel="3">
-      <x:c r="B386" s="40" t="s"/>
-      <x:c r="C386" s="44" t="s"/>
+      <x:c r="B386" s="35" t="s"/>
+      <x:c r="C386" s="36" t="s"/>
       <x:c r="D386" s="37" t="n">
         <x:v>1122</x:v>
       </x:c>
@@ -7472,8 +7396,8 @@
       </x:c>
     </x:row>
     <x:row r="387" spans="1:10" outlineLevel="3">
-      <x:c r="B387" s="40" t="s"/>
-      <x:c r="C387" s="44" t="s"/>
+      <x:c r="B387" s="35" t="s"/>
+      <x:c r="C387" s="36" t="s"/>
       <x:c r="D387" s="37" t="n">
         <x:v>1121</x:v>
       </x:c>
@@ -7491,8 +7415,8 @@
       </x:c>
     </x:row>
     <x:row r="388" spans="1:10" outlineLevel="3">
-      <x:c r="B388" s="40" t="s"/>
-      <x:c r="C388" s="42" t="s"/>
+      <x:c r="B388" s="35" t="s"/>
+      <x:c r="C388" s="36" t="s"/>
       <x:c r="D388" s="37" t="n">
         <x:v>1022</x:v>
       </x:c>
@@ -7510,7 +7434,7 @@
       </x:c>
     </x:row>
     <x:row r="389" spans="1:10" outlineLevel="2">
-      <x:c r="B389" s="43" t="s"/>
+      <x:c r="B389" s="35" t="s"/>
       <x:c r="C389" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -7555,7 +7479,7 @@
       <x:c r="H391" s="34" t="s"/>
     </x:row>
     <x:row r="392" spans="1:10" outlineLevel="2">
-      <x:c r="B392" s="39" t="s"/>
+      <x:c r="B392" s="35" t="s"/>
       <x:c r="C392" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -7566,8 +7490,8 @@
       <x:c r="H392" s="34" t="s"/>
     </x:row>
     <x:row r="393" spans="1:10" outlineLevel="3">
-      <x:c r="B393" s="40" t="s"/>
-      <x:c r="C393" s="41" t="s"/>
+      <x:c r="B393" s="35" t="s"/>
+      <x:c r="C393" s="36" t="s"/>
       <x:c r="D393" s="37" t="n">
         <x:v>1101</x:v>
       </x:c>
@@ -7585,8 +7509,8 @@
       </x:c>
     </x:row>
     <x:row r="394" spans="1:10" outlineLevel="3">
-      <x:c r="B394" s="40" t="s"/>
-      <x:c r="C394" s="42" t="s"/>
+      <x:c r="B394" s="35" t="s"/>
+      <x:c r="C394" s="36" t="s"/>
       <x:c r="D394" s="37" t="n">
         <x:v>1051</x:v>
       </x:c>
@@ -7604,7 +7528,7 @@
       </x:c>
     </x:row>
     <x:row r="395" spans="1:10" outlineLevel="2">
-      <x:c r="B395" s="43" t="s"/>
+      <x:c r="B395" s="35" t="s"/>
       <x:c r="C395" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -7649,7 +7573,7 @@
       <x:c r="H397" s="34" t="s"/>
     </x:row>
     <x:row r="398" spans="1:10" outlineLevel="2">
-      <x:c r="B398" s="39" t="s"/>
+      <x:c r="B398" s="35" t="s"/>
       <x:c r="C398" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -7660,8 +7584,8 @@
       <x:c r="H398" s="34" t="s"/>
     </x:row>
     <x:row r="399" spans="1:10" outlineLevel="3">
-      <x:c r="B399" s="40" t="s"/>
-      <x:c r="C399" s="41" t="s"/>
+      <x:c r="B399" s="35" t="s"/>
+      <x:c r="C399" s="36" t="s"/>
       <x:c r="D399" s="37" t="n">
         <x:v>1052</x:v>
       </x:c>
@@ -7679,8 +7603,8 @@
       </x:c>
     </x:row>
     <x:row r="400" spans="1:10" outlineLevel="3">
-      <x:c r="B400" s="40" t="s"/>
-      <x:c r="C400" s="44" t="s"/>
+      <x:c r="B400" s="35" t="s"/>
+      <x:c r="C400" s="36" t="s"/>
       <x:c r="D400" s="37" t="n">
         <x:v>1155</x:v>
       </x:c>
@@ -7698,8 +7622,8 @@
       </x:c>
     </x:row>
     <x:row r="401" spans="1:10" outlineLevel="3">
-      <x:c r="B401" s="40" t="s"/>
-      <x:c r="C401" s="44" t="s"/>
+      <x:c r="B401" s="35" t="s"/>
+      <x:c r="C401" s="36" t="s"/>
       <x:c r="D401" s="37" t="n">
         <x:v>1152</x:v>
       </x:c>
@@ -7717,8 +7641,8 @@
       </x:c>
     </x:row>
     <x:row r="402" spans="1:10" outlineLevel="3">
-      <x:c r="B402" s="40" t="s"/>
-      <x:c r="C402" s="44" t="s"/>
+      <x:c r="B402" s="35" t="s"/>
+      <x:c r="C402" s="36" t="s"/>
       <x:c r="D402" s="37" t="n">
         <x:v>1163</x:v>
       </x:c>
@@ -7736,8 +7660,8 @@
       </x:c>
     </x:row>
     <x:row r="403" spans="1:10" outlineLevel="3">
-      <x:c r="B403" s="40" t="s"/>
-      <x:c r="C403" s="44" t="s"/>
+      <x:c r="B403" s="35" t="s"/>
+      <x:c r="C403" s="36" t="s"/>
       <x:c r="D403" s="37" t="n">
         <x:v>1087</x:v>
       </x:c>
@@ -7755,8 +7679,8 @@
       </x:c>
     </x:row>
     <x:row r="404" spans="1:10" outlineLevel="3">
-      <x:c r="B404" s="40" t="s"/>
-      <x:c r="C404" s="44" t="s"/>
+      <x:c r="B404" s="35" t="s"/>
+      <x:c r="C404" s="36" t="s"/>
       <x:c r="D404" s="37" t="n">
         <x:v>1055</x:v>
       </x:c>
@@ -7774,8 +7698,8 @@
       </x:c>
     </x:row>
     <x:row r="405" spans="1:10" outlineLevel="3">
-      <x:c r="B405" s="40" t="s"/>
-      <x:c r="C405" s="44" t="s"/>
+      <x:c r="B405" s="35" t="s"/>
+      <x:c r="C405" s="36" t="s"/>
       <x:c r="D405" s="37" t="n">
         <x:v>1003</x:v>
       </x:c>
@@ -7793,8 +7717,8 @@
       </x:c>
     </x:row>
     <x:row r="406" spans="1:10" outlineLevel="3">
-      <x:c r="B406" s="40" t="s"/>
-      <x:c r="C406" s="42" t="s"/>
+      <x:c r="B406" s="35" t="s"/>
+      <x:c r="C406" s="36" t="s"/>
       <x:c r="D406" s="37" t="n">
         <x:v>1255</x:v>
       </x:c>
@@ -7812,7 +7736,7 @@
       </x:c>
     </x:row>
     <x:row r="407" spans="1:10" outlineLevel="2">
-      <x:c r="B407" s="40" t="s"/>
+      <x:c r="B407" s="35" t="s"/>
       <x:c r="C407" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -7829,7 +7753,7 @@
       </x:c>
     </x:row>
     <x:row r="408" spans="1:10" outlineLevel="2">
-      <x:c r="B408" s="40" t="s"/>
+      <x:c r="B408" s="35" t="s"/>
       <x:c r="C408" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -7840,8 +7764,8 @@
       <x:c r="H408" s="34" t="s"/>
     </x:row>
     <x:row r="409" spans="1:10" outlineLevel="3">
-      <x:c r="B409" s="40" t="s"/>
-      <x:c r="C409" s="41" t="s"/>
+      <x:c r="B409" s="35" t="s"/>
+      <x:c r="C409" s="36" t="s"/>
       <x:c r="D409" s="37" t="n">
         <x:v>1275</x:v>
       </x:c>
@@ -7859,8 +7783,8 @@
       </x:c>
     </x:row>
     <x:row r="410" spans="1:10" outlineLevel="3">
-      <x:c r="B410" s="40" t="s"/>
-      <x:c r="C410" s="42" t="s"/>
+      <x:c r="B410" s="35" t="s"/>
+      <x:c r="C410" s="36" t="s"/>
       <x:c r="D410" s="37" t="n">
         <x:v>1075</x:v>
       </x:c>
@@ -7878,7 +7802,7 @@
       </x:c>
     </x:row>
     <x:row r="411" spans="1:10" outlineLevel="2">
-      <x:c r="B411" s="40" t="s"/>
+      <x:c r="B411" s="35" t="s"/>
       <x:c r="C411" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -7895,7 +7819,7 @@
       </x:c>
     </x:row>
     <x:row r="412" spans="1:10" outlineLevel="2">
-      <x:c r="B412" s="40" t="s"/>
+      <x:c r="B412" s="35" t="s"/>
       <x:c r="C412" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -7906,7 +7830,7 @@
       <x:c r="H412" s="34" t="s"/>
     </x:row>
     <x:row r="413" spans="1:10" outlineLevel="3">
-      <x:c r="B413" s="40" t="s"/>
+      <x:c r="B413" s="35" t="s"/>
       <x:c r="C413" s="36" t="s"/>
       <x:c r="D413" s="37" t="n">
         <x:v>1067</x:v>
@@ -7925,7 +7849,7 @@
       </x:c>
     </x:row>
     <x:row r="414" spans="1:10" outlineLevel="2">
-      <x:c r="B414" s="43" t="s"/>
+      <x:c r="B414" s="35" t="s"/>
       <x:c r="C414" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -7970,7 +7894,7 @@
       <x:c r="H416" s="34" t="s"/>
     </x:row>
     <x:row r="417" spans="1:10" outlineLevel="2">
-      <x:c r="B417" s="39" t="s"/>
+      <x:c r="B417" s="35" t="s"/>
       <x:c r="C417" s="29" t="s">
         <x:v>34</x:v>
       </x:c>
@@ -7981,8 +7905,8 @@
       <x:c r="H417" s="34" t="s"/>
     </x:row>
     <x:row r="418" spans="1:10" outlineLevel="3">
-      <x:c r="B418" s="40" t="s"/>
-      <x:c r="C418" s="41" t="s"/>
+      <x:c r="B418" s="35" t="s"/>
+      <x:c r="C418" s="36" t="s"/>
       <x:c r="D418" s="37" t="n">
         <x:v>1171</x:v>
       </x:c>
@@ -8000,8 +7924,8 @@
       </x:c>
     </x:row>
     <x:row r="419" spans="1:10" outlineLevel="3">
-      <x:c r="B419" s="40" t="s"/>
-      <x:c r="C419" s="44" t="s"/>
+      <x:c r="B419" s="35" t="s"/>
+      <x:c r="C419" s="36" t="s"/>
       <x:c r="D419" s="37" t="n">
         <x:v>1271</x:v>
       </x:c>
@@ -8019,8 +7943,8 @@
       </x:c>
     </x:row>
     <x:row r="420" spans="1:10" outlineLevel="3">
-      <x:c r="B420" s="40" t="s"/>
-      <x:c r="C420" s="42" t="s"/>
+      <x:c r="B420" s="35" t="s"/>
+      <x:c r="C420" s="36" t="s"/>
       <x:c r="D420" s="37" t="n">
         <x:v>1071</x:v>
       </x:c>
@@ -8038,7 +7962,7 @@
       </x:c>
     </x:row>
     <x:row r="421" spans="1:10" outlineLevel="2">
-      <x:c r="B421" s="40" t="s"/>
+      <x:c r="B421" s="35" t="s"/>
       <x:c r="C421" s="29" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -8055,7 +7979,7 @@
       </x:c>
     </x:row>
     <x:row r="422" spans="1:10" outlineLevel="2">
-      <x:c r="B422" s="40" t="s"/>
+      <x:c r="B422" s="35" t="s"/>
       <x:c r="C422" s="29" t="s">
         <x:v>56</x:v>
       </x:c>
@@ -8066,8 +7990,8 @@
       <x:c r="H422" s="34" t="s"/>
     </x:row>
     <x:row r="423" spans="1:10" outlineLevel="3">
-      <x:c r="B423" s="40" t="s"/>
-      <x:c r="C423" s="41" t="s"/>
+      <x:c r="B423" s="35" t="s"/>
+      <x:c r="C423" s="36" t="s"/>
       <x:c r="D423" s="37" t="n">
         <x:v>1011</x:v>
       </x:c>
@@ -8085,8 +8009,8 @@
       </x:c>
     </x:row>
     <x:row r="424" spans="1:10" outlineLevel="3">
-      <x:c r="B424" s="40" t="s"/>
-      <x:c r="C424" s="42" t="s"/>
+      <x:c r="B424" s="35" t="s"/>
+      <x:c r="C424" s="36" t="s"/>
       <x:c r="D424" s="37" t="n">
         <x:v>1111</x:v>
       </x:c>
@@ -8104,7 +8028,7 @@
       </x:c>
     </x:row>
     <x:row r="425" spans="1:10" outlineLevel="2">
-      <x:c r="B425" s="40" t="s"/>
+      <x:c r="B425" s="35" t="s"/>
       <x:c r="C425" s="29" t="s">
         <x:v>57</x:v>
       </x:c>
@@ -8121,7 +8045,7 @@
       </x:c>
     </x:row>
     <x:row r="426" spans="1:10" outlineLevel="2">
-      <x:c r="B426" s="40" t="s"/>
+      <x:c r="B426" s="35" t="s"/>
       <x:c r="C426" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -8132,7 +8056,7 @@
       <x:c r="H426" s="34" t="s"/>
     </x:row>
     <x:row r="427" spans="1:10" outlineLevel="3">
-      <x:c r="B427" s="40" t="s"/>
+      <x:c r="B427" s="35" t="s"/>
       <x:c r="C427" s="36" t="s"/>
       <x:c r="D427" s="37" t="n">
         <x:v>1035</x:v>
@@ -8151,7 +8075,7 @@
       </x:c>
     </x:row>
     <x:row r="428" spans="1:10" outlineLevel="2">
-      <x:c r="B428" s="40" t="s"/>
+      <x:c r="B428" s="35" t="s"/>
       <x:c r="C428" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -8168,7 +8092,7 @@
       </x:c>
     </x:row>
     <x:row r="429" spans="1:10" outlineLevel="2">
-      <x:c r="B429" s="40" t="s"/>
+      <x:c r="B429" s="35" t="s"/>
       <x:c r="C429" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -8179,7 +8103,7 @@
       <x:c r="H429" s="34" t="s"/>
     </x:row>
     <x:row r="430" spans="1:10" outlineLevel="3">
-      <x:c r="B430" s="40" t="s"/>
+      <x:c r="B430" s="35" t="s"/>
       <x:c r="C430" s="36" t="s"/>
       <x:c r="D430" s="37" t="n">
         <x:v>1154</x:v>
@@ -8198,7 +8122,7 @@
       </x:c>
     </x:row>
     <x:row r="431" spans="1:10" outlineLevel="2">
-      <x:c r="B431" s="43" t="s"/>
+      <x:c r="B431" s="35" t="s"/>
       <x:c r="C431" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -8243,7 +8167,7 @@
       <x:c r="H433" s="34" t="s"/>
     </x:row>
     <x:row r="434" spans="1:10" outlineLevel="2">
-      <x:c r="B434" s="39" t="s"/>
+      <x:c r="B434" s="35" t="s"/>
       <x:c r="C434" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -8254,7 +8178,7 @@
       <x:c r="H434" s="34" t="s"/>
     </x:row>
     <x:row r="435" spans="1:10" outlineLevel="3">
-      <x:c r="B435" s="40" t="s"/>
+      <x:c r="B435" s="35" t="s"/>
       <x:c r="C435" s="36" t="s"/>
       <x:c r="D435" s="37" t="n">
         <x:v>1053</x:v>
@@ -8273,7 +8197,7 @@
       </x:c>
     </x:row>
     <x:row r="436" spans="1:10" outlineLevel="2">
-      <x:c r="B436" s="43" t="s"/>
+      <x:c r="B436" s="35" t="s"/>
       <x:c r="C436" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -8318,7 +8242,7 @@
       <x:c r="H438" s="34" t="s"/>
     </x:row>
     <x:row r="439" spans="1:10" outlineLevel="2">
-      <x:c r="B439" s="39" t="s"/>
+      <x:c r="B439" s="35" t="s"/>
       <x:c r="C439" s="29" t="s">
         <x:v>34</x:v>
       </x:c>
@@ -8329,8 +8253,8 @@
       <x:c r="H439" s="34" t="s"/>
     </x:row>
     <x:row r="440" spans="1:10" outlineLevel="3">
-      <x:c r="B440" s="40" t="s"/>
-      <x:c r="C440" s="41" t="s"/>
+      <x:c r="B440" s="35" t="s"/>
+      <x:c r="C440" s="36" t="s"/>
       <x:c r="D440" s="37" t="n">
         <x:v>1059</x:v>
       </x:c>
@@ -8348,8 +8272,8 @@
       </x:c>
     </x:row>
     <x:row r="441" spans="1:10" outlineLevel="3">
-      <x:c r="B441" s="40" t="s"/>
-      <x:c r="C441" s="42" t="s"/>
+      <x:c r="B441" s="35" t="s"/>
+      <x:c r="C441" s="36" t="s"/>
       <x:c r="D441" s="37" t="n">
         <x:v>1072</x:v>
       </x:c>
@@ -8367,7 +8291,7 @@
       </x:c>
     </x:row>
     <x:row r="442" spans="1:10" outlineLevel="2">
-      <x:c r="B442" s="40" t="s"/>
+      <x:c r="B442" s="35" t="s"/>
       <x:c r="C442" s="29" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -8384,7 +8308,7 @@
       </x:c>
     </x:row>
     <x:row r="443" spans="1:10" outlineLevel="2">
-      <x:c r="B443" s="40" t="s"/>
+      <x:c r="B443" s="35" t="s"/>
       <x:c r="C443" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -8395,8 +8319,8 @@
       <x:c r="H443" s="34" t="s"/>
     </x:row>
     <x:row r="444" spans="1:10" outlineLevel="3">
-      <x:c r="B444" s="40" t="s"/>
-      <x:c r="C444" s="41" t="s"/>
+      <x:c r="B444" s="35" t="s"/>
+      <x:c r="C444" s="36" t="s"/>
       <x:c r="D444" s="37" t="n">
         <x:v>1280</x:v>
       </x:c>
@@ -8414,8 +8338,8 @@
       </x:c>
     </x:row>
     <x:row r="445" spans="1:10" outlineLevel="3">
-      <x:c r="B445" s="40" t="s"/>
-      <x:c r="C445" s="44" t="s"/>
+      <x:c r="B445" s="35" t="s"/>
+      <x:c r="C445" s="36" t="s"/>
       <x:c r="D445" s="37" t="n">
         <x:v>1080</x:v>
       </x:c>
@@ -8433,8 +8357,8 @@
       </x:c>
     </x:row>
     <x:row r="446" spans="1:10" outlineLevel="3">
-      <x:c r="B446" s="40" t="s"/>
-      <x:c r="C446" s="42" t="s"/>
+      <x:c r="B446" s="35" t="s"/>
+      <x:c r="C446" s="36" t="s"/>
       <x:c r="D446" s="37" t="n">
         <x:v>1180</x:v>
       </x:c>
@@ -8452,7 +8376,7 @@
       </x:c>
     </x:row>
     <x:row r="447" spans="1:10" outlineLevel="2">
-      <x:c r="B447" s="40" t="s"/>
+      <x:c r="B447" s="35" t="s"/>
       <x:c r="C447" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -8469,7 +8393,7 @@
       </x:c>
     </x:row>
     <x:row r="448" spans="1:10" outlineLevel="2">
-      <x:c r="B448" s="40" t="s"/>
+      <x:c r="B448" s="35" t="s"/>
       <x:c r="C448" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -8480,8 +8404,8 @@
       <x:c r="H448" s="34" t="s"/>
     </x:row>
     <x:row r="449" spans="1:10" outlineLevel="3">
-      <x:c r="B449" s="40" t="s"/>
-      <x:c r="C449" s="41" t="s"/>
+      <x:c r="B449" s="35" t="s"/>
+      <x:c r="C449" s="36" t="s"/>
       <x:c r="D449" s="37" t="n">
         <x:v>1105</x:v>
       </x:c>
@@ -8499,8 +8423,8 @@
       </x:c>
     </x:row>
     <x:row r="450" spans="1:10" outlineLevel="3">
-      <x:c r="B450" s="40" t="s"/>
-      <x:c r="C450" s="44" t="s"/>
+      <x:c r="B450" s="35" t="s"/>
+      <x:c r="C450" s="36" t="s"/>
       <x:c r="D450" s="37" t="n">
         <x:v>1005</x:v>
       </x:c>
@@ -8518,8 +8442,8 @@
       </x:c>
     </x:row>
     <x:row r="451" spans="1:10" outlineLevel="3">
-      <x:c r="B451" s="40" t="s"/>
-      <x:c r="C451" s="44" t="s"/>
+      <x:c r="B451" s="35" t="s"/>
+      <x:c r="C451" s="36" t="s"/>
       <x:c r="D451" s="37" t="n">
         <x:v>1305</x:v>
       </x:c>
@@ -8537,8 +8461,8 @@
       </x:c>
     </x:row>
     <x:row r="452" spans="1:10" outlineLevel="3">
-      <x:c r="B452" s="40" t="s"/>
-      <x:c r="C452" s="42" t="s"/>
+      <x:c r="B452" s="35" t="s"/>
+      <x:c r="C452" s="36" t="s"/>
       <x:c r="D452" s="37" t="n">
         <x:v>1266</x:v>
       </x:c>
@@ -8556,7 +8480,7 @@
       </x:c>
     </x:row>
     <x:row r="453" spans="1:10" outlineLevel="2">
-      <x:c r="B453" s="43" t="s"/>
+      <x:c r="B453" s="35" t="s"/>
       <x:c r="C453" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -8601,7 +8525,7 @@
       <x:c r="H455" s="34" t="s"/>
     </x:row>
     <x:row r="456" spans="1:10" outlineLevel="2">
-      <x:c r="B456" s="39" t="s"/>
+      <x:c r="B456" s="35" t="s"/>
       <x:c r="C456" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -8612,8 +8536,8 @@
       <x:c r="H456" s="34" t="s"/>
     </x:row>
     <x:row r="457" spans="1:10" outlineLevel="3">
-      <x:c r="B457" s="40" t="s"/>
-      <x:c r="C457" s="41" t="s"/>
+      <x:c r="B457" s="35" t="s"/>
+      <x:c r="C457" s="36" t="s"/>
       <x:c r="D457" s="37" t="n">
         <x:v>1119</x:v>
       </x:c>
@@ -8631,8 +8555,8 @@
       </x:c>
     </x:row>
     <x:row r="458" spans="1:10" outlineLevel="3">
-      <x:c r="B458" s="40" t="s"/>
-      <x:c r="C458" s="42" t="s"/>
+      <x:c r="B458" s="35" t="s"/>
+      <x:c r="C458" s="36" t="s"/>
       <x:c r="D458" s="37" t="n">
         <x:v>1036</x:v>
       </x:c>
@@ -8650,7 +8574,7 @@
       </x:c>
     </x:row>
     <x:row r="459" spans="1:10" outlineLevel="2">
-      <x:c r="B459" s="40" t="s"/>
+      <x:c r="B459" s="35" t="s"/>
       <x:c r="C459" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -8667,7 +8591,7 @@
       </x:c>
     </x:row>
     <x:row r="460" spans="1:10" outlineLevel="2">
-      <x:c r="B460" s="40" t="s"/>
+      <x:c r="B460" s="35" t="s"/>
       <x:c r="C460" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -8678,7 +8602,7 @@
       <x:c r="H460" s="34" t="s"/>
     </x:row>
     <x:row r="461" spans="1:10" outlineLevel="3">
-      <x:c r="B461" s="40" t="s"/>
+      <x:c r="B461" s="35" t="s"/>
       <x:c r="C461" s="36" t="s"/>
       <x:c r="D461" s="37" t="n">
         <x:v>1195</x:v>
@@ -8697,7 +8621,7 @@
       </x:c>
     </x:row>
     <x:row r="462" spans="1:10" outlineLevel="2">
-      <x:c r="B462" s="43" t="s"/>
+      <x:c r="B462" s="35" t="s"/>
       <x:c r="C462" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -8742,7 +8666,7 @@
       <x:c r="H464" s="34" t="s"/>
     </x:row>
     <x:row r="465" spans="1:10" outlineLevel="2">
-      <x:c r="B465" s="39" t="s"/>
+      <x:c r="B465" s="35" t="s"/>
       <x:c r="C465" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -8753,7 +8677,7 @@
       <x:c r="H465" s="34" t="s"/>
     </x:row>
     <x:row r="466" spans="1:10" outlineLevel="3">
-      <x:c r="B466" s="40" t="s"/>
+      <x:c r="B466" s="35" t="s"/>
       <x:c r="C466" s="36" t="s"/>
       <x:c r="D466" s="37" t="n">
         <x:v>1115</x:v>
@@ -8772,7 +8696,7 @@
       </x:c>
     </x:row>
     <x:row r="467" spans="1:10" outlineLevel="2">
-      <x:c r="B467" s="43" t="s"/>
+      <x:c r="B467" s="35" t="s"/>
       <x:c r="C467" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -8817,7 +8741,7 @@
       <x:c r="H469" s="34" t="s"/>
     </x:row>
     <x:row r="470" spans="1:10" outlineLevel="2">
-      <x:c r="B470" s="39" t="s"/>
+      <x:c r="B470" s="35" t="s"/>
       <x:c r="C470" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -8828,7 +8752,7 @@
       <x:c r="H470" s="34" t="s"/>
     </x:row>
     <x:row r="471" spans="1:10" outlineLevel="3">
-      <x:c r="B471" s="40" t="s"/>
+      <x:c r="B471" s="35" t="s"/>
       <x:c r="C471" s="36" t="s"/>
       <x:c r="D471" s="37" t="n">
         <x:v>1070</x:v>
@@ -8847,7 +8771,7 @@
       </x:c>
     </x:row>
     <x:row r="472" spans="1:10" outlineLevel="2">
-      <x:c r="B472" s="43" t="s"/>
+      <x:c r="B472" s="35" t="s"/>
       <x:c r="C472" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -8892,7 +8816,7 @@
       <x:c r="H474" s="34" t="s"/>
     </x:row>
     <x:row r="475" spans="1:10" outlineLevel="2">
-      <x:c r="B475" s="39" t="s"/>
+      <x:c r="B475" s="35" t="s"/>
       <x:c r="C475" s="29" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -8903,8 +8827,8 @@
       <x:c r="H475" s="34" t="s"/>
     </x:row>
     <x:row r="476" spans="1:10" outlineLevel="3">
-      <x:c r="B476" s="40" t="s"/>
-      <x:c r="C476" s="41" t="s"/>
+      <x:c r="B476" s="35" t="s"/>
+      <x:c r="C476" s="36" t="s"/>
       <x:c r="D476" s="37" t="n">
         <x:v>1250</x:v>
       </x:c>
@@ -8922,8 +8846,8 @@
       </x:c>
     </x:row>
     <x:row r="477" spans="1:10" outlineLevel="3">
-      <x:c r="B477" s="40" t="s"/>
-      <x:c r="C477" s="44" t="s"/>
+      <x:c r="B477" s="35" t="s"/>
+      <x:c r="C477" s="36" t="s"/>
       <x:c r="D477" s="37" t="n">
         <x:v>1350</x:v>
       </x:c>
@@ -8941,8 +8865,8 @@
       </x:c>
     </x:row>
     <x:row r="478" spans="1:10" outlineLevel="3">
-      <x:c r="B478" s="40" t="s"/>
-      <x:c r="C478" s="44" t="s"/>
+      <x:c r="B478" s="35" t="s"/>
+      <x:c r="C478" s="36" t="s"/>
       <x:c r="D478" s="37" t="n">
         <x:v>1050</x:v>
       </x:c>
@@ -8960,8 +8884,8 @@
       </x:c>
     </x:row>
     <x:row r="479" spans="1:10" outlineLevel="3">
-      <x:c r="B479" s="40" t="s"/>
-      <x:c r="C479" s="42" t="s"/>
+      <x:c r="B479" s="35" t="s"/>
+      <x:c r="C479" s="36" t="s"/>
       <x:c r="D479" s="37" t="n">
         <x:v>1150</x:v>
       </x:c>
@@ -8979,7 +8903,7 @@
       </x:c>
     </x:row>
     <x:row r="480" spans="1:10" outlineLevel="2">
-      <x:c r="B480" s="43" t="s"/>
+      <x:c r="B480" s="35" t="s"/>
       <x:c r="C480" s="29" t="s">
         <x:v>29</x:v>
       </x:c>
@@ -9024,7 +8948,7 @@
       <x:c r="H482" s="34" t="s"/>
     </x:row>
     <x:row r="483" spans="1:10" outlineLevel="2">
-      <x:c r="B483" s="39" t="s"/>
+      <x:c r="B483" s="35" t="s"/>
       <x:c r="C483" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -9035,8 +8959,8 @@
       <x:c r="H483" s="34" t="s"/>
     </x:row>
     <x:row r="484" spans="1:10" outlineLevel="3">
-      <x:c r="B484" s="40" t="s"/>
-      <x:c r="C484" s="41" t="s"/>
+      <x:c r="B484" s="35" t="s"/>
+      <x:c r="C484" s="36" t="s"/>
       <x:c r="D484" s="37" t="n">
         <x:v>1060</x:v>
       </x:c>
@@ -9054,8 +8978,8 @@
       </x:c>
     </x:row>
     <x:row r="485" spans="1:10" outlineLevel="3">
-      <x:c r="B485" s="40" t="s"/>
-      <x:c r="C485" s="42" t="s"/>
+      <x:c r="B485" s="35" t="s"/>
+      <x:c r="C485" s="36" t="s"/>
       <x:c r="D485" s="37" t="n">
         <x:v>1160</x:v>
       </x:c>
@@ -9073,7 +8997,7 @@
       </x:c>
     </x:row>
     <x:row r="486" spans="1:10" outlineLevel="2">
-      <x:c r="B486" s="40" t="s"/>
+      <x:c r="B486" s="35" t="s"/>
       <x:c r="C486" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -9090,7 +9014,7 @@
       </x:c>
     </x:row>
     <x:row r="487" spans="1:10" outlineLevel="2">
-      <x:c r="B487" s="40" t="s"/>
+      <x:c r="B487" s="35" t="s"/>
       <x:c r="C487" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -9101,8 +9025,8 @@
       <x:c r="H487" s="34" t="s"/>
     </x:row>
     <x:row r="488" spans="1:10" outlineLevel="3">
-      <x:c r="B488" s="40" t="s"/>
-      <x:c r="C488" s="41" t="s"/>
+      <x:c r="B488" s="35" t="s"/>
+      <x:c r="C488" s="36" t="s"/>
       <x:c r="D488" s="37" t="n">
         <x:v>1202</x:v>
       </x:c>
@@ -9120,8 +9044,8 @@
       </x:c>
     </x:row>
     <x:row r="489" spans="1:10" outlineLevel="3">
-      <x:c r="B489" s="40" t="s"/>
-      <x:c r="C489" s="44" t="s"/>
+      <x:c r="B489" s="35" t="s"/>
+      <x:c r="C489" s="36" t="s"/>
       <x:c r="D489" s="37" t="n">
         <x:v>1178</x:v>
       </x:c>
@@ -9139,8 +9063,8 @@
       </x:c>
     </x:row>
     <x:row r="490" spans="1:10" outlineLevel="3">
-      <x:c r="B490" s="40" t="s"/>
-      <x:c r="C490" s="44" t="s"/>
+      <x:c r="B490" s="35" t="s"/>
+      <x:c r="C490" s="36" t="s"/>
       <x:c r="D490" s="37" t="n">
         <x:v>1302</x:v>
       </x:c>
@@ -9158,8 +9082,8 @@
       </x:c>
     </x:row>
     <x:row r="491" spans="1:10" outlineLevel="3">
-      <x:c r="B491" s="40" t="s"/>
-      <x:c r="C491" s="44" t="s"/>
+      <x:c r="B491" s="35" t="s"/>
+      <x:c r="C491" s="36" t="s"/>
       <x:c r="D491" s="37" t="n">
         <x:v>1278</x:v>
       </x:c>
@@ -9177,8 +9101,8 @@
       </x:c>
     </x:row>
     <x:row r="492" spans="1:10" outlineLevel="3">
-      <x:c r="B492" s="40" t="s"/>
-      <x:c r="C492" s="42" t="s"/>
+      <x:c r="B492" s="35" t="s"/>
+      <x:c r="C492" s="36" t="s"/>
       <x:c r="D492" s="37" t="n">
         <x:v>1102</x:v>
       </x:c>
@@ -9196,7 +9120,7 @@
       </x:c>
     </x:row>
     <x:row r="493" spans="1:10" outlineLevel="2">
-      <x:c r="B493" s="40" t="s"/>
+      <x:c r="B493" s="35" t="s"/>
       <x:c r="C493" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -9213,7 +9137,7 @@
       </x:c>
     </x:row>
     <x:row r="494" spans="1:10" outlineLevel="2">
-      <x:c r="B494" s="40" t="s"/>
+      <x:c r="B494" s="35" t="s"/>
       <x:c r="C494" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -9224,8 +9148,8 @@
       <x:c r="H494" s="34" t="s"/>
     </x:row>
     <x:row r="495" spans="1:10" outlineLevel="3">
-      <x:c r="B495" s="40" t="s"/>
-      <x:c r="C495" s="41" t="s"/>
+      <x:c r="B495" s="35" t="s"/>
+      <x:c r="C495" s="36" t="s"/>
       <x:c r="D495" s="37" t="n">
         <x:v>1073</x:v>
       </x:c>
@@ -9243,8 +9167,8 @@
       </x:c>
     </x:row>
     <x:row r="496" spans="1:10" outlineLevel="3">
-      <x:c r="B496" s="40" t="s"/>
-      <x:c r="C496" s="42" t="s"/>
+      <x:c r="B496" s="35" t="s"/>
+      <x:c r="C496" s="36" t="s"/>
       <x:c r="D496" s="37" t="n">
         <x:v>1173</x:v>
       </x:c>
@@ -9262,7 +9186,7 @@
       </x:c>
     </x:row>
     <x:row r="497" spans="1:10" outlineLevel="2">
-      <x:c r="B497" s="43" t="s"/>
+      <x:c r="B497" s="35" t="s"/>
       <x:c r="C497" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -9307,7 +9231,7 @@
       <x:c r="H499" s="34" t="s"/>
     </x:row>
     <x:row r="500" spans="1:10" outlineLevel="2">
-      <x:c r="B500" s="39" t="s"/>
+      <x:c r="B500" s="35" t="s"/>
       <x:c r="C500" s="29" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -9318,7 +9242,7 @@
       <x:c r="H500" s="34" t="s"/>
     </x:row>
     <x:row r="501" spans="1:10" outlineLevel="3">
-      <x:c r="B501" s="40" t="s"/>
+      <x:c r="B501" s="35" t="s"/>
       <x:c r="C501" s="36" t="s"/>
       <x:c r="D501" s="37" t="n">
         <x:v>1296</x:v>
@@ -9337,7 +9261,7 @@
       </x:c>
     </x:row>
     <x:row r="502" spans="1:10" outlineLevel="2">
-      <x:c r="B502" s="43" t="s"/>
+      <x:c r="B502" s="35" t="s"/>
       <x:c r="C502" s="29" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -9382,7 +9306,7 @@
       <x:c r="H504" s="34" t="s"/>
     </x:row>
     <x:row r="505" spans="1:10" outlineLevel="2">
-      <x:c r="B505" s="39" t="s"/>
+      <x:c r="B505" s="35" t="s"/>
       <x:c r="C505" s="29" t="s">
         <x:v>34</x:v>
       </x:c>
@@ -9393,7 +9317,7 @@
       <x:c r="H505" s="34" t="s"/>
     </x:row>
     <x:row r="506" spans="1:10" outlineLevel="3">
-      <x:c r="B506" s="40" t="s"/>
+      <x:c r="B506" s="35" t="s"/>
       <x:c r="C506" s="36" t="s"/>
       <x:c r="D506" s="37" t="n">
         <x:v>1033</x:v>
@@ -9412,7 +9336,7 @@
       </x:c>
     </x:row>
     <x:row r="507" spans="1:10" outlineLevel="2">
-      <x:c r="B507" s="40" t="s"/>
+      <x:c r="B507" s="35" t="s"/>
       <x:c r="C507" s="29" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -9429,7 +9353,7 @@
       </x:c>
     </x:row>
     <x:row r="508" spans="1:10" outlineLevel="2">
-      <x:c r="B508" s="40" t="s"/>
+      <x:c r="B508" s="35" t="s"/>
       <x:c r="C508" s="29" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -9440,7 +9364,7 @@
       <x:c r="H508" s="34" t="s"/>
     </x:row>
     <x:row r="509" spans="1:10" outlineLevel="3">
-      <x:c r="B509" s="40" t="s"/>
+      <x:c r="B509" s="35" t="s"/>
       <x:c r="C509" s="36" t="s"/>
       <x:c r="D509" s="37" t="n">
         <x:v>1124</x:v>
@@ -9459,7 +9383,7 @@
       </x:c>
     </x:row>
     <x:row r="510" spans="1:10" outlineLevel="2">
-      <x:c r="B510" s="40" t="s"/>
+      <x:c r="B510" s="35" t="s"/>
       <x:c r="C510" s="29" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -9476,7 +9400,7 @@
       </x:c>
     </x:row>
     <x:row r="511" spans="1:10" outlineLevel="2">
-      <x:c r="B511" s="40" t="s"/>
+      <x:c r="B511" s="35" t="s"/>
       <x:c r="C511" s="29" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -9487,8 +9411,8 @@
       <x:c r="H511" s="34" t="s"/>
     </x:row>
     <x:row r="512" spans="1:10" outlineLevel="3">
-      <x:c r="B512" s="40" t="s"/>
-      <x:c r="C512" s="41" t="s"/>
+      <x:c r="B512" s="35" t="s"/>
+      <x:c r="C512" s="36" t="s"/>
       <x:c r="D512" s="37" t="n">
         <x:v>1200</x:v>
       </x:c>
@@ -9506,8 +9430,8 @@
       </x:c>
     </x:row>
     <x:row r="513" spans="1:10" outlineLevel="3">
-      <x:c r="B513" s="40" t="s"/>
-      <x:c r="C513" s="44" t="s"/>
+      <x:c r="B513" s="35" t="s"/>
+      <x:c r="C513" s="36" t="s"/>
       <x:c r="D513" s="37" t="n">
         <x:v>1300</x:v>
       </x:c>
@@ -9525,8 +9449,8 @@
       </x:c>
     </x:row>
     <x:row r="514" spans="1:10" outlineLevel="3">
-      <x:c r="B514" s="40" t="s"/>
-      <x:c r="C514" s="42" t="s"/>
+      <x:c r="B514" s="35" t="s"/>
+      <x:c r="C514" s="36" t="s"/>
       <x:c r="D514" s="37" t="n">
         <x:v>1100</x:v>
       </x:c>
@@ -9544,7 +9468,7 @@
       </x:c>
     </x:row>
     <x:row r="515" spans="1:10" outlineLevel="2">
-      <x:c r="B515" s="40" t="s"/>
+      <x:c r="B515" s="35" t="s"/>
       <x:c r="C515" s="29" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -9561,7 +9485,7 @@
       </x:c>
     </x:row>
     <x:row r="516" spans="1:10" outlineLevel="2">
-      <x:c r="B516" s="40" t="s"/>
+      <x:c r="B516" s="35" t="s"/>
       <x:c r="C516" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -9572,8 +9496,8 @@
       <x:c r="H516" s="34" t="s"/>
     </x:row>
     <x:row r="517" spans="1:10" outlineLevel="3">
-      <x:c r="B517" s="40" t="s"/>
-      <x:c r="C517" s="41" t="s"/>
+      <x:c r="B517" s="35" t="s"/>
+      <x:c r="C517" s="36" t="s"/>
       <x:c r="D517" s="37" t="n">
         <x:v>1127</x:v>
       </x:c>
@@ -9591,8 +9515,8 @@
       </x:c>
     </x:row>
     <x:row r="518" spans="1:10" outlineLevel="3">
-      <x:c r="B518" s="40" t="s"/>
-      <x:c r="C518" s="44" t="s"/>
+      <x:c r="B518" s="35" t="s"/>
+      <x:c r="C518" s="36" t="s"/>
       <x:c r="D518" s="37" t="n">
         <x:v>1207</x:v>
       </x:c>
@@ -9610,8 +9534,8 @@
       </x:c>
     </x:row>
     <x:row r="519" spans="1:10" outlineLevel="3">
-      <x:c r="B519" s="40" t="s"/>
-      <x:c r="C519" s="44" t="s"/>
+      <x:c r="B519" s="35" t="s"/>
+      <x:c r="C519" s="36" t="s"/>
       <x:c r="D519" s="37" t="n">
         <x:v>1027</x:v>
       </x:c>
@@ -9629,8 +9553,8 @@
       </x:c>
     </x:row>
     <x:row r="520" spans="1:10" outlineLevel="3">
-      <x:c r="B520" s="40" t="s"/>
-      <x:c r="C520" s="44" t="s"/>
+      <x:c r="B520" s="35" t="s"/>
+      <x:c r="C520" s="36" t="s"/>
       <x:c r="D520" s="37" t="n">
         <x:v>1107</x:v>
       </x:c>
@@ -9648,8 +9572,8 @@
       </x:c>
     </x:row>
     <x:row r="521" spans="1:10" outlineLevel="3">
-      <x:c r="B521" s="40" t="s"/>
-      <x:c r="C521" s="42" t="s"/>
+      <x:c r="B521" s="35" t="s"/>
+      <x:c r="C521" s="36" t="s"/>
       <x:c r="D521" s="37" t="n">
         <x:v>1007</x:v>
       </x:c>
@@ -9667,7 +9591,7 @@
       </x:c>
     </x:row>
     <x:row r="522" spans="1:10" outlineLevel="2">
-      <x:c r="B522" s="43" t="s"/>
+      <x:c r="B522" s="35" t="s"/>
       <x:c r="C522" s="29" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -9712,7 +9636,7 @@
       <x:c r="H524" s="34" t="s"/>
     </x:row>
     <x:row r="525" spans="1:10" outlineLevel="2">
-      <x:c r="B525" s="39" t="s"/>
+      <x:c r="B525" s="35" t="s"/>
       <x:c r="C525" s="29" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -9723,8 +9647,8 @@
       <x:c r="H525" s="34" t="s"/>
     </x:row>
     <x:row r="526" spans="1:10" outlineLevel="3">
-      <x:c r="B526" s="40" t="s"/>
-      <x:c r="C526" s="41" t="s"/>
+      <x:c r="B526" s="35" t="s"/>
+      <x:c r="C526" s="36" t="s"/>
       <x:c r="D526" s="37" t="n">
         <x:v>1140</x:v>
       </x:c>
@@ -9742,8 +9666,8 @@
       </x:c>
     </x:row>
     <x:row r="527" spans="1:10" outlineLevel="3">
-      <x:c r="B527" s="40" t="s"/>
-      <x:c r="C527" s="42" t="s"/>
+      <x:c r="B527" s="35" t="s"/>
+      <x:c r="C527" s="36" t="s"/>
       <x:c r="D527" s="37" t="n">
         <x:v>1040</x:v>
       </x:c>
@@ -9761,7 +9685,7 @@
       </x:c>
     </x:row>
     <x:row r="528" spans="1:10" outlineLevel="2">
-      <x:c r="B528" s="43" t="s"/>
+      <x:c r="B528" s="35" t="s"/>
       <x:c r="C528" s="29" t="s">
         <x:v>15</x:v>
       </x:c>

</xml_diff>